<commit_message>
- added delta_error while loop termination criterion
- added plot of sigma-yy during iterations
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\theia\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D2A52B-C44E-48B6-8E83-FD9F440FF0F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A0B507-1663-4944-A115-896A53F02D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2898" yWindow="2898" windowWidth="16578" windowHeight="9444" xr2:uid="{BEE921D4-70B4-4CBA-B92B-ED4A2FE488D6}"/>
   </bookViews>
@@ -392,28 +392,28 @@
         <v>9.8638999999999993E-7</v>
       </c>
       <c r="D1">
-        <v>-55258.776760583278</v>
+        <v>-52574.49324095156</v>
       </c>
       <c r="E1">
-        <v>-19662902.672270495</v>
+        <v>-19637559.673730545</v>
       </c>
       <c r="F1">
-        <v>29370.516814876257</v>
+        <v>27198.29371853482</v>
       </c>
       <c r="G1">
-        <v>28590314623.3783</v>
+        <v>28554189234.009251</v>
       </c>
       <c r="H1">
-        <v>0.19066785928657268</v>
+        <v>0.19053993175046344</v>
       </c>
       <c r="I1">
-        <v>1.2920391752696569E-4</v>
+        <v>1.2920949927140387E-4</v>
       </c>
       <c r="J1">
-        <v>-6.8744219582176171E-4</v>
+        <v>-6.875041999116838E-4</v>
       </c>
       <c r="K1">
-        <v>2.4465273371682052E-6</v>
+        <v>2.2683927375611538E-6</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -427,28 +427,28 @@
         <v>1.0629E-6</v>
       </c>
       <c r="D2">
-        <v>-87395.652797130402</v>
+        <v>-82098.303442748729</v>
       </c>
       <c r="E2">
-        <v>-19605941.830610249</v>
+        <v>-19597051.270668078</v>
       </c>
       <c r="F2">
-        <v>16127.507867300479</v>
+        <v>15545.818495249572</v>
       </c>
       <c r="G2">
-        <v>28552183574.346733</v>
+        <v>28540719379.741333</v>
       </c>
       <c r="H2">
-        <v>0.18971355822873209</v>
+        <v>0.18945495145104352</v>
       </c>
       <c r="I2">
-        <v>1.2719872734224733E-4</v>
+        <v>1.2719464609811497E-4</v>
       </c>
       <c r="J2">
-        <v>-6.8610189272280079E-4</v>
+        <v>-6.8614569788610241E-4</v>
       </c>
       <c r="K2">
-        <v>1.3440050328634686E-6</v>
+        <v>1.2958310874412781E-6</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -462,28 +462,28 @@
         <v>5.6680000000000002E-7</v>
       </c>
       <c r="D3">
-        <v>-102131.11953055812</v>
+        <v>-96291.906450588722</v>
       </c>
       <c r="E3">
-        <v>-19404341.101993013</v>
+        <v>-19429589.007951941</v>
       </c>
       <c r="F3">
-        <v>4218.7682666626579</v>
+        <v>4097.600918829995</v>
       </c>
       <c r="G3">
-        <v>28392078951.536369</v>
+        <v>28430721314.269814</v>
       </c>
       <c r="H3">
-        <v>0.18959504624349194</v>
+        <v>0.18929870141310784</v>
       </c>
       <c r="I3">
-        <v>1.2595046507444472E-4</v>
+        <v>1.2593021263157208E-4</v>
       </c>
       <c r="J3">
-        <v>-6.826835083324895E-4</v>
+        <v>-6.8264469313741524E-4</v>
       </c>
       <c r="K3">
-        <v>3.5347655521870969E-7</v>
+        <v>3.4274725717266166E-7</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -497,28 +497,28 @@
         <v>2.6828999999999998E-7</v>
       </c>
       <c r="D4">
-        <v>-106197.49672722491</v>
+        <v>-99838.385674901307</v>
       </c>
       <c r="E4">
-        <v>-19349581.059765611</v>
+        <v>-19363543.241970498</v>
       </c>
       <c r="F4">
-        <v>2254.0440261222566</v>
+        <v>1808.8738484155506</v>
       </c>
       <c r="G4">
-        <v>28500131926.165546</v>
+        <v>28522550760.21537</v>
       </c>
       <c r="H4">
-        <v>0.19041184263595612</v>
+        <v>0.19009150464079744</v>
       </c>
       <c r="I4">
-        <v>1.2552730975861633E-4</v>
+        <v>1.2550321041655669E-4</v>
       </c>
       <c r="J4">
-        <v>-6.781895214443656E-4</v>
+        <v>-6.7812755402399871E-4</v>
       </c>
       <c r="K4">
-        <v>1.8828426052335586E-7</v>
+        <v>1.509228556420333E-7</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -532,28 +532,28 @@
         <v>7.9642000000000006E-8</v>
       </c>
       <c r="D5">
-        <v>-106150.5595281464</v>
+        <v>-99497.062710464001</v>
       </c>
       <c r="E5">
-        <v>-19340433.217157595</v>
+        <v>-19353756.207503397</v>
       </c>
       <c r="F5">
-        <v>-986.17734662297903</v>
+        <v>-862.02882056240742</v>
       </c>
       <c r="G5">
-        <v>28716695255.3988</v>
+        <v>28738449601.332626</v>
       </c>
       <c r="H5">
-        <v>0.19232104464688496</v>
+        <v>0.19198630732287406</v>
       </c>
       <c r="I5">
-        <v>1.2580648474760919E-4</v>
+        <v>1.2578324766461313E-4</v>
       </c>
       <c r="J5">
-        <v>-6.7274929576549851E-4</v>
+        <v>-6.726931818612855E-4</v>
       </c>
       <c r="K5">
-        <v>-8.188687197486751E-8</v>
+        <v>-7.1496876573123001E-8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -567,28 +567,28 @@
         <v>-1.1014000000000001E-7</v>
       </c>
       <c r="D6">
-        <v>-102816.1528808563</v>
+        <v>-96128.809375999961</v>
       </c>
       <c r="E6">
-        <v>-19406358.849063225</v>
+        <v>-19408667.078194577</v>
       </c>
       <c r="F6">
-        <v>-2139.8538546465393</v>
+        <v>-2298.2913984574693</v>
       </c>
       <c r="G6">
-        <v>29078867366.55154</v>
+        <v>29084334628.9613</v>
       </c>
       <c r="H6">
-        <v>0.19510285980587555</v>
+        <v>0.194770781836588</v>
       </c>
       <c r="I6">
-        <v>1.2665219768810655E-4</v>
+        <v>1.2663351614645638E-4</v>
       </c>
       <c r="J6">
-        <v>-6.6667831122616797E-4</v>
+        <v>-6.666454454945939E-4</v>
       </c>
       <c r="K6">
-        <v>-1.7588598882884278E-7</v>
+        <v>-1.8880855418788303E-7</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -602,28 +602,28 @@
         <v>-3.6507000000000003E-7</v>
       </c>
       <c r="D7">
-        <v>-94572.761377775576</v>
+        <v>-88290.778497054707</v>
       </c>
       <c r="E7">
-        <v>-19492782.224834599</v>
+        <v>-19488150.096440647</v>
       </c>
       <c r="F7">
-        <v>-6167.0028760930063</v>
+        <v>-5607.0339427583776</v>
       </c>
       <c r="G7">
-        <v>29499378857.144569</v>
+        <v>29494291215.188057</v>
       </c>
       <c r="H7">
-        <v>0.19845433819926722</v>
+        <v>0.19814578294240925</v>
       </c>
       <c r="I7">
-        <v>1.279163118460647E-4</v>
+        <v>1.2790353592574054E-4</v>
       </c>
       <c r="J7">
-        <v>-6.6016214883876418E-4</v>
+        <v>-6.6015604719304359E-4</v>
       </c>
       <c r="K7">
-        <v>-5.0108564326887184E-7</v>
+        <v>-4.5553699736121844E-7</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -637,28 +637,28 @@
         <v>-6.8467E-7</v>
       </c>
       <c r="D8">
-        <v>-79602.451128169429</v>
+        <v>-74245.31761188386</v>
       </c>
       <c r="E8">
-        <v>-19569862.922971375</v>
+        <v>-19564828.535578143</v>
       </c>
       <c r="F8">
-        <v>-9361.9192060312635</v>
+        <v>-9030.8860331184333</v>
       </c>
       <c r="G8">
-        <v>29929408859.422836</v>
+        <v>29923388985.933365</v>
       </c>
       <c r="H8">
-        <v>0.2020434950895981</v>
+        <v>0.2017818590053097</v>
       </c>
       <c r="I8">
-        <v>1.294382520218988E-4</v>
+        <v>1.2943084466735094E-4</v>
       </c>
       <c r="J8">
-        <v>-6.5333728420666377E-4</v>
+        <v>-6.5335335486259424E-4</v>
       </c>
       <c r="K8">
-        <v>-7.5199419086435229E-7</v>
+        <v>-7.2540003707681901E-7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -672,28 +672,28 @@
         <v>-9.8098000000000009E-7</v>
       </c>
       <c r="D9">
-        <v>-56318.860040936619</v>
+        <v>-52229.152718294878</v>
       </c>
       <c r="E9">
-        <v>-19620036.163593922</v>
+        <v>-19606674.406468868</v>
       </c>
       <c r="F9">
-        <v>-15908.333103451416</v>
+        <v>-14917.170945250087</v>
       </c>
       <c r="G9">
-        <v>30346157394.361351</v>
+        <v>30326791961.517979</v>
       </c>
       <c r="H9">
-        <v>0.20542497475801286</v>
+        <v>0.20522712919702216</v>
       </c>
       <c r="I9">
-        <v>1.3095563105610552E-4</v>
+        <v>1.3095524461778838E-4</v>
       </c>
       <c r="J9">
-        <v>-6.4618726411319583E-4</v>
+        <v>-6.4622581411004408E-4</v>
       </c>
       <c r="K9">
-        <v>-1.2638751473973309E-6</v>
+        <v>-1.1857501000934713E-6</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -707,28 +707,28 @@
         <v>-7.3865000000000001E-7</v>
       </c>
       <c r="D10">
-        <v>-26566.910089452751</v>
+        <v>-24890.75978482049</v>
       </c>
       <c r="E10">
-        <v>-19547759.957739543</v>
+        <v>-19550180.481492933</v>
       </c>
       <c r="F10">
-        <v>-17407.550588106598</v>
+        <v>-15935.175840928887</v>
       </c>
       <c r="G10">
-        <v>30628071334.639191</v>
+        <v>30632410444.567127</v>
       </c>
       <c r="H10">
-        <v>0.20824299702931856</v>
+        <v>0.20816094010579747</v>
       </c>
       <c r="I10">
-        <v>1.3203308305591036E-4</v>
+        <v>1.320322463924544E-4</v>
       </c>
       <c r="J10">
-        <v>-6.3803740298017195E-4</v>
+        <v>-6.3804943118888648E-4</v>
       </c>
       <c r="K10">
-        <v>-1.3733833694856679E-6</v>
+        <v>-1.2569736090003222E-6</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -742,28 +742,28 @@
         <v>1.5813E-6</v>
       </c>
       <c r="D11">
-        <v>41427.558924157172</v>
+        <v>37238.491016909014</v>
       </c>
       <c r="E11">
-        <v>-19713058.024123732</v>
+        <v>-19683553.910390392</v>
       </c>
       <c r="F11">
-        <v>38688.366883495168</v>
+        <v>37311.821682238471</v>
       </c>
       <c r="G11">
-        <v>29009087895.858925</v>
+        <v>28964567581.168037</v>
       </c>
       <c r="H11">
-        <v>0.18207641049875123</v>
+        <v>0.18227937066241134</v>
       </c>
       <c r="I11">
-        <v>1.2518245402436037E-4</v>
+        <v>1.252048631792662E-4</v>
       </c>
       <c r="J11">
-        <v>-6.7988423743740238E-4</v>
+        <v>-6.7995913014005276E-4</v>
       </c>
       <c r="K11">
-        <v>3.1533815845533855E-6</v>
+        <v>3.0467472840032162E-6</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -777,28 +777,28 @@
         <v>1.9032E-6</v>
       </c>
       <c r="D12">
-        <v>38321.874063051771</v>
+        <v>30271.592396956868</v>
       </c>
       <c r="E12">
-        <v>-19558292.583523057</v>
+        <v>-19557563.242755894</v>
       </c>
       <c r="F12">
-        <v>34878.578128844129</v>
+        <v>35043.009628027627</v>
       </c>
       <c r="G12">
-        <v>28882518184.538246</v>
+        <v>28879297943.221111</v>
       </c>
       <c r="H12">
-        <v>0.18196654896796491</v>
+        <v>0.18236440839988444</v>
       </c>
       <c r="I12">
-        <v>1.2456981028067539E-4</v>
+        <v>1.2458866440125268E-4</v>
       </c>
       <c r="J12">
-        <v>-6.7740583218767734E-4</v>
+        <v>-6.7743587639711449E-4</v>
       </c>
       <c r="K12">
-        <v>2.8547553623410864E-6</v>
+        <v>2.8696743608102107E-6</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -812,28 +812,28 @@
         <v>1.1694E-6</v>
       </c>
       <c r="D13">
-        <v>25301.242074573413</v>
+        <v>15978.404820718337</v>
       </c>
       <c r="E13">
-        <v>-19419044.806234088</v>
+        <v>-19436580.771778539</v>
       </c>
       <c r="F13">
-        <v>14864.997206903556</v>
+        <v>15123.341395588544</v>
       </c>
       <c r="G13">
-        <v>28808251492.879688</v>
+        <v>28831741610.175434</v>
       </c>
       <c r="H13">
-        <v>0.1829780344525051</v>
+        <v>0.18344270580352753</v>
       </c>
       <c r="I13">
-        <v>1.242371424571507E-4</v>
+        <v>1.2424739674928492E-4</v>
       </c>
       <c r="J13">
-        <v>-6.7419469751623393E-4</v>
+        <v>-6.7417165060788071E-4</v>
       </c>
       <c r="K13">
-        <v>1.2207854192288056E-6</v>
+        <v>1.2414576118548464E-6</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -847,28 +847,28 @@
         <v>6.7472E-7</v>
       </c>
       <c r="D14">
-        <v>14613.212327204645</v>
+        <v>4973.0279171881266</v>
       </c>
       <c r="E14">
-        <v>-19332644.792350132</v>
+        <v>-19352299.119870096</v>
       </c>
       <c r="F14">
-        <v>8969.6781376993004</v>
+        <v>8006.7176727810029</v>
       </c>
       <c r="G14">
-        <v>28846238909.82793</v>
+        <v>28872905917.122257</v>
       </c>
       <c r="H14">
-        <v>0.18475686666255234</v>
+        <v>0.18523874360764903</v>
       </c>
       <c r="I14">
-        <v>1.2434905882423135E-4</v>
+        <v>1.2435272640279809E-4</v>
       </c>
       <c r="J14">
-        <v>-6.7025025699122068E-4</v>
+        <v>-6.7019102129844401E-4</v>
       </c>
       <c r="K14">
-        <v>7.3677625114397169E-7</v>
+        <v>6.5729173180471964E-7</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -882,28 +882,28 @@
         <v>3.4219000000000002E-7</v>
       </c>
       <c r="D15">
-        <v>6082.1839387831278</v>
+        <v>-2902.8463025172241</v>
       </c>
       <c r="E15">
-        <v>-19345999.097770818</v>
+        <v>-19355634.752403524</v>
       </c>
       <c r="F15">
-        <v>2170.4861705971894</v>
+        <v>1916.9677604145618</v>
       </c>
       <c r="G15">
-        <v>29063720784.746933</v>
+        <v>29075665224.83905</v>
       </c>
       <c r="H15">
-        <v>0.18732438220898001</v>
+        <v>0.18777241513638648</v>
       </c>
       <c r="I15">
-        <v>1.24922772337991E-4</v>
+        <v>1.2492650499724343E-4</v>
       </c>
       <c r="J15">
-        <v>-6.656698025978658E-4</v>
+        <v>-6.6562065240490247E-4</v>
       </c>
       <c r="K15">
-        <v>1.7734219131220049E-7</v>
+        <v>1.5661390042297219E-7</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -917,28 +917,28 @@
         <v>-5.1307999999999999E-8</v>
       </c>
       <c r="D16">
-        <v>891.71465301280841</v>
+        <v>-7189.7051248415373</v>
       </c>
       <c r="E16">
-        <v>-19397971.359792985</v>
+        <v>-19402364.466673315</v>
       </c>
       <c r="F16">
-        <v>-2378.0672403283952</v>
+        <v>-3124.06923358623</v>
       </c>
       <c r="G16">
-        <v>29366206772.856865</v>
+        <v>29370522861.789349</v>
       </c>
       <c r="H16">
-        <v>0.1904909889164268</v>
+        <v>0.19089235975254443</v>
       </c>
       <c r="I16">
-        <v>1.2588197054536559E-4</v>
+        <v>1.2588761068418062E-4</v>
       </c>
       <c r="J16">
-        <v>-6.6055948491278496E-4</v>
+        <v>-6.6053086847458033E-4</v>
       </c>
       <c r="K16">
-        <v>-1.9281652275022522E-7</v>
+        <v>-2.5334402042453269E-7</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -952,28 +952,28 @@
         <v>-6.4053999999999999E-7</v>
       </c>
       <c r="D17">
-        <v>-2109.8173003285192</v>
+        <v>-8984.1581835229881</v>
       </c>
       <c r="E17">
-        <v>-19486669.108623978</v>
+        <v>-19482585.674849831</v>
       </c>
       <c r="F17">
-        <v>-11396.410870952215</v>
+        <v>-11077.294040573363</v>
       </c>
       <c r="G17">
-        <v>29746841648.055958</v>
+        <v>29738565385.967209</v>
       </c>
       <c r="H17">
-        <v>0.19414435474885619</v>
+        <v>0.19448391711547269</v>
       </c>
       <c r="I17">
-        <v>1.27131918361633E-4</v>
+        <v>1.2714042062669204E-4</v>
       </c>
       <c r="J17">
-        <v>-6.5508771342016122E-4</v>
+        <v>-6.5508497208475883E-4</v>
       </c>
       <c r="K17">
-        <v>-9.1503186516308306E-7</v>
+        <v>-8.8991660568302168E-7</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -987,28 +987,28 @@
         <v>-1.3919E-6</v>
       </c>
       <c r="D18">
-        <v>-963.98121668584645</v>
+        <v>-6321.8810634822585</v>
       </c>
       <c r="E18">
-        <v>-19565419.78529058</v>
+        <v>-19558492.998047926</v>
       </c>
       <c r="F18">
-        <v>-21275.157445537643</v>
+        <v>-21266.340821899859</v>
       </c>
       <c r="G18">
-        <v>30130960556.120914</v>
+        <v>30118657314.499115</v>
       </c>
       <c r="H18">
-        <v>0.19794021811464263</v>
+        <v>0.19820342933926149</v>
       </c>
       <c r="I18">
-        <v>1.2851773142996494E-4</v>
+        <v>1.2852845909858317E-4</v>
       </c>
       <c r="J18">
-        <v>-6.4935758997337564E-4</v>
+        <v>-6.4937990124340006E-4</v>
       </c>
       <c r="K18">
-        <v>-1.6917843360006153E-6</v>
+        <v>-1.6922176284420111E-6</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1022,28 +1022,28 @@
         <v>-2.0153999999999998E-6</v>
       </c>
       <c r="D19">
-        <v>6568.3643705635332</v>
+        <v>2592.0772352721542</v>
       </c>
       <c r="E19">
-        <v>-19603635.431005687</v>
+        <v>-19594370.525521912</v>
       </c>
       <c r="F19">
-        <v>-34714.314093945039</v>
+        <v>-33716.805124729326</v>
       </c>
       <c r="G19">
-        <v>30472344027.103584</v>
+        <v>30456693233.291237</v>
       </c>
       <c r="H19">
-        <v>0.20138070461746618</v>
+        <v>0.20157541154787978</v>
       </c>
       <c r="I19">
-        <v>1.2978401543998114E-4</v>
+        <v>1.2979497428701622E-4</v>
       </c>
       <c r="J19">
-        <v>-6.4339101527120205E-4</v>
+        <v>-6.4342217383073848E-4</v>
       </c>
       <c r="K19">
-        <v>-2.737375005968279E-6</v>
+        <v>-2.6606584327019478E-6</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1057,28 +1057,28 @@
         <v>-1.4313E-6</v>
       </c>
       <c r="D20">
-        <v>11141.134429818019</v>
+        <v>9294.6230011940934</v>
       </c>
       <c r="E20">
-        <v>-19577265.011284523</v>
+        <v>-19576554.537708156</v>
       </c>
       <c r="F20">
-        <v>-29808.156876806966</v>
+        <v>-28217.348918333031</v>
       </c>
       <c r="G20">
-        <v>30737169925.737873</v>
+        <v>30735454281.670883</v>
       </c>
       <c r="H20">
-        <v>0.20447693429937452</v>
+        <v>0.20456752166205233</v>
       </c>
       <c r="I20">
-        <v>1.3060301645854733E-4</v>
+        <v>1.3061017235436992E-4</v>
       </c>
       <c r="J20">
-        <v>-6.3699589820541218E-4</v>
+        <v>-6.3701717128366469E-4</v>
       </c>
       <c r="K20">
-        <v>-2.3361480966409341E-6</v>
+        <v>-2.2118426846807256E-6</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1092,28 +1092,28 @@
         <v>6.5932E-7</v>
       </c>
       <c r="D21">
-        <v>-4282.5030953050591</v>
+        <v>-1941.8966078381054</v>
       </c>
       <c r="E21">
-        <v>-19747930.914007384</v>
+        <v>-19717648.476236295</v>
       </c>
       <c r="F21">
-        <v>13738.368145997661</v>
+        <v>14515.656357896365</v>
       </c>
       <c r="G21">
-        <v>29326308429.744038</v>
+        <v>29281967781.114414</v>
       </c>
       <c r="H21">
-        <v>0.18100427965159718</v>
+        <v>0.18088972630679054</v>
       </c>
       <c r="I21">
-        <v>1.2174652200604413E-4</v>
+        <v>1.2175691479906093E-4</v>
       </c>
       <c r="J21">
-        <v>-6.7343361508625187E-4</v>
+        <v>-6.7350924264852267E-4</v>
       </c>
       <c r="K21">
-        <v>1.1066320913333347E-6</v>
+        <v>1.1710267859739443E-6</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1127,28 +1127,28 @@
         <v>8.9069000000000004E-7</v>
       </c>
       <c r="D22">
-        <v>31854.334055593237</v>
+        <v>33246.887300440576</v>
       </c>
       <c r="E22">
-        <v>-19539520.584106088</v>
+        <v>-19542962.796934903</v>
       </c>
       <c r="F22">
-        <v>19615.891980164248</v>
+        <v>22061.15697874633</v>
       </c>
       <c r="G22">
-        <v>29192954529.22578</v>
+        <v>29198475751.706978</v>
       </c>
       <c r="H22">
-        <v>0.17989559919475734</v>
+        <v>0.17982666915469905</v>
       </c>
       <c r="I22">
-        <v>1.2148990591024972E-4</v>
+        <v>1.2149757127049362E-4</v>
       </c>
       <c r="J22">
-        <v>-6.695010433000688E-4</v>
+        <v>-6.6951854879784009E-4</v>
       </c>
       <c r="K22">
-        <v>1.585580275466369E-6</v>
+        <v>1.7828508254689752E-6</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1162,28 +1162,28 @@
         <v>7.1518000000000003E-7</v>
       </c>
       <c r="D23">
-        <v>58714.760738809593</v>
+        <v>56977.269174656831</v>
       </c>
       <c r="E23">
-        <v>-19415277.201508749</v>
+        <v>-19428531.501888864</v>
       </c>
       <c r="F23">
-        <v>11933.591865746055</v>
+        <v>13974.773695346206</v>
       </c>
       <c r="G23">
-        <v>29157874372.920795</v>
+        <v>29177311740.273926</v>
       </c>
       <c r="H23">
-        <v>0.18001510012600699</v>
+        <v>0.18010349324496394</v>
       </c>
       <c r="I23">
-        <v>1.2187411658089083E-4</v>
+        <v>1.2188434858381703E-4</v>
       </c>
       <c r="J23">
-        <v>-6.6619359647510752E-4</v>
+        <v>-6.6617354425027944E-4</v>
       </c>
       <c r="K23">
-        <v>9.6585009056322476E-7</v>
+        <v>1.1303713791186581E-6</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1197,28 +1197,28 @@
         <v>6.525E-7</v>
       </c>
       <c r="D24">
-        <v>69375.601899312809</v>
+        <v>65353.289393544197</v>
       </c>
       <c r="E24">
-        <v>-19330844.967479993</v>
+        <v>-19351098.186510492</v>
       </c>
       <c r="F24">
-        <v>9901.4462094852661</v>
+        <v>9823.6009917357678</v>
       </c>
       <c r="G24">
-        <v>29187065710.597454</v>
+        <v>29216544239.458866</v>
       </c>
       <c r="H24">
-        <v>0.18146072574691002</v>
+        <v>0.18166537245703185</v>
       </c>
       <c r="I24">
-        <v>1.2255732594882373E-4</v>
+        <v>1.2256818833547675E-4</v>
       </c>
       <c r="J24">
-        <v>-6.6269279877882606E-4</v>
+        <v>-6.6264125255950516E-4</v>
       </c>
       <c r="K24">
-        <v>8.0154881158974161E-7</v>
+        <v>7.945410881971763E-7</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1232,28 +1232,28 @@
         <v>6.2223000000000003E-7</v>
       </c>
       <c r="D25">
-        <v>70273.064542424865</v>
+        <v>65195.068744348828</v>
       </c>
       <c r="E25">
-        <v>-19341191.713702574</v>
+        <v>-19350472.855905831</v>
       </c>
       <c r="F25">
-        <v>8469.223593528086</v>
+        <v>7741.2652099550769</v>
       </c>
       <c r="G25">
-        <v>29375605061.336929</v>
+        <v>29388298533.175678</v>
       </c>
       <c r="H25">
-        <v>0.18392453354460508</v>
+        <v>0.18417978333737783</v>
       </c>
       <c r="I25">
-        <v>1.2349607756459441E-4</v>
+        <v>1.235103562367298E-4</v>
       </c>
       <c r="J25">
-        <v>-6.5883843954714382E-4</v>
+        <v>-6.5879022815015938E-4</v>
       </c>
       <c r="K25">
-        <v>6.8266522140872409E-7</v>
+        <v>6.2382569800269834E-7</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1267,28 +1267,28 @@
         <v>3.9292E-7</v>
       </c>
       <c r="D26">
-        <v>62259.730800341815</v>
+        <v>57412.610962906852</v>
       </c>
       <c r="E26">
-        <v>-19394253.514238369</v>
+        <v>-19397842.0612523</v>
       </c>
       <c r="F26">
-        <v>4113.589015683694</v>
+        <v>2777.7909017571874</v>
       </c>
       <c r="G26">
-        <v>29645904021.634235</v>
+        <v>29650019808.879314</v>
       </c>
       <c r="H26">
-        <v>0.18726767712670367</v>
+        <v>0.18750938086978564</v>
       </c>
       <c r="I26">
-        <v>1.246177724255455E-4</v>
+        <v>1.2463431593735509E-4</v>
       </c>
       <c r="J26">
-        <v>-6.5458903941975611E-4</v>
+        <v>-6.5456344689107529E-4</v>
       </c>
       <c r="K26">
-        <v>3.2948725619890654E-7</v>
+        <v>2.2250528124368374E-7</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1302,28 +1302,28 @@
         <v>-1.6742E-7</v>
       </c>
       <c r="D27">
-        <v>51446.462211755104</v>
+        <v>47552.832364575472</v>
       </c>
       <c r="E27">
-        <v>-19474234.063167743</v>
+        <v>-19472154.900890801</v>
       </c>
       <c r="F27">
-        <v>-4000.2657435809292</v>
+        <v>-5216.666331783541</v>
       </c>
       <c r="G27">
-        <v>29973176144.312286</v>
+        <v>29968848517.921589</v>
       </c>
       <c r="H27">
-        <v>0.1910410086636283</v>
+        <v>0.19123336343478484</v>
       </c>
       <c r="I27">
-        <v>1.2584787527139573E-4</v>
+        <v>1.2586486261514904E-4</v>
       </c>
       <c r="J27">
-        <v>-6.500585403218153E-4</v>
+        <v>-6.5005844363854063E-4</v>
       </c>
       <c r="K27">
-        <v>-3.1792303991533873E-7</v>
+        <v>-4.1473295021561638E-7</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1337,28 +1337,28 @@
         <v>-9.6919999999999997E-7</v>
       </c>
       <c r="D28">
-        <v>38144.900609401986</v>
+        <v>35650.200976342428</v>
       </c>
       <c r="E28">
-        <v>-19556608.274553459</v>
+        <v>-19547159.988068908</v>
       </c>
       <c r="F28">
-        <v>-15714.924467613764</v>
+        <v>-17104.164160659919</v>
       </c>
       <c r="G28">
-        <v>30316826182.377052</v>
+        <v>30301441971.825321</v>
       </c>
       <c r="H28">
-        <v>0.19504974855096319</v>
+        <v>0.19517149319387755</v>
       </c>
       <c r="I28">
-        <v>1.2708778843241889E-4</v>
+        <v>1.271044713803816E-4</v>
       </c>
       <c r="J28">
-        <v>-6.4534310766613983E-4</v>
+        <v>-6.4536651500028642E-4</v>
       </c>
       <c r="K28">
-        <v>-1.2389738293847301E-6</v>
+        <v>-1.3493947429254029E-6</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1372,28 +1372,28 @@
         <v>-1.6011E-6</v>
       </c>
       <c r="D29">
-        <v>19102.399127574172</v>
+        <v>18529.35658733733</v>
       </c>
       <c r="E29">
-        <v>-19589838.957130011</v>
+        <v>-19584659.998612054</v>
       </c>
       <c r="F29">
-        <v>-27473.060009223049</v>
+        <v>-28181.992870398666</v>
       </c>
       <c r="G29">
-        <v>30588336485.229156</v>
+        <v>30580077837.558163</v>
       </c>
       <c r="H29">
-        <v>0.19920029401429637</v>
+        <v>0.19922804526311969</v>
       </c>
       <c r="I29">
-        <v>1.2820079992790118E-4</v>
+        <v>1.2821121524192252E-4</v>
       </c>
       <c r="J29">
-        <v>-6.4056909253417478E-4</v>
+        <v>-6.405911618708141E-4</v>
       </c>
       <c r="K29">
-        <v>-2.1541664085965176E-6</v>
+        <v>-2.2104957227064761E-6</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1407,28 +1407,28 @@
         <v>-1.1000000000000001E-6</v>
       </c>
       <c r="D30">
-        <v>370.72654795181006</v>
+        <v>971.12659987062216</v>
       </c>
       <c r="E30">
-        <v>-19610299.810105346</v>
+        <v>-19607469.233699232</v>
       </c>
       <c r="F30">
-        <v>-20583.860590204295</v>
+        <v>-20391.420772648413</v>
       </c>
       <c r="G30">
-        <v>30832975178.145695</v>
+        <v>30828715567.236919</v>
       </c>
       <c r="H30">
-        <v>0.20300952025599794</v>
+        <v>0.20298017787182568</v>
       </c>
       <c r="I30">
-        <v>1.2912759230583701E-4</v>
+        <v>1.2913335827741899E-4</v>
       </c>
       <c r="J30">
-        <v>-6.3601989709680281E-4</v>
+        <v>-6.3604638118092236E-4</v>
       </c>
       <c r="K30">
-        <v>-1.606236688681483E-6</v>
+        <v>-1.5914679339405161E-6</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1442,28 +1442,28 @@
         <v>-3.6991000000000001E-7</v>
       </c>
       <c r="D31">
-        <v>24080.861665114295</v>
+        <v>21154.74785068538</v>
       </c>
       <c r="E31">
-        <v>-19750757.354816508</v>
+        <v>-19722539.060428768</v>
       </c>
       <c r="F31">
-        <v>-2477.1072888550048</v>
+        <v>-1177.7248039361498</v>
       </c>
       <c r="G31">
-        <v>29586693571.762554</v>
+        <v>29543657021.601696</v>
       </c>
       <c r="H31">
-        <v>0.17768730631224383</v>
+        <v>0.1778293048731488</v>
       </c>
       <c r="I31">
-        <v>1.1945059450050991E-4</v>
+        <v>1.1946806205292483E-4</v>
       </c>
       <c r="J31">
-        <v>-6.6777069344492782E-4</v>
+        <v>-6.6784304836752027E-4</v>
       </c>
       <c r="K31">
-        <v>-1.9722351899558767E-7</v>
+        <v>-9.3927289610603454E-8</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1477,28 +1477,28 @@
         <v>-7.9564999999999995E-7</v>
       </c>
       <c r="D32">
-        <v>35531.631087009795</v>
+        <v>32957.998564688955</v>
       </c>
       <c r="E32">
-        <v>-19540643.181719489</v>
+        <v>-19545159.714193176</v>
       </c>
       <c r="F32">
-        <v>-8043.4826522510666</v>
+        <v>-5277.9280031790404</v>
       </c>
       <c r="G32">
-        <v>29483947110.262032</v>
+        <v>29490070980.568775</v>
       </c>
       <c r="H32">
-        <v>0.17818785686891525</v>
+        <v>0.17831584955560659</v>
       </c>
       <c r="I32">
-        <v>1.1930462332874797E-4</v>
+        <v>1.193095471715964E-4</v>
       </c>
       <c r="J32">
-        <v>-6.629523389590831E-4</v>
+        <v>-6.6296500624984261E-4</v>
       </c>
       <c r="K32">
-        <v>-6.4282939501016188E-7</v>
+        <v>-4.2177586550998323E-7</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1512,28 +1512,28 @@
         <v>-4.9912000000000004E-7</v>
       </c>
       <c r="D33">
-        <v>52538.842181542888</v>
+        <v>52435.477274132892</v>
       </c>
       <c r="E33">
-        <v>-19413430.599600635</v>
+        <v>-19424942.213370148</v>
       </c>
       <c r="F33">
-        <v>-6118.2196263617279</v>
+        <v>-3680.2663478076693</v>
       </c>
       <c r="G33">
-        <v>29455787818.367317</v>
+        <v>29473216022.637047</v>
       </c>
       <c r="H33">
-        <v>0.17932287086440515</v>
+        <v>0.17932963433648244</v>
       </c>
       <c r="I33">
-        <v>1.1996474017374415E-4</v>
+        <v>1.199623890843395E-4</v>
       </c>
       <c r="J33">
-        <v>-6.5935943026054354E-4</v>
+        <v>-6.5933816191945244E-4</v>
       </c>
       <c r="K33">
-        <v>-4.8988841260737097E-7</v>
+        <v>-2.9449894521117737E-7</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1547,28 +1547,28 @@
         <v>1.1864E-7</v>
       </c>
       <c r="D34">
-        <v>67312.492807658855</v>
+        <v>68189.958212159574</v>
       </c>
       <c r="E34">
-        <v>-19339408.254082259</v>
+        <v>-19357436.821504183</v>
       </c>
       <c r="F34">
-        <v>933.50382020950292</v>
+        <v>1531.8123484904038</v>
       </c>
       <c r="G34">
-        <v>29495332647.375092</v>
+        <v>29523049448.036961</v>
       </c>
       <c r="H34">
-        <v>0.1810157752547677</v>
+        <v>0.1809750617740144</v>
       </c>
       <c r="I34">
-        <v>1.2095871506820718E-4</v>
+        <v>1.2095303765480075E-4</v>
       </c>
       <c r="J34">
-        <v>-6.5604601227192E-4</v>
+        <v>-6.5600023698685083E-4</v>
       </c>
       <c r="K34">
-        <v>7.4751102028310784E-8</v>
+        <v>1.2253366481218032E-7</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1582,28 +1582,28 @@
         <v>6.9874999999999998E-7</v>
       </c>
       <c r="D35">
-        <v>72938.386325036641</v>
+        <v>74278.246955776587</v>
       </c>
       <c r="E35">
-        <v>-19342339.976892285</v>
+        <v>-19351510.892674614</v>
       </c>
       <c r="F35">
-        <v>9387.8518339219954</v>
+        <v>8481.0215676835924</v>
       </c>
       <c r="G35">
-        <v>29654853598.19379</v>
+        <v>29669272034.946236</v>
       </c>
       <c r="H35">
-        <v>0.18347357079859869</v>
+        <v>0.18340843040676869</v>
       </c>
       <c r="I35">
-        <v>1.2212194889226906E-4</v>
+        <v>1.2211740970956362E-4</v>
       </c>
       <c r="J35">
-        <v>-6.5268557519119618E-4</v>
+        <v>-6.5263674693438029E-4</v>
       </c>
       <c r="K35">
-        <v>7.4928395048755574E-7</v>
+        <v>6.7649315710371395E-7</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1617,28 +1617,28 @@
         <v>9.4620000000000004E-7</v>
       </c>
       <c r="D36">
-        <v>71320.141630524304</v>
+        <v>72694.390283033717</v>
       </c>
       <c r="E36">
-        <v>-19391252.782119229</v>
+        <v>-19394040.813785322</v>
       </c>
       <c r="F36">
-        <v>12097.853259415291</v>
+        <v>10631.627916071899</v>
       </c>
       <c r="G36">
-        <v>29894547771.393219</v>
+        <v>29899227022.612877</v>
       </c>
       <c r="H36">
-        <v>0.18645387257582982</v>
+        <v>0.18638607025039516</v>
       </c>
       <c r="I36">
-        <v>1.2332399646465092E-4</v>
+        <v>1.233241761410133E-4</v>
       </c>
       <c r="J36">
-        <v>-6.4909864855962796E-4</v>
+        <v>-6.4907135297588635E-4</v>
       </c>
       <c r="K36">
-        <v>9.6026931797389171E-7</v>
+        <v>8.436773586864392E-7</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1652,28 +1652,28 @@
         <v>7.2341999999999995E-7</v>
       </c>
       <c r="D37">
-        <v>60558.309050767682</v>
+        <v>61841.882014318369</v>
       </c>
       <c r="E37">
-        <v>-19467989.188959904</v>
+        <v>-19466193.517374862</v>
       </c>
       <c r="F37">
-        <v>9554.3568911769835</v>
+        <v>7658.5364268710437</v>
       </c>
       <c r="G37">
-        <v>30186728084.567959</v>
+        <v>30184314129.828671</v>
       </c>
       <c r="H37">
-        <v>0.18999889194023942</v>
+        <v>0.18993513817770391</v>
       </c>
       <c r="I37">
-        <v>1.2453559018681798E-4</v>
+        <v>1.2454024085523693E-4</v>
       </c>
       <c r="J37">
-        <v>-6.4530416261236148E-4</v>
+        <v>-6.4530508813455834E-4</v>
       </c>
       <c r="K37">
-        <v>7.5328938294136772E-7</v>
+        <v>6.0383836617884136E-7</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1687,28 +1687,28 @@
         <v>1.3049E-7</v>
       </c>
       <c r="D38">
-        <v>43640.637441180181</v>
+        <v>44515.670457735192</v>
       </c>
       <c r="E38">
-        <v>-19543452.887378167</v>
+        <v>-19533913.746838801</v>
       </c>
       <c r="F38">
-        <v>1063.2271645133792</v>
+        <v>-548.12449535759129</v>
       </c>
       <c r="G38">
-        <v>30481277141.583244</v>
+        <v>30466666929.936077</v>
       </c>
       <c r="H38">
-        <v>0.19380153591876997</v>
+        <v>0.19375737477715554</v>
       </c>
       <c r="I38">
-        <v>1.2569102239749021E-4</v>
+        <v>1.2569771717442003E-4</v>
       </c>
       <c r="J38">
-        <v>-6.4146302701671124E-4</v>
+        <v>-6.4148186968406018E-4</v>
       </c>
       <c r="K38">
-        <v>8.3285355601133391E-8</v>
+        <v>-4.2956451197658473E-8</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1722,28 +1722,28 @@
         <v>-4.7189999999999998E-7</v>
       </c>
       <c r="D39">
-        <v>26877.784014733508</v>
+        <v>26193.554770272691</v>
       </c>
       <c r="E39">
-        <v>-19583817.814102031</v>
+        <v>-19580128.336271994</v>
       </c>
       <c r="F39">
-        <v>-8042.1588880451845</v>
+        <v>-8919.5780750893682</v>
       </c>
       <c r="G39">
-        <v>30717923008.014725</v>
+        <v>30711928433.971867</v>
       </c>
       <c r="H39">
-        <v>0.19745508567297815</v>
+        <v>0.19748838232891078</v>
       </c>
       <c r="I39">
-        <v>1.2676268103740024E-4</v>
+        <v>1.2676861551141308E-4</v>
       </c>
       <c r="J39">
-        <v>-6.3771667378153044E-4</v>
+        <v>-6.3773341150682962E-4</v>
       </c>
       <c r="K39">
-        <v>-6.270113578913045E-7</v>
+        <v>-6.9559558967240837E-7</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1757,28 +1757,28 @@
         <v>-4.6591999999999998E-7</v>
       </c>
       <c r="D40">
-        <v>12519.165961920284</v>
+        <v>11279.284283846617</v>
       </c>
       <c r="E40">
-        <v>-19626907.960329011</v>
+        <v>-19624134.883557599</v>
       </c>
       <c r="F40">
-        <v>-8355.8245136940059</v>
+        <v>-8699.3765337892437</v>
       </c>
       <c r="G40">
-        <v>30933914370.778183</v>
+        <v>30929153458.664318</v>
       </c>
       <c r="H40">
-        <v>0.20086606240218605</v>
+        <v>0.20092659277927258</v>
       </c>
       <c r="I40">
-        <v>1.278532867291898E-4</v>
+        <v>1.2786088976296945E-4</v>
       </c>
       <c r="J40">
-        <v>-6.3456139042270367E-4</v>
+        <v>-6.3458799846335327E-4</v>
       </c>
       <c r="K40">
-        <v>-6.4875652512467498E-7</v>
+        <v>-6.755986820296267E-7</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1792,28 +1792,28 @@
         <v>-1.2176E-6</v>
       </c>
       <c r="D41">
-        <v>2485.4170976411551</v>
+        <v>4762.9841436487623</v>
       </c>
       <c r="E41">
-        <v>-19728355.145181429</v>
+        <v>-19703353.286422022</v>
       </c>
       <c r="F41">
-        <v>-17592.403602728449</v>
+        <v>-15807.972101692856</v>
       </c>
       <c r="G41">
-        <v>29766743840.449642</v>
+        <v>29729627480.963093</v>
       </c>
       <c r="H41">
-        <v>0.17823264998473964</v>
+        <v>0.1781207188498394</v>
       </c>
       <c r="I41">
-        <v>1.1821343912644076E-4</v>
+        <v>1.1822393770036634E-4</v>
       </c>
       <c r="J41">
-        <v>-6.6283977389064788E-4</v>
+        <v>-6.6290214820008777E-4</v>
       </c>
       <c r="K41">
-        <v>-1.3928046618422738E-6</v>
+        <v>-1.2530897630496371E-6</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1827,28 +1827,28 @@
         <v>-2.4233000000000002E-6</v>
       </c>
       <c r="D42">
-        <v>24638.397158198059</v>
+        <v>26072.33188107796</v>
       </c>
       <c r="E42">
-        <v>-19543785.584705528</v>
+        <v>-19547434.395631455</v>
       </c>
       <c r="F42">
-        <v>-30583.342241102917</v>
+        <v>-27783.007745806655</v>
       </c>
       <c r="G42">
-        <v>29722035012.351536</v>
+        <v>29727954116.037762</v>
       </c>
       <c r="H42">
-        <v>0.17845132289158097</v>
+        <v>0.17838094330470736</v>
       </c>
       <c r="I42">
-        <v>1.1816128731874625E-4</v>
+        <v>1.1816681347671064E-4</v>
       </c>
       <c r="J42">
-        <v>-6.5768281324598741E-4</v>
+        <v>-6.5769548053586872E-4</v>
       </c>
       <c r="K42">
-        <v>-2.4251217855156097E-6</v>
+        <v>-2.2025473947324915E-6</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1862,28 +1862,28 @@
         <v>-1.9112E-6</v>
       </c>
       <c r="D43">
-        <v>47602.349975207821</v>
+        <v>47091.722271656618</v>
       </c>
       <c r="E43">
-        <v>-19420404.600569636</v>
+        <v>-19431626.161513627</v>
       </c>
       <c r="F43">
-        <v>-24578.256144768518</v>
+        <v>-22615.285974861396</v>
       </c>
       <c r="G43">
-        <v>29713325245.300159</v>
+        <v>29730339903.640064</v>
       </c>
       <c r="H43">
-        <v>0.17946642235286692</v>
+        <v>0.17949346209465467</v>
       </c>
       <c r="I43">
-        <v>1.1889599605744415E-4</v>
+        <v>1.1889398287143974E-4</v>
       </c>
       <c r="J43">
-        <v>-6.538507242896301E-4</v>
+        <v>-6.5383014998345273E-4</v>
       </c>
       <c r="K43">
-        <v>-1.9511773214349153E-6</v>
+        <v>-1.7943046712265648E-6</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1897,28 +1897,28 @@
         <v>-6.7843000000000002E-7</v>
       </c>
       <c r="D44">
-        <v>60485.745108628646</v>
+        <v>60042.777836396825</v>
       </c>
       <c r="E44">
-        <v>-19355891.664489046</v>
+        <v>-19370729.325672884</v>
       </c>
       <c r="F44">
-        <v>-9852.8742393491157</v>
+        <v>-9601.1013259297688</v>
       </c>
       <c r="G44">
-        <v>29767698852.415321</v>
+        <v>29790383254.213459</v>
       </c>
       <c r="H44">
-        <v>0.18139393226220291</v>
+        <v>0.18141837561328142</v>
       </c>
       <c r="I44">
-        <v>1.1997647071564972E-4</v>
+        <v>1.1996661631334535E-4</v>
       </c>
       <c r="J44">
-        <v>-6.5056545487762523E-4</v>
+        <v>-6.5052596603180956E-4</v>
       </c>
       <c r="K44">
-        <v>-7.8202566100343991E-7</v>
+        <v>-7.6142906875399825E-7</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1932,28 +1932,28 @@
         <v>5.8530000000000003E-7</v>
       </c>
       <c r="D45">
-        <v>66878.109784403816</v>
+        <v>66856.814896214288</v>
       </c>
       <c r="E45">
-        <v>-19352533.652974207</v>
+        <v>-19361569.31053241</v>
       </c>
       <c r="F45">
-        <v>7111.9882679454586</v>
+        <v>5721.9693313299504</v>
       </c>
       <c r="G45">
-        <v>29909379077.602287</v>
+        <v>29923327384.438328</v>
       </c>
       <c r="H45">
-        <v>0.18382816223594511</v>
+        <v>0.1838308289812581</v>
       </c>
       <c r="I45">
-        <v>1.211799403739835E-4</v>
+        <v>1.2116650721073416E-4</v>
       </c>
       <c r="J45">
-        <v>-6.4743592676411751E-4</v>
+        <v>-6.4739114665741406E-4</v>
       </c>
       <c r="K45">
-        <v>5.6298173151938732E-7</v>
+        <v>4.5270402207584111E-7</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1967,28 +1967,28 @@
         <v>1.4465E-6</v>
       </c>
       <c r="D46">
-        <v>63696.207122332416</v>
+        <v>64330.072103064042</v>
       </c>
       <c r="E46">
-        <v>-19396719.142742857</v>
+        <v>-19398932.411509626</v>
       </c>
       <c r="F46">
-        <v>18797.181428637152</v>
+        <v>17089.756745486684</v>
       </c>
       <c r="G46">
-        <v>30125910663.50433</v>
+        <v>30129520955.562828</v>
       </c>
       <c r="H46">
-        <v>0.18678992673225303</v>
+        <v>0.1867589089726174</v>
       </c>
       <c r="I46">
-        <v>1.2238123045381501E-4</v>
+        <v>1.2236959067886839E-4</v>
       </c>
       <c r="J46">
-        <v>-6.4425093933639303E-4</v>
+        <v>-6.4422457969483715E-4</v>
       </c>
       <c r="K46">
-        <v>1.4810088814138419E-6</v>
+        <v>1.3462191043485394E-6</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2002,28 +2002,28 @@
         <v>1.7081E-6</v>
       </c>
       <c r="D47">
-        <v>53913.905758093111</v>
+        <v>54825.809241429437</v>
       </c>
       <c r="E47">
-        <v>-19464574.480993502</v>
+        <v>-19462532.660233412</v>
       </c>
       <c r="F47">
-        <v>22864.835934728097</v>
+        <v>20915.379091400031</v>
       </c>
       <c r="G47">
-        <v>30383362678.784096</v>
+        <v>30380435570.0303</v>
       </c>
       <c r="H47">
-        <v>0.19005501520293444</v>
+        <v>0.19000978827372478</v>
       </c>
       <c r="I47">
-        <v>1.2353111929225223E-4</v>
+        <v>1.2352436501939849E-4</v>
       </c>
       <c r="J47">
-        <v>-6.4097536260958755E-4</v>
+        <v>-6.4097549911556789E-4</v>
       </c>
       <c r="K47">
-        <v>1.7911546153939577E-6</v>
+        <v>1.638521370472823E-6</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2037,28 +2037,28 @@
         <v>1.4191999999999999E-6</v>
       </c>
       <c r="D48">
-        <v>40132.303105918691</v>
+        <v>41048.503565996885</v>
       </c>
       <c r="E48">
-        <v>-19534811.98368511</v>
+        <v>-19526643.519797105</v>
       </c>
       <c r="F48">
-        <v>18560.759569902311</v>
+        <v>17333.988376171867</v>
       </c>
       <c r="G48">
-        <v>30644925368.247841</v>
+        <v>30632387065.486702</v>
       </c>
       <c r="H48">
-        <v>0.19342551587999188</v>
+        <v>0.19337963299509794</v>
       </c>
       <c r="I48">
-        <v>1.2461287899638023E-4</v>
+        <v>1.246117226262433E-4</v>
       </c>
       <c r="J48">
-        <v>-6.3773013598407554E-4</v>
+        <v>-6.3774471318422195E-4</v>
       </c>
       <c r="K48">
-        <v>1.4456915129403176E-6</v>
+        <v>1.35066287644558E-6</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2072,28 +2072,28 @@
         <v>8.1691000000000003E-7</v>
       </c>
       <c r="D49">
-        <v>20029.609920558985</v>
+        <v>21592.677397949621</v>
       </c>
       <c r="E49">
-        <v>-19577699.240789119</v>
+        <v>-19574198.09487465</v>
       </c>
       <c r="F49">
-        <v>11483.065700707037</v>
+        <v>11125.804634555534</v>
       </c>
       <c r="G49">
-        <v>30851328841.836441</v>
+        <v>30846294527.236816</v>
       </c>
       <c r="H49">
-        <v>0.19702846930324319</v>
+        <v>0.19695155873371631</v>
       </c>
       <c r="I49">
-        <v>1.2567704924538943E-4</v>
+        <v>1.2567813309554535E-4</v>
       </c>
       <c r="J49">
-        <v>-6.3471529846959333E-4</v>
+        <v>-6.3472950662491964E-4</v>
       </c>
       <c r="K49">
-        <v>8.9108644717368103E-7</v>
+        <v>8.6346572490702579E-7</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2107,28 +2107,28 @@
         <v>2.0029E-7</v>
       </c>
       <c r="D50">
-        <v>3233.1773052723147</v>
+        <v>4654.6084058438428</v>
       </c>
       <c r="E50">
-        <v>-19625224.503869217</v>
+        <v>-19622980.833812445</v>
       </c>
       <c r="F50">
-        <v>3789.0453260064119</v>
+        <v>3620.468969299644</v>
       </c>
       <c r="G50">
-        <v>31034445674.839321</v>
+        <v>31031347701.16275</v>
       </c>
       <c r="H50">
-        <v>0.20046173110341339</v>
+        <v>0.20039218893319877</v>
       </c>
       <c r="I50">
-        <v>1.2686615002053644E-4</v>
+        <v>1.2686920456555625E-4</v>
       </c>
       <c r="J50">
-        <v>-6.3238956490063725E-4</v>
+        <v>-6.3241189412075426E-4</v>
       </c>
       <c r="K50">
-        <v>2.9313095960921062E-7</v>
+        <v>2.8011052730851464E-7</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2142,28 +2142,28 @@
         <v>-1.8450999999999999E-6</v>
       </c>
       <c r="D51">
-        <v>8927.451617971994</v>
+        <v>6801.9679042501375</v>
       </c>
       <c r="E51">
-        <v>-19686714.935798824</v>
+        <v>-19665430.156397562</v>
       </c>
       <c r="F51">
-        <v>-25643.453647061135</v>
+        <v>-23817.704360538733</v>
       </c>
       <c r="G51">
-        <v>29894649185.952183</v>
+        <v>29861746693.091282</v>
       </c>
       <c r="H51">
-        <v>0.17871623713195606</v>
+        <v>0.17882061212520403</v>
       </c>
       <c r="I51">
-        <v>1.1800700783031999E-4</v>
+        <v>1.180141721482433E-4</v>
       </c>
       <c r="J51">
-        <v>-6.5864321009717034E-4</v>
+        <v>-6.5869522768018346E-4</v>
       </c>
       <c r="K51">
-        <v>-2.0223756576863428E-6</v>
+        <v>-1.8807662234029791E-6</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2177,28 +2177,28 @@
         <v>-3.7050999999999999E-6</v>
       </c>
       <c r="D52">
-        <v>18784.912469093688</v>
+        <v>17045.887952831108</v>
       </c>
       <c r="E52">
-        <v>-19545163.301176891</v>
+        <v>-19547243.487801734</v>
       </c>
       <c r="F52">
-        <v>-50258.801415929935</v>
+        <v>-47222.749162333188</v>
       </c>
       <c r="G52">
-        <v>29910885658.516121</v>
+        <v>29913565285.046421</v>
       </c>
       <c r="H52">
-        <v>0.17971069948136137</v>
+        <v>0.17979763756889544</v>
       </c>
       <c r="I52">
-        <v>1.1806536365425991E-4</v>
+        <v>1.1806288298416565E-4</v>
       </c>
       <c r="J52">
-        <v>-6.535495879863803E-4</v>
+        <v>-6.5356194832491858E-4</v>
       </c>
       <c r="K52">
-        <v>-3.9644801959779971E-6</v>
+        <v>-3.7249751479850185E-6</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2212,28 +2212,28 @@
         <v>-3.1369E-6</v>
       </c>
       <c r="D53">
-        <v>31756.762368204538</v>
+        <v>31810.553307261318</v>
       </c>
       <c r="E53">
-        <v>-19433528.76155147</v>
+        <v>-19444286.705933001</v>
       </c>
       <c r="F53">
-        <v>-41825.889710640513</v>
+        <v>-39953.070169072489</v>
       </c>
       <c r="G53">
-        <v>29923638775.061672</v>
+        <v>29940199349.290527</v>
       </c>
       <c r="H53">
-        <v>0.18120053209772619</v>
+        <v>0.18119912639815947</v>
       </c>
       <c r="I53">
-        <v>1.1873547881755491E-4</v>
+        <v>1.1873031507171909E-4</v>
       </c>
       <c r="J53">
-        <v>-6.4960142841036846E-4</v>
+        <v>-6.4958238058160822E-4</v>
       </c>
       <c r="K53">
-        <v>-3.3019166045973863E-6</v>
+        <v>-3.152217883556005E-6</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2247,28 +2247,28 @@
         <v>-1.4591999999999999E-6</v>
       </c>
       <c r="D54">
-        <v>45793.151799906511</v>
+        <v>46030.933141239453</v>
       </c>
       <c r="E54">
-        <v>-19379397.607608296</v>
+        <v>-19391244.773958568</v>
       </c>
       <c r="F54">
-        <v>-20496.363305351242</v>
+        <v>-20434.957183548137</v>
       </c>
       <c r="G54">
-        <v>29999507291.134853</v>
+        <v>30017905194.086548</v>
       </c>
       <c r="H54">
-        <v>0.18298004879640675</v>
+        <v>0.18296960008033947</v>
       </c>
       <c r="I54">
-        <v>1.1972365664546437E-4</v>
+        <v>1.1971974651671846E-4</v>
       </c>
       <c r="J54">
-        <v>-6.462429450431505E-4</v>
+        <v>-6.4620925179187621E-4</v>
       </c>
       <c r="K54">
-        <v>-1.6164093256455011E-6</v>
+        <v>-1.6104855970486623E-6</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2282,28 +2282,28 @@
         <v>3.9359999999999998E-7</v>
       </c>
       <c r="D55">
-        <v>51522.32592557231</v>
+        <v>52040.345561175607</v>
       </c>
       <c r="E55">
-        <v>-19372095.811816182</v>
+        <v>-19380515.652785897</v>
       </c>
       <c r="F55">
-        <v>4654.1746715834261</v>
+        <v>2830.6558973881934</v>
       </c>
       <c r="G55">
-        <v>30135025202.121334</v>
+        <v>30148262521.020409</v>
       </c>
       <c r="H55">
-        <v>0.18530225175153711</v>
+        <v>0.18527759110319236</v>
       </c>
       <c r="I55">
-        <v>1.2082439677762042E-4</v>
+        <v>1.2082162360744852E-4</v>
       </c>
       <c r="J55">
-        <v>-6.4314469061311575E-4</v>
+        <v>-6.4310903667254738E-4</v>
       </c>
       <c r="K55">
-        <v>3.661156794982235E-7</v>
+        <v>2.2255691211193855E-7</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2317,28 +2317,28 @@
         <v>1.8341999999999999E-6</v>
       </c>
       <c r="D56">
-        <v>50094.321894938126</v>
+        <v>51003.65371711133</v>
       </c>
       <c r="E56">
-        <v>-19409402.835353047</v>
+        <v>-19411480.209311519</v>
       </c>
       <c r="F56">
-        <v>24564.489198089028</v>
+        <v>22321.45679700531</v>
       </c>
       <c r="G56">
-        <v>30337169526.921307</v>
+        <v>30340668339.405308</v>
       </c>
       <c r="H56">
-        <v>0.18796594071389949</v>
+        <v>0.18792128480673503</v>
       </c>
       <c r="I56">
-        <v>1.2190625292674061E-4</v>
+        <v>1.2190532140370097E-4</v>
       </c>
       <c r="J56">
-        <v>-6.4009928270147777E-4</v>
+        <v>-6.400789498975355E-4</v>
       </c>
       <c r="K56">
-        <v>1.9238191611597229E-6</v>
+        <v>1.7478343577880147E-6</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2352,28 +2352,28 @@
         <v>2.5646E-6</v>
       </c>
       <c r="D57">
-        <v>42196.473479119129</v>
+        <v>43582.836809405591</v>
       </c>
       <c r="E57">
-        <v>-19466663.385712478</v>
+        <v>-19464609.265058983</v>
       </c>
       <c r="F57">
-        <v>34525.366911849531</v>
+        <v>32406.675907642999</v>
       </c>
       <c r="G57">
-        <v>30570167357.202095</v>
+        <v>30567340094.933075</v>
       </c>
       <c r="H57">
-        <v>0.19089523480754594</v>
+        <v>0.19082674264078844</v>
       </c>
       <c r="I57">
-        <v>1.229368633680701E-4</v>
+        <v>1.2293726315407811E-4</v>
       </c>
       <c r="J57">
-        <v>-6.3705503346858086E-4</v>
+        <v>-6.370551158510528E-4</v>
       </c>
       <c r="K57">
-        <v>2.6899572069000611E-6</v>
+        <v>2.5249727488934302E-6</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2387,28 +2387,28 @@
         <v>2.5523000000000001E-6</v>
       </c>
       <c r="D58">
-        <v>29097.525730762631</v>
+        <v>30310.977741361596</v>
       </c>
       <c r="E58">
-        <v>-19528423.860541064</v>
+        <v>-19522219.565580044</v>
       </c>
       <c r="F58">
-        <v>33961.332893330378</v>
+        <v>32999.587453838845</v>
       </c>
       <c r="G58">
-        <v>30805498349.654198</v>
+        <v>30796076418.070671</v>
       </c>
       <c r="H58">
-        <v>0.19405292709929023</v>
+        <v>0.1939928143065037</v>
       </c>
       <c r="I58">
-        <v>1.2396035022279055E-4</v>
+        <v>1.2396015907266717E-4</v>
       </c>
       <c r="J58">
-        <v>-6.341245964018769E-4</v>
+        <v>-6.3413620271565588E-4</v>
       </c>
       <c r="K58">
-        <v>2.6328055304405528E-6</v>
+        <v>2.5589390727550482E-6</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2422,28 +2422,28 @@
         <v>1.9263000000000001E-6</v>
       </c>
       <c r="D59">
-        <v>17371.265071565285</v>
+        <v>17056.446690602228</v>
       </c>
       <c r="E59">
-        <v>-19571393.023994781</v>
+        <v>-19567947.870363038</v>
       </c>
       <c r="F59">
-        <v>27902.751884073987</v>
+        <v>28092.596099565628</v>
       </c>
       <c r="G59">
-        <v>30998332363.273384</v>
+        <v>30992779874.723587</v>
       </c>
       <c r="H59">
-        <v>0.19712601314155648</v>
+        <v>0.19714129881838088</v>
       </c>
       <c r="I59">
-        <v>1.2502331453931737E-4</v>
+        <v>1.2502302219805024E-4</v>
       </c>
       <c r="J59">
-        <v>-6.3148641176400777E-4</v>
+        <v>-6.3149961505167581E-4</v>
       </c>
       <c r="K59">
-        <v>2.1551847660663745E-6</v>
+        <v>2.1703017823620271E-6</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2457,28 +2457,28 @@
         <v>7.6183000000000004E-7</v>
       </c>
       <c r="D60">
-        <v>7594.5947754373774</v>
+        <v>6568.048539057374</v>
       </c>
       <c r="E60">
-        <v>-19607216.47644699</v>
+        <v>-19605022.312809385</v>
       </c>
       <c r="F60">
-        <v>12616.39252003356</v>
+        <v>12777.508719941277</v>
       </c>
       <c r="G60">
-        <v>31151191676.204086</v>
+        <v>31147380392.545612</v>
       </c>
       <c r="H60">
-        <v>0.20019361751266054</v>
+        <v>0.20024382791698866</v>
       </c>
       <c r="I60">
-        <v>1.2625359910233675E-4</v>
+        <v>1.2625694378787095E-4</v>
       </c>
       <c r="J60">
-        <v>-6.2947153153697583E-4</v>
+        <v>-6.2949090701201142E-4</v>
       </c>
       <c r="K60">
-        <v>9.72176061322114E-7</v>
+        <v>9.847824246527262E-7</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2492,28 +2492,28 @@
         <v>-2.2411E-6</v>
       </c>
       <c r="D61">
-        <v>5394.5823665531352</v>
+        <v>7633.0477393367328</v>
       </c>
       <c r="E61">
-        <v>-19634063.914272889</v>
+        <v>-19616323.009216748</v>
       </c>
       <c r="F61">
-        <v>-31730.090438942603</v>
+        <v>-30101.568924252344</v>
       </c>
       <c r="G61">
-        <v>29973973848.326557</v>
+        <v>29947498748.003807</v>
       </c>
       <c r="H61">
-        <v>0.18078309443658858</v>
+        <v>0.18067271781520283</v>
       </c>
       <c r="I61">
-        <v>1.1859868798481965E-4</v>
+        <v>1.1861092879982005E-4</v>
       </c>
       <c r="J61">
-        <v>-6.5511138122781093E-4</v>
+        <v>-6.5515442424753795E-4</v>
       </c>
       <c r="K61">
-        <v>-2.5000577764237343E-6</v>
+        <v>-2.3737875317650196E-6</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2527,28 +2527,28 @@
         <v>-4.5117000000000004E-6</v>
       </c>
       <c r="D62">
-        <v>8241.5714575918391</v>
+        <v>10550.363233648241</v>
       </c>
       <c r="E62">
-        <v>-19539766.05688113</v>
+        <v>-19541015.725587312</v>
       </c>
       <c r="F62">
-        <v>-61016.167717832097</v>
+        <v>-57849.903857647631</v>
       </c>
       <c r="G62">
-        <v>30044578507.181541</v>
+        <v>30047109787.924103</v>
       </c>
       <c r="H62">
-        <v>0.18222979276870838</v>
+        <v>0.18211654412257203</v>
       </c>
       <c r="I62">
-        <v>1.1877732150261644E-4</v>
+        <v>1.1878863709229904E-4</v>
       </c>
       <c r="J62">
-        <v>-6.5039923890945197E-4</v>
+        <v>-6.5041363958130141E-4</v>
       </c>
       <c r="K62">
-        <v>-4.8017380499371619E-6</v>
+        <v>-4.5518888410779872E-6</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2562,28 +2562,28 @@
         <v>-3.9497999999999999E-6</v>
       </c>
       <c r="D63">
-        <v>18906.123635229189</v>
+        <v>18853.023670815397</v>
       </c>
       <c r="E63">
-        <v>-19452957.46073338</v>
+        <v>-19462368.984319557</v>
       </c>
       <c r="F63">
-        <v>-54157.075959804075</v>
+        <v>-51944.115513212142</v>
       </c>
       <c r="G63">
-        <v>30095524003.046329</v>
+        <v>30110044589.833221</v>
       </c>
       <c r="H63">
-        <v>0.18368778117601561</v>
+        <v>0.18369147654356566</v>
       </c>
       <c r="I63">
-        <v>1.1935197593905468E-4</v>
+        <v>1.1935788424802496E-4</v>
       </c>
       <c r="J63">
-        <v>-6.4646368298550442E-4</v>
+        <v>-6.4645007285464009E-4</v>
       </c>
       <c r="K63">
-        <v>-4.2599247505902861E-6</v>
+        <v>-4.0838523341463987E-6</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2597,28 +2597,28 @@
         <v>-2.0140000000000001E-6</v>
       </c>
       <c r="D64">
-        <v>26021.530828304123</v>
+        <v>24870.985406497028</v>
       </c>
       <c r="E64">
-        <v>-19405759.856169622</v>
+        <v>-19415407.332451712</v>
       </c>
       <c r="F64">
-        <v>-29509.293563220224</v>
+        <v>-29042.272471369019</v>
       </c>
       <c r="G64">
-        <v>30185683678.799549</v>
+        <v>30200354131.06834</v>
       </c>
       <c r="H64">
-        <v>0.18558299600487788</v>
+        <v>0.18564092906496868</v>
       </c>
       <c r="I64">
-        <v>1.2016669193902707E-4</v>
+        <v>1.2016939289825017E-4</v>
       </c>
       <c r="J64">
-        <v>-6.4301903541663999E-4</v>
+        <v>-6.4299058983243937E-4</v>
       </c>
       <c r="K64">
-        <v>-2.3179626430819451E-6</v>
+        <v>-2.2802039966011989E-6</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2632,28 +2632,28 @@
         <v>2.4084999999999999E-7</v>
       </c>
       <c r="D65">
-        <v>31976.189207663294</v>
+        <v>29906.129008769989</v>
       </c>
       <c r="E65">
-        <v>-19401385.912291918</v>
+        <v>-19407987.607301179</v>
       </c>
       <c r="F65">
-        <v>1334.7706268700795</v>
+        <v>-393.7344257567064</v>
       </c>
       <c r="G65">
-        <v>30333043255.778168</v>
+        <v>30342759157.448322</v>
       </c>
       <c r="H65">
-        <v>0.18760717314921588</v>
+        <v>0.18771062253243481</v>
       </c>
       <c r="I65">
-        <v>1.2105110850410029E-4</v>
+        <v>1.2105574269600421E-4</v>
       </c>
       <c r="J65">
-        <v>-6.3979887419809891E-4</v>
+        <v>-6.3977316601152197E-4</v>
       </c>
       <c r="K65">
-        <v>1.0451719090719125E-7</v>
+        <v>-3.0822735995255854E-8</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2667,28 +2667,28 @@
         <v>2.1055E-6</v>
       </c>
       <c r="D66">
-        <v>33491.840790631715</v>
+        <v>31110.311883753631</v>
       </c>
       <c r="E66">
-        <v>-19427217.138826445</v>
+        <v>-19429786.012396716</v>
       </c>
       <c r="F66">
-        <v>27804.456402856413</v>
+        <v>25349.281221541514</v>
       </c>
       <c r="G66">
-        <v>30524263866.921772</v>
+        <v>30527581935.587009</v>
       </c>
       <c r="H66">
-        <v>0.18983798412104824</v>
+        <v>0.18995668734703702</v>
       </c>
       <c r="I66">
-        <v>1.2192262695731425E-4</v>
+        <v>1.2193210197233736E-4</v>
       </c>
       <c r="J66">
-        <v>-6.3665762212143824E-4</v>
+        <v>-6.3664404369960081E-4</v>
       </c>
       <c r="K66">
-        <v>2.167640601960551E-6</v>
+        <v>1.9762049726969062E-6</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2702,28 +2702,28 @@
         <v>3.1677000000000002E-6</v>
       </c>
       <c r="D67">
-        <v>28853.862871553283</v>
+        <v>26668.455635876395</v>
       </c>
       <c r="E67">
-        <v>-19474694.608428564</v>
+        <v>-19472329.564865749</v>
       </c>
       <c r="F67">
-        <v>43512.597479904944</v>
+        <v>40976.00296890091</v>
       </c>
       <c r="G67">
-        <v>30746814525.281128</v>
+        <v>30742402015.808266</v>
       </c>
       <c r="H67">
-        <v>0.19237958755723419</v>
+        <v>0.19248803044390622</v>
       </c>
       <c r="I67">
-        <v>1.2279300473905079E-4</v>
+        <v>1.2280666888226231E-4</v>
       </c>
       <c r="J67">
-        <v>-6.3357774747168152E-4</v>
+        <v>-6.3357853566775395E-4</v>
       </c>
       <c r="K67">
-        <v>3.3749403227775407E-6</v>
+        <v>3.1789984649146456E-6</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2737,28 +2737,28 @@
         <v>3.3098000000000001E-6</v>
       </c>
       <c r="D68">
-        <v>20768.081120300107</v>
+        <v>19596.803385453299</v>
       </c>
       <c r="E68">
-        <v>-19522459.212166246</v>
+        <v>-19518982.952234607</v>
       </c>
       <c r="F68">
-        <v>45455.876543084152</v>
+        <v>44257.077610348948</v>
       </c>
       <c r="G68">
-        <v>30962049432.252838</v>
+        <v>30956166348.940155</v>
       </c>
       <c r="H68">
-        <v>0.19515178280108347</v>
+        <v>0.19520959023328499</v>
       </c>
       <c r="I68">
-        <v>1.2372006581252978E-4</v>
+        <v>1.2373458952974955E-4</v>
       </c>
       <c r="J68">
-        <v>-6.306673309016313E-4</v>
+        <v>-6.3067794072723163E-4</v>
       </c>
       <c r="K68">
-        <v>3.5092812314041141E-6</v>
+        <v>3.4176582248460728E-6</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2772,28 +2772,28 @@
         <v>2.6205000000000002E-6</v>
       </c>
       <c r="D69">
-        <v>9667.1684427508153</v>
+        <v>10322.077247548383</v>
       </c>
       <c r="E69">
-        <v>-19564765.763456512</v>
+        <v>-19561288.641388245</v>
       </c>
       <c r="F69">
-        <v>39035.534424193473</v>
+        <v>39228.355956927575</v>
       </c>
       <c r="G69">
-        <v>31153203111.912193</v>
+        <v>31147874618.31601</v>
       </c>
       <c r="H69">
-        <v>0.19817746854753218</v>
+        <v>0.19814518004963538</v>
       </c>
       <c r="I69">
-        <v>1.2476522047172149E-4</v>
+        <v>1.2477673382904375E-4</v>
       </c>
       <c r="J69">
-        <v>-6.2808473700211851E-4</v>
+        <v>-6.2810031834829752E-4</v>
       </c>
       <c r="K69">
-        <v>3.0026821756180735E-6</v>
+        <v>3.0180580861945226E-6</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2807,28 +2807,28 @@
         <v>1.1069999999999999E-6</v>
       </c>
       <c r="D70">
-        <v>2255.6162518342026</v>
+        <v>3339.0279052886181</v>
       </c>
       <c r="E70">
-        <v>-19576930.076773193</v>
+        <v>-19574510.170238052</v>
       </c>
       <c r="F70">
-        <v>19269.392202925956</v>
+        <v>19520.877434410988</v>
       </c>
       <c r="G70">
-        <v>31274291668.278645</v>
+        <v>31270774757.950253</v>
       </c>
       <c r="H70">
-        <v>0.20115423295152779</v>
+        <v>0.20110108560874393</v>
       </c>
       <c r="I70">
-        <v>1.2598578766649985E-4</v>
+        <v>1.2599157024467954E-4</v>
       </c>
       <c r="J70">
-        <v>-6.2599125849756364E-4</v>
+        <v>-6.2600735364648648E-4</v>
       </c>
       <c r="K70">
-        <v>1.4801576385574736E-6</v>
+        <v>1.4996211969474718E-6</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2842,28 +2842,28 @@
         <v>-2.3705E-6</v>
       </c>
       <c r="D71">
-        <v>546.11846595210955</v>
+        <v>-3000.9439296289347</v>
       </c>
       <c r="E71">
-        <v>-19573581.044403829</v>
+        <v>-19560673.556180269</v>
       </c>
       <c r="F71">
-        <v>-35763.954229185423</v>
+        <v>-32907.205658703089</v>
       </c>
       <c r="G71">
-        <v>30011352396.266186</v>
+        <v>29990543770.253361</v>
       </c>
       <c r="H71">
-        <v>0.18376258995701913</v>
+        <v>0.18393826933856439</v>
       </c>
       <c r="I71">
-        <v>1.1988603538191E-4</v>
+        <v>1.1989253080089751E-4</v>
       </c>
       <c r="J71">
-        <v>-6.5224412531758157E-4</v>
+        <v>-6.5227052288303585E-4</v>
       </c>
       <c r="K71">
-        <v>-2.821523278811848E-6</v>
+        <v>-2.5984409201852687E-6</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2877,28 +2877,28 @@
         <v>-4.6960999999999998E-6</v>
       </c>
       <c r="D72">
-        <v>10447.700657612178</v>
+        <v>3896.3421981781721</v>
       </c>
       <c r="E72">
-        <v>-19535590.592238612</v>
+        <v>-19534785.349273104</v>
       </c>
       <c r="F72">
-        <v>-66106.628489936193</v>
+        <v>-61620.675625047297</v>
       </c>
       <c r="G72">
-        <v>30143128459.029095</v>
+        <v>30139966637.190613</v>
       </c>
       <c r="H72">
-        <v>0.18482152941968372</v>
+        <v>0.18514684212937085</v>
       </c>
       <c r="I72">
-        <v>1.2014502405906105E-4</v>
+        <v>1.2015929723385157E-4</v>
       </c>
       <c r="J72">
-        <v>-6.4815872313185845E-4</v>
+        <v>-6.4817824701112131E-4</v>
       </c>
       <c r="K72">
-        <v>-5.1969580353718008E-6</v>
+        <v>-4.846332964739521E-6</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2912,28 +2912,28 @@
         <v>-4.1685E-6</v>
       </c>
       <c r="D73">
-        <v>6274.8418939169496</v>
+        <v>546.074103503488</v>
       </c>
       <c r="E73">
-        <v>-19470231.041351926</v>
+        <v>-19478988.693605278</v>
       </c>
       <c r="F73">
-        <v>-57667.559599690139</v>
+        <v>-54998.261248712784</v>
       </c>
       <c r="G73">
-        <v>30217315238.452488</v>
+        <v>30229217911.341671</v>
       </c>
       <c r="H73">
-        <v>0.18670465696953734</v>
+        <v>0.18698939660815503</v>
       </c>
       <c r="I73">
-        <v>1.2051639800491232E-4</v>
+        <v>1.2053162655035869E-4</v>
       </c>
       <c r="J73">
-        <v>-6.4435810330975467E-4</v>
+        <v>-6.4434786291176415E-4</v>
       </c>
       <c r="K73">
-        <v>-4.5294003098153221E-6</v>
+        <v>-4.319101301634206E-6</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2947,28 +2947,28 @@
         <v>-2.1983000000000002E-6</v>
       </c>
       <c r="D74">
-        <v>3662.9831257015467</v>
+        <v>-1242.9950752216391</v>
       </c>
       <c r="E74">
-        <v>-19437807.904079672</v>
+        <v>-19444307.578595497</v>
       </c>
       <c r="F74">
-        <v>-31942.91108781999</v>
+        <v>-31383.489691726416</v>
       </c>
       <c r="G74">
-        <v>30332865265.42651</v>
+        <v>30341559271.789429</v>
       </c>
       <c r="H74">
-        <v>0.18869477257172079</v>
+        <v>0.18893823809592614</v>
       </c>
       <c r="I74">
-        <v>1.2104543045387466E-4</v>
+        <v>1.2106026443062316E-4</v>
       </c>
       <c r="J74">
-        <v>-6.4082796221084926E-4</v>
+        <v>-6.408090072709898E-4</v>
       </c>
       <c r="K74">
-        <v>-2.5035609891102539E-6</v>
+        <v>-2.459500798568208E-6</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2982,28 +2982,28 @@
         <v>1.9805999999999999E-7</v>
       </c>
       <c r="D75">
-        <v>-287.46107546053827</v>
+        <v>-4334.3751577581279</v>
       </c>
       <c r="E75">
-        <v>-19432934.407409571</v>
+        <v>-19438090.816047531</v>
       </c>
       <c r="F75">
-        <v>1560.6593106670016</v>
+        <v>-133.24303680589188</v>
       </c>
       <c r="G75">
-        <v>30487251998.86647</v>
+        <v>30494128228.74567</v>
       </c>
       <c r="H75">
-        <v>0.1908647368229125</v>
+        <v>0.19106534187040544</v>
       </c>
       <c r="I75">
-        <v>1.2165472733202367E-4</v>
+        <v>1.2166735367922875E-4</v>
       </c>
       <c r="J75">
-        <v>-6.3740156848379617E-4</v>
+        <v>-6.3738531691029431E-4</v>
       </c>
       <c r="K75">
-        <v>1.2192145297106223E-7</v>
+        <v>-1.0408536633933416E-8</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3017,28 +3017,28 @@
         <v>2.2446999999999999E-6</v>
       </c>
       <c r="D76">
-        <v>-4997.8779295631684</v>
+        <v>-8991.0594336492941</v>
       </c>
       <c r="E76">
-        <v>-19450652.589918114</v>
+        <v>-19453368.883470703</v>
       </c>
       <c r="F76">
-        <v>30498.577982222716</v>
+        <v>28148.658034923854</v>
       </c>
       <c r="G76">
-        <v>30678717427.340221</v>
+        <v>30681769294.090961</v>
       </c>
       <c r="H76">
-        <v>0.19313965131424665</v>
+        <v>0.1933375717975459</v>
       </c>
       <c r="I76">
-        <v>1.222968283008869E-4</v>
+        <v>1.2230690890805015E-4</v>
       </c>
       <c r="J76">
-        <v>-6.3397624379545308E-4</v>
+        <v>-6.3396830567369984E-4</v>
       </c>
       <c r="K76">
-        <v>2.3722783939967088E-6</v>
+        <v>2.1896439771124012E-6</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3052,28 +3052,28 @@
         <v>3.4273000000000002E-6</v>
       </c>
       <c r="D77">
-        <v>-7202.7408084389754</v>
+        <v>-11611.600203420501</v>
       </c>
       <c r="E77">
-        <v>-19484633.329969857</v>
+        <v>-19481650.374316145</v>
       </c>
       <c r="F77">
-        <v>47772.608051003081</v>
+        <v>45169.41867793991</v>
       </c>
       <c r="G77">
-        <v>30896361810.974846</v>
+        <v>30890238075.404293</v>
       </c>
       <c r="H77">
-        <v>0.19537538046507802</v>
+        <v>0.19559370451526514</v>
       </c>
       <c r="I77">
-        <v>1.2299196114773175E-4</v>
+        <v>1.2300007587359138E-4</v>
       </c>
       <c r="J77">
-        <v>-6.3061139511477E-4</v>
+        <v>-6.3061069529248351E-4</v>
       </c>
       <c r="K77">
-        <v>3.6967502053050771E-6</v>
+        <v>3.4966710480582343E-6</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3087,28 +3087,28 @@
         <v>3.5425E-6</v>
       </c>
       <c r="D78">
-        <v>-6794.4770830301568</v>
+        <v>-11879.924630754162</v>
       </c>
       <c r="E78">
-        <v>-19516150.167137746</v>
+        <v>-19515695.568533812</v>
       </c>
       <c r="F78">
-        <v>49465.147032535686</v>
+        <v>47748.261931297253</v>
       </c>
       <c r="G78">
-        <v>31102300775.113487</v>
+        <v>31099953378.459255</v>
       </c>
       <c r="H78">
-        <v>0.19764343710234522</v>
+        <v>0.19789425343612357</v>
       </c>
       <c r="I78">
-        <v>1.2381298310044911E-4</v>
+        <v>1.238196023301464E-4</v>
       </c>
       <c r="J78">
-        <v>-6.2744219045808352E-4</v>
+        <v>-6.2744727009298503E-4</v>
       </c>
       <c r="K78">
-        <v>3.8095515002547695E-6</v>
+        <v>3.6784276533068788E-6</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3122,28 +3122,28 @@
         <v>2.7062999999999998E-6</v>
       </c>
       <c r="D79">
-        <v>-1195.6678600455634</v>
+        <v>-6209.3273286907934</v>
       </c>
       <c r="E79">
-        <v>-19557850.835537016</v>
+        <v>-19553289.164917685</v>
       </c>
       <c r="F79">
-        <v>41137.342724507689</v>
+        <v>39974.45188703094</v>
       </c>
       <c r="G79">
-        <v>31307751288.846371</v>
+        <v>31298832925.839443</v>
       </c>
       <c r="H79">
-        <v>0.19991670342932921</v>
+        <v>0.20016309948574509</v>
       </c>
       <c r="I79">
-        <v>1.2486507947542835E-4</v>
+        <v>1.2487175337248406E-4</v>
       </c>
       <c r="J79">
-        <v>-6.247008198044259E-4</v>
+        <v>-6.2471817377680958E-4</v>
       </c>
       <c r="K79">
-        <v>3.1534174968982608E-6</v>
+        <v>3.0658744658330905E-6</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3157,28 +3157,28 @@
         <v>1.1195E-6</v>
       </c>
       <c r="D80">
-        <v>2081.4032796286047</v>
+        <v>-351.78670966345817</v>
       </c>
       <c r="E80">
-        <v>-19540568.087953094</v>
+        <v>-19539150.015059311</v>
       </c>
       <c r="F80">
-        <v>21046.718305631843</v>
+        <v>20002.084729680195</v>
       </c>
       <c r="G80">
-        <v>31400250199.552898</v>
+        <v>31397175430.26099</v>
       </c>
       <c r="H80">
-        <v>0.20251008135922363</v>
+        <v>0.20262960019032386</v>
       </c>
       <c r="I80">
-        <v>1.2609700824093488E-4</v>
+        <v>1.2609954976188945E-4</v>
       </c>
       <c r="J80">
-        <v>-6.2232293405589667E-4</v>
+        <v>-6.2233035271055644E-4</v>
       </c>
       <c r="K80">
-        <v>1.6120417763113709E-6</v>
+        <v>1.5323520053305353E-6</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3192,28 +3192,28 @@
         <v>-2.0524999999999998E-6</v>
       </c>
       <c r="D81">
-        <v>-2771.8793644011021</v>
+        <v>-455.4016686193645</v>
       </c>
       <c r="E81">
-        <v>-19518557.827183712</v>
+        <v>-19512550.865275774</v>
       </c>
       <c r="F81">
-        <v>-28809.592477663165</v>
+        <v>-24698.013733591193</v>
       </c>
       <c r="G81">
-        <v>30021300644.157509</v>
+        <v>30012707743.184231</v>
       </c>
       <c r="H81">
-        <v>0.18721942398618935</v>
+        <v>0.18710546430659317</v>
       </c>
       <c r="I81">
-        <v>1.2162730863535828E-4</v>
+        <v>1.2162397153411874E-4</v>
       </c>
       <c r="J81">
-        <v>-6.5015525643981548E-4</v>
+        <v>-6.5016293024506081E-4</v>
       </c>
       <c r="K81">
-        <v>-2.278641633048431E-6</v>
+        <v>-1.953824337842195E-6</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3227,28 +3227,28 @@
         <v>-3.9267E-6</v>
       </c>
       <c r="D82">
-        <v>-39826.260114990175</v>
+        <v>-37661.033214484807</v>
       </c>
       <c r="E82">
-        <v>-19528569.369198266</v>
+        <v>-19525110.376377668</v>
       </c>
       <c r="F82">
-        <v>-52372.99478633621</v>
+        <v>-45968.901367059807</v>
       </c>
       <c r="G82">
-        <v>30179972119.981674</v>
+        <v>30175207886.714306</v>
       </c>
       <c r="H82">
-        <v>0.19022516399559913</v>
+        <v>0.19012022534031878</v>
       </c>
       <c r="I82">
-        <v>1.217691886048367E-4</v>
+        <v>1.2175753834909979E-4</v>
       </c>
       <c r="J82">
-        <v>-6.4682468680899319E-4</v>
+        <v>-6.4683939397724771E-4</v>
       </c>
       <c r="K82">
-        <v>-4.1309552703885921E-6</v>
+        <v>-3.6260832242296544E-6</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3262,28 +3262,28 @@
         <v>-3.5599E-6</v>
       </c>
       <c r="D83">
-        <v>-56376.915970219299</v>
+        <v>-59121.501922517084</v>
       </c>
       <c r="E83">
-        <v>-19486438.150919847</v>
+        <v>-19493602.952467706</v>
       </c>
       <c r="F83">
-        <v>-51019.168838151971</v>
+        <v>-46597.924873810007</v>
       </c>
       <c r="G83">
-        <v>30279295710.394665</v>
+        <v>30289561624.809975</v>
       </c>
       <c r="H83">
-        <v>0.19208998799880972</v>
+        <v>0.19222566397417806</v>
       </c>
       <c r="I83">
-        <v>1.2176921531601435E-4</v>
+        <v>1.2175260477050747E-4</v>
       </c>
       <c r="J83">
-        <v>-6.4318189727686353E-4</v>
+        <v>-6.4317130948457349E-4</v>
       </c>
       <c r="K83">
-        <v>-4.0171947472927676E-6</v>
+        <v>-3.668105802703478E-6</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3297,28 +3297,28 @@
         <v>-1.8969E-6</v>
       </c>
       <c r="D84">
-        <v>-62403.127901489846</v>
+        <v>-68276.990344908088</v>
       </c>
       <c r="E84">
-        <v>-19466840.878038667</v>
+        <v>-19469688.182040755</v>
       </c>
       <c r="F84">
-        <v>-29424.891325015069</v>
+        <v>-28571.747695968133</v>
       </c>
       <c r="G84">
-        <v>30415662113.612724</v>
+        <v>30418299004.987659</v>
       </c>
       <c r="H84">
-        <v>0.19371234895586142</v>
+        <v>0.19400238172503234</v>
       </c>
       <c r="I84">
-        <v>1.2195046891625815E-4</v>
+        <v>1.2193750812132461E-4</v>
       </c>
       <c r="J84">
-        <v>-6.3962933388377313E-4</v>
+        <v>-6.3961312641438702E-4</v>
       </c>
       <c r="K84">
-        <v>-2.3097193766986532E-6</v>
+        <v>-2.2430154562129954E-6</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3332,28 +3332,28 @@
         <v>2.3398999999999999E-7</v>
       </c>
       <c r="D85">
-        <v>-61827.553369420115</v>
+        <v>-68347.748708378524</v>
       </c>
       <c r="E85">
-        <v>-19467980.396672193</v>
+        <v>-19471144.295924392</v>
       </c>
       <c r="F85">
-        <v>2412.8253139539074</v>
+        <v>299.32770591577975</v>
       </c>
       <c r="G85">
-        <v>30592971515.278664</v>
+        <v>30595909223.369419</v>
       </c>
       <c r="H85">
-        <v>0.19528571723203669</v>
+        <v>0.19560731204092552</v>
       </c>
       <c r="I85">
-        <v>1.2227126064712495E-4</v>
+        <v>1.222624432902644E-4</v>
       </c>
       <c r="J85">
-        <v>-6.3595740052130702E-4</v>
+        <v>-6.3594754236991589E-4</v>
       </c>
       <c r="K85">
-        <v>1.8854569704823687E-7</v>
+        <v>2.33938705750808E-8</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3367,28 +3367,28 @@
         <v>2.0866999999999999E-6</v>
       </c>
       <c r="D86">
-        <v>-56682.054795323405</v>
+        <v>-61094.622217683122</v>
       </c>
       <c r="E86">
-        <v>-19471343.854145087</v>
+        <v>-19473984.999170534</v>
       </c>
       <c r="F86">
-        <v>30073.426859771411</v>
+        <v>26272.57654924475</v>
       </c>
       <c r="G86">
-        <v>30784139352.5369</v>
+        <v>30786900934.936863</v>
       </c>
       <c r="H86">
-        <v>0.19691462798723117</v>
+        <v>0.19713258833496994</v>
       </c>
       <c r="I86">
-        <v>1.227240374447488E-4</v>
+        <v>1.2271697051785519E-4</v>
       </c>
       <c r="J86">
-        <v>-6.3214684154723607E-4</v>
+        <v>-6.3213909626025225E-4</v>
       </c>
       <c r="K86">
-        <v>2.3385989828261788E-6</v>
+        <v>2.0431799091220719E-6</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3402,28 +3402,28 @@
         <v>3.1294000000000001E-6</v>
       </c>
       <c r="D87">
-        <v>-51006.438602563459</v>
+        <v>-51903.371008773334</v>
       </c>
       <c r="E87">
-        <v>-19496821.504667308</v>
+        <v>-19493313.482409127</v>
       </c>
       <c r="F87">
-        <v>46002.002362123916</v>
+        <v>42053.962915331853</v>
       </c>
       <c r="G87">
-        <v>31014484562.101761</v>
+        <v>31008579705.876579</v>
       </c>
       <c r="H87">
-        <v>0.19880129599962471</v>
+        <v>0.19884682286677768</v>
       </c>
       <c r="I87">
-        <v>1.2333626783424847E-4</v>
+        <v>1.2332939330277629E-4</v>
       </c>
       <c r="J87">
-        <v>-6.283208860639153E-4</v>
+        <v>-6.2831954477829844E-4</v>
       </c>
       <c r="K87">
-        <v>3.5563162615356685E-6</v>
+        <v>3.2518028667966048E-6</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3437,28 +3437,28 @@
         <v>3.0937000000000001E-6</v>
       </c>
       <c r="D88">
-        <v>-45065.264005239122</v>
+        <v>-42472.391093106475</v>
       </c>
       <c r="E88">
-        <v>-19505208.133810811</v>
+        <v>-19507278.589631751</v>
       </c>
       <c r="F88">
-        <v>45397.439722016905</v>
+        <v>42454.883135079988</v>
       </c>
       <c r="G88">
-        <v>31209369314.297672</v>
+        <v>31213500675.871017</v>
       </c>
       <c r="H88">
-        <v>0.20092360929796571</v>
+        <v>0.20079647491577993</v>
       </c>
       <c r="I88">
-        <v>1.2412363883396269E-4</v>
+        <v>1.241125770982339E-4</v>
       </c>
       <c r="J88">
-        <v>-6.2468217945584742E-4</v>
+        <v>-6.2467998266435305E-4</v>
       </c>
       <c r="K88">
-        <v>3.493691410873679E-6</v>
+        <v>3.2663978559955772E-6</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3472,28 +3472,28 @@
         <v>2.0702000000000001E-6</v>
       </c>
       <c r="D89">
-        <v>-35347.345776624046</v>
+        <v>-30743.708767697681</v>
       </c>
       <c r="E89">
-        <v>-19546134.113766059</v>
+        <v>-19540531.768169846</v>
       </c>
       <c r="F89">
-        <v>29291.620477213455</v>
+        <v>27236.496154561773</v>
       </c>
       <c r="G89">
-        <v>31433841553.106678</v>
+        <v>31426332719.695374</v>
       </c>
       <c r="H89">
-        <v>0.20313695471912604</v>
+        <v>0.2029118602699353</v>
       </c>
       <c r="I89">
-        <v>1.2518207589557031E-4</v>
+        <v>1.2517353272603992E-4</v>
       </c>
       <c r="J89">
-        <v>-6.2159971203358403E-4</v>
+        <v>-6.2161315476648741E-4</v>
       </c>
       <c r="K89">
-        <v>2.2422928374374144E-6</v>
+        <v>2.0850921271147252E-6</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3507,28 +3507,28 @@
         <v>6.4796000000000004E-7</v>
       </c>
       <c r="D90">
-        <v>-13022.443196480162</v>
+        <v>-10487.969428312033</v>
       </c>
       <c r="E90">
-        <v>-19512105.771598019</v>
+        <v>-19512794.488532148</v>
       </c>
       <c r="F90">
-        <v>8449.3326920352192</v>
+        <v>7519.3412102170487</v>
       </c>
       <c r="G90">
-        <v>31515122451.388397</v>
+        <v>31517074782.572021</v>
       </c>
       <c r="H90">
-        <v>0.20496866684369422</v>
+        <v>0.20484424746035096</v>
       </c>
       <c r="I90">
-        <v>1.2648356346962793E-4</v>
+        <v>1.2647848014292842E-4</v>
       </c>
       <c r="J90">
-        <v>-6.1904696934790256E-4</v>
+        <v>-6.1904502144937562E-4</v>
       </c>
       <c r="K90">
-        <v>6.4610580895055683E-7</v>
+        <v>5.7489052212537223E-7</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3542,28 +3542,28 @@
         <v>-7.7293999999999998E-7</v>
       </c>
       <c r="D91">
-        <v>-20548.830917146523</v>
+        <v>-19618.503207665402</v>
       </c>
       <c r="E91">
-        <v>-19484766.766594984</v>
+        <v>-19484106.788605209</v>
       </c>
       <c r="F91">
-        <v>-5421.7411937053039</v>
+        <v>-4395.8127762935401</v>
       </c>
       <c r="G91">
-        <v>29994038732.721886</v>
+        <v>29993297289.169518</v>
       </c>
       <c r="H91">
-        <v>0.19147344494700971</v>
+        <v>0.19142750701619446</v>
       </c>
       <c r="I91">
-        <v>1.2369783169271478E-4</v>
+        <v>1.2369689641746951E-4</v>
       </c>
       <c r="J91">
-        <v>-6.4949185283624377E-4</v>
+        <v>-6.4949138652944461E-4</v>
       </c>
       <c r="K91">
-        <v>-4.3074264550590352E-7</v>
+        <v>-3.4922992917397339E-7</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3577,28 +3577,28 @@
         <v>-1.6673999999999999E-6</v>
       </c>
       <c r="D92">
-        <v>-40598.508036150597</v>
+        <v>-34282.066870448645</v>
       </c>
       <c r="E92">
-        <v>-19525112.778229348</v>
+        <v>-19521672.017066762</v>
       </c>
       <c r="F92">
-        <v>-20470.493596479893</v>
+        <v>-15957.462117574716</v>
       </c>
       <c r="G92">
-        <v>30198036237.223198</v>
+        <v>30194595521.891518</v>
       </c>
       <c r="H92">
-        <v>0.19257723647233349</v>
+        <v>0.19226642517550252</v>
       </c>
       <c r="I92">
-        <v>1.2315418969750889E-4</v>
+        <v>1.2314804518610346E-4</v>
       </c>
       <c r="J92">
-        <v>-6.4631473893446987E-4</v>
+        <v>-6.4632221975776836E-4</v>
       </c>
       <c r="K92">
-        <v>-1.6168130811807999E-6</v>
+        <v>-1.2601782624376869E-6</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3612,28 +3612,28 @@
         <v>-1.6525000000000001E-6</v>
       </c>
       <c r="D93">
-        <v>-82586.887366747484</v>
+        <v>-68279.116249450017</v>
       </c>
       <c r="E93">
-        <v>-19483502.440691274</v>
+        <v>-19488184.907574106</v>
       </c>
       <c r="F93">
-        <v>-27774.384081397882</v>
+        <v>-24268.278496856801</v>
       </c>
       <c r="G93">
-        <v>30280196058.687946</v>
+        <v>30291870440.472782</v>
       </c>
       <c r="H93">
-        <v>0.19472936298091051</v>
+        <v>0.19402240375385055</v>
       </c>
       <c r="I93">
-        <v>1.2253000525948201E-4</v>
+        <v>1.2250346053612826E-4</v>
       </c>
       <c r="J93">
-        <v>-6.4288910896659335E-4</v>
+        <v>-6.4287919659757314E-4</v>
       </c>
       <c r="K93">
-        <v>-2.1915506413423304E-6</v>
+        <v>-1.9129361058262823E-6</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3647,28 +3647,28 @@
         <v>-8.8332E-7</v>
       </c>
       <c r="D94">
-        <v>-118664.09326798469</v>
+        <v>-100102.60081182048</v>
       </c>
       <c r="E94">
-        <v>-19500240.077943567</v>
+        <v>-19498518.871966507</v>
       </c>
       <c r="F94">
-        <v>-15531.109077218276</v>
+        <v>-14960.527640280061</v>
       </c>
       <c r="G94">
-        <v>30465957649.004864</v>
+        <v>30469122533.261196</v>
       </c>
       <c r="H94">
-        <v>0.19686193994413204</v>
+        <v>0.19594725042957675</v>
       </c>
       <c r="I94">
-        <v>1.2206617846056045E-4</v>
+        <v>1.2202456506321988E-4</v>
       </c>
       <c r="J94">
-        <v>-6.3929679640329067E-4</v>
+        <v>-6.3928761482148159E-4</v>
       </c>
       <c r="K94">
-        <v>-1.2202115472256109E-6</v>
+        <v>-1.1742847200349286E-6</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3682,28 +3682,28 @@
         <v>1.4308000000000001E-7</v>
       </c>
       <c r="D95">
-        <v>-131404.68575084163</v>
+        <v>-113194.57228704775</v>
       </c>
       <c r="E95">
-        <v>-19482887.483509433</v>
+        <v>-19486219.037065025</v>
       </c>
       <c r="F95">
-        <v>436.40706982155103</v>
+        <v>-711.53904409959659</v>
       </c>
       <c r="G95">
-        <v>30620824366.767307</v>
+        <v>30631922021.745312</v>
       </c>
       <c r="H95">
-        <v>0.19869365688320573</v>
+        <v>0.19779472750046181</v>
       </c>
       <c r="I95">
-        <v>1.2208625459110404E-4</v>
+        <v>1.2203988945467934E-4</v>
       </c>
       <c r="J95">
-        <v>-6.3539285820815583E-4</v>
+        <v>-6.3537892444688431E-4</v>
       </c>
       <c r="K95">
-        <v>3.4164745257251466E-8</v>
+        <v>-5.5637472590446685E-8</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3717,28 +3717,28 @@
         <v>1.0394E-6</v>
       </c>
       <c r="D96">
-        <v>-117257.87128599035</v>
+        <v>-103146.84279758669</v>
       </c>
       <c r="E96">
-        <v>-19498163.510840867</v>
+        <v>-19497011.456440561</v>
       </c>
       <c r="F96">
-        <v>16447.112312740515</v>
+        <v>13406.371235180402</v>
       </c>
       <c r="G96">
-        <v>30850523679.062454</v>
+        <v>30853277003.881588</v>
       </c>
       <c r="H96">
-        <v>0.20013694726146131</v>
+        <v>0.19944263478351754</v>
       </c>
       <c r="I96">
-        <v>1.2265952833565919E-4</v>
+        <v>1.2262083812218996E-4</v>
       </c>
       <c r="J96">
-        <v>-6.3125701993819614E-4</v>
+        <v>-6.3125021658555231E-4</v>
       </c>
       <c r="K96">
-        <v>1.2795841819266546E-6</v>
+        <v>1.042254901146341E-6</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3752,28 +3752,28 @@
         <v>1.5324999999999999E-6</v>
       </c>
       <c r="D97">
-        <v>-82077.255282173865</v>
+        <v>-73681.908172719181</v>
       </c>
       <c r="E97">
-        <v>-19494309.187987357</v>
+        <v>-19494685.204471983</v>
       </c>
       <c r="F97">
-        <v>24586.300382609137</v>
+        <v>21922.277914114697</v>
       </c>
       <c r="G97">
-        <v>31065072086.464699</v>
+        <v>31068403397.023418</v>
       </c>
       <c r="H97">
-        <v>0.2012993752513996</v>
+        <v>0.20088637402528756</v>
       </c>
       <c r="I97">
-        <v>1.236622104722545E-4</v>
+        <v>1.2363576013390816E-4</v>
       </c>
       <c r="J97">
-        <v>-6.2699568100676789E-4</v>
+        <v>-6.2698818170075967E-4</v>
       </c>
       <c r="K97">
-        <v>1.9014712443637428E-6</v>
+        <v>1.6945969691507627E-6</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3787,28 +3787,28 @@
         <v>1.4609000000000001E-6</v>
       </c>
       <c r="D98">
-        <v>-39357.274574467447</v>
+        <v>-36202.641727597453</v>
       </c>
       <c r="E98">
-        <v>-19506777.938895628</v>
+        <v>-19506624.433555204</v>
       </c>
       <c r="F98">
-        <v>24904.953484223595</v>
+        <v>22533.442058970053</v>
       </c>
       <c r="G98">
-        <v>31303300823.305454</v>
+        <v>31304077500.302967</v>
       </c>
       <c r="H98">
-        <v>0.20244878899318022</v>
+        <v>0.20229399077741747</v>
       </c>
       <c r="I98">
-        <v>1.248934460043618E-4</v>
+        <v>1.2488303494343606E-4</v>
       </c>
       <c r="J98">
-        <v>-6.228984406725039E-4</v>
+        <v>-6.228975715552457E-4</v>
       </c>
       <c r="K98">
-        <v>1.9133220034331204E-6</v>
+        <v>1.7308377958645017E-6</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3822,28 +3822,28 @@
         <v>7.8472E-7</v>
       </c>
       <c r="D99">
-        <v>-6754.7172700888477</v>
+        <v>-7104.0011142236181</v>
       </c>
       <c r="E99">
-        <v>-19514116.207767718</v>
+        <v>-19512373.837993585</v>
       </c>
       <c r="F99">
-        <v>10309.223629161434</v>
+        <v>9309.067264653755</v>
       </c>
       <c r="G99">
-        <v>31506206240.35096</v>
+        <v>31503275759.845673</v>
       </c>
       <c r="H99">
-        <v>0.20393889373057228</v>
+        <v>0.20395612879064043</v>
       </c>
       <c r="I99">
-        <v>1.261018873385418E-4</v>
+        <v>1.2610273987307172E-4</v>
       </c>
       <c r="J99">
-        <v>-6.1933388659805811E-4</v>
+        <v>-6.1933887026701133E-4</v>
       </c>
       <c r="K99">
-        <v>7.8789374959118558E-7</v>
+        <v>7.1153756381727232E-7</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3857,28 +3857,28 @@
         <v>-5.1198E-8</v>
       </c>
       <c r="D100">
-        <v>393.53473403211683</v>
+        <v>-376.20281229075044</v>
       </c>
       <c r="E100">
-        <v>-19510123.607539542</v>
+        <v>-19510603.445260979</v>
       </c>
       <c r="F100">
-        <v>-7486.2689296795206</v>
+        <v>-6877.5383978366071</v>
       </c>
       <c r="G100">
-        <v>31640569899.216831</v>
+        <v>31641089708.048248</v>
       </c>
       <c r="H100">
-        <v>0.20625021115185385</v>
+        <v>0.20628800730980618</v>
       </c>
       <c r="I100">
-        <v>1.2719156562574125E-4</v>
+        <v>1.2719268059476385E-4</v>
       </c>
       <c r="J100">
-        <v>-6.1661924561812707E-4</v>
+        <v>-6.1661827615052756E-4</v>
       </c>
       <c r="K100">
-        <v>-5.7080678335375001E-7</v>
+        <v>-5.2440070043031223E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- added Gaussian and moving average filters
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\theia\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A0B507-1663-4944-A115-896A53F02D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB73FF7-3B9C-49F8-9F46-AE67064D4BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2898" yWindow="2898" windowWidth="16578" windowHeight="9444" xr2:uid="{BEE921D4-70B4-4CBA-B92B-ED4A2FE488D6}"/>
   </bookViews>
@@ -392,28 +392,28 @@
         <v>9.8638999999999993E-7</v>
       </c>
       <c r="D1">
-        <v>-52574.49324095156</v>
+        <v>-47047.705648741219</v>
       </c>
       <c r="E1">
-        <v>-19637559.673730545</v>
+        <v>-19612218.777395152</v>
       </c>
       <c r="F1">
-        <v>27198.29371853482</v>
+        <v>20918.903357329837</v>
       </c>
       <c r="G1">
-        <v>28554189234.009251</v>
+        <v>28518846959.097855</v>
       </c>
       <c r="H1">
-        <v>0.19053993175046344</v>
+        <v>0.19027243415419051</v>
       </c>
       <c r="I1">
-        <v>1.2920949927140387E-4</v>
+        <v>1.2920008037307603E-4</v>
       </c>
       <c r="J1">
-        <v>-6.875041999116838E-4</v>
+        <v>-6.8739386686173811E-4</v>
       </c>
       <c r="K1">
-        <v>2.2683927375611538E-6</v>
+        <v>1.7461896756991446E-6</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -427,28 +427,28 @@
         <v>1.0629E-6</v>
       </c>
       <c r="D2">
-        <v>-82098.303442748729</v>
+        <v>-60183.341167257167</v>
       </c>
       <c r="E2">
-        <v>-19597051.270668078</v>
+        <v>-19582579.313726109</v>
       </c>
       <c r="F2">
-        <v>15545.818495249572</v>
+        <v>10321.715663007195</v>
       </c>
       <c r="G2">
-        <v>28540719379.741333</v>
+        <v>28525759898.826687</v>
       </c>
       <c r="H2">
-        <v>0.18945495145104352</v>
+        <v>0.18837910062082308</v>
       </c>
       <c r="I2">
-        <v>1.2719464609811497E-4</v>
+        <v>1.2721277934731176E-4</v>
       </c>
       <c r="J2">
-        <v>-6.8614569788610241E-4</v>
+        <v>-6.8610606575834085E-4</v>
       </c>
       <c r="K2">
-        <v>1.2958310874412781E-6</v>
+        <v>8.600220868735511E-7</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -462,28 +462,28 @@
         <v>5.6680000000000002E-7</v>
       </c>
       <c r="D3">
-        <v>-96291.906450588722</v>
+        <v>-72651.875285565387</v>
       </c>
       <c r="E3">
-        <v>-19429589.007951941</v>
+        <v>-19441933.608082011</v>
       </c>
       <c r="F3">
-        <v>4097.600918829995</v>
+        <v>4175.5484432395479</v>
       </c>
       <c r="G3">
-        <v>28430721314.269814</v>
+        <v>28455481226.033035</v>
       </c>
       <c r="H3">
-        <v>0.18929870141310784</v>
+        <v>0.18812301442251217</v>
       </c>
       <c r="I3">
-        <v>1.2593021263157208E-4</v>
+        <v>1.2597654846403789E-4</v>
       </c>
       <c r="J3">
-        <v>-6.8264469313741524E-4</v>
+        <v>-6.8273851585720147E-4</v>
       </c>
       <c r="K3">
-        <v>3.4274725717266166E-7</v>
+        <v>3.4867879712165151E-7</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -497,28 +497,28 @@
         <v>2.6828999999999998E-7</v>
       </c>
       <c r="D4">
-        <v>-99838.385674901307</v>
+        <v>-78167.316555941943</v>
       </c>
       <c r="E4">
-        <v>-19363543.241970498</v>
+        <v>-19402466.159873668</v>
       </c>
       <c r="F4">
-        <v>1808.8738484155506</v>
+        <v>2923.5272089540845</v>
       </c>
       <c r="G4">
-        <v>28522550760.21537</v>
+        <v>28586140272.142601</v>
       </c>
       <c r="H4">
-        <v>0.19009150464079744</v>
+        <v>0.18900470237168984</v>
       </c>
       <c r="I4">
-        <v>1.2550321041655669E-4</v>
+        <v>1.2555125708062323E-4</v>
       </c>
       <c r="J4">
-        <v>-6.7812755402399871E-4</v>
+        <v>-6.7822391806356336E-4</v>
       </c>
       <c r="K4">
-        <v>1.509228556420333E-7</v>
+        <v>2.4320246891942855E-7</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -532,28 +532,28 @@
         <v>7.9642000000000006E-8</v>
       </c>
       <c r="D5">
-        <v>-99497.062710464001</v>
+        <v>-79871.633340924513</v>
       </c>
       <c r="E5">
-        <v>-19353756.207503397</v>
+        <v>-19378468.460848324</v>
       </c>
       <c r="F5">
-        <v>-862.02882056240742</v>
+        <v>-43.146110518205198</v>
       </c>
       <c r="G5">
-        <v>28738449601.332626</v>
+        <v>28780898024.765957</v>
       </c>
       <c r="H5">
-        <v>0.19198630732287406</v>
+        <v>0.19100436633098961</v>
       </c>
       <c r="I5">
-        <v>1.2578324766461313E-4</v>
+        <v>1.2582712829821999E-4</v>
       </c>
       <c r="J5">
-        <v>-6.726931818612855E-4</v>
+        <v>-6.7276132600068946E-4</v>
       </c>
       <c r="K5">
-        <v>-7.1496876573123001E-8</v>
+        <v>-3.5708280778871254E-9</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -567,28 +567,28 @@
         <v>-1.1014000000000001E-7</v>
       </c>
       <c r="D6">
-        <v>-96128.809375999961</v>
+        <v>-78040.303920174018</v>
       </c>
       <c r="E6">
-        <v>-19408667.078194577</v>
+        <v>-19416750.699542314</v>
       </c>
       <c r="F6">
-        <v>-2298.2913984574693</v>
+        <v>-1360.5618524248016</v>
       </c>
       <c r="G6">
-        <v>29084334628.9613</v>
+        <v>29101849228.460297</v>
       </c>
       <c r="H6">
-        <v>0.194770781836588</v>
+        <v>0.19387237344223701</v>
       </c>
       <c r="I6">
-        <v>1.2663351614645638E-4</v>
+        <v>1.2666959079990009E-4</v>
       </c>
       <c r="J6">
-        <v>-6.666454454945939E-4</v>
+        <v>-6.6667469848731846E-4</v>
       </c>
       <c r="K6">
-        <v>-1.8880855418788303E-7</v>
+        <v>-1.1163039869376262E-7</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -602,28 +602,28 @@
         <v>-3.6507000000000003E-7</v>
       </c>
       <c r="D7">
-        <v>-88290.778497054707</v>
+        <v>-71927.190088324714</v>
       </c>
       <c r="E7">
-        <v>-19488150.096440647</v>
+        <v>-19473754.695107389</v>
       </c>
       <c r="F7">
-        <v>-5607.0339427583776</v>
+        <v>-4729.2957270288043</v>
       </c>
       <c r="G7">
-        <v>29494291215.188057</v>
+        <v>29477483305.119827</v>
       </c>
       <c r="H7">
-        <v>0.19814578294240925</v>
+        <v>0.19734157872825828</v>
       </c>
       <c r="I7">
-        <v>1.2790353592574054E-4</v>
+        <v>1.2792956495333001E-4</v>
       </c>
       <c r="J7">
-        <v>-6.6015604719304359E-4</v>
+        <v>-6.6014591897772638E-4</v>
       </c>
       <c r="K7">
-        <v>-4.5553699736121844E-7</v>
+        <v>-3.8419494429245415E-7</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -637,28 +637,28 @@
         <v>-6.8467E-7</v>
       </c>
       <c r="D8">
-        <v>-74245.31761188386</v>
+        <v>-59823.571466428228</v>
       </c>
       <c r="E8">
-        <v>-19564828.535578143</v>
+        <v>-19531590.922716297</v>
       </c>
       <c r="F8">
-        <v>-9030.8860331184333</v>
+        <v>-7719.6000643490579</v>
       </c>
       <c r="G8">
-        <v>29923388985.933365</v>
+        <v>29877031241.331367</v>
       </c>
       <c r="H8">
-        <v>0.2017818590053097</v>
+        <v>0.20107968052249525</v>
       </c>
       <c r="I8">
-        <v>1.2943084466735094E-4</v>
+        <v>1.2944899932494953E-4</v>
       </c>
       <c r="J8">
-        <v>-6.5335335486259424E-4</v>
+        <v>-6.5332345072636523E-4</v>
       </c>
       <c r="K8">
-        <v>-7.2540003707681901E-7</v>
+        <v>-6.2066171465415812E-7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -672,28 +672,28 @@
         <v>-9.8098000000000009E-7</v>
       </c>
       <c r="D9">
-        <v>-52229.152718294878</v>
+        <v>-40992.692186202854</v>
       </c>
       <c r="E9">
-        <v>-19606674.406468868</v>
+        <v>-19584893.004257727</v>
       </c>
       <c r="F9">
-        <v>-14917.170945250087</v>
+        <v>-11677.611853121232</v>
       </c>
       <c r="G9">
-        <v>30326791961.517979</v>
+        <v>30296678259.083061</v>
       </c>
       <c r="H9">
-        <v>0.20522712919702216</v>
+        <v>0.204680548918727</v>
       </c>
       <c r="I9">
-        <v>1.3095524461778838E-4</v>
+        <v>1.3096173652642589E-4</v>
       </c>
       <c r="J9">
-        <v>-6.4622581411004408E-4</v>
+        <v>-6.4616926223837136E-4</v>
       </c>
       <c r="K9">
-        <v>-1.1857501000934713E-6</v>
+        <v>-9.2868199465778441E-7</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -707,28 +707,28 @@
         <v>-7.3865000000000001E-7</v>
       </c>
       <c r="D10">
-        <v>-24890.75978482049</v>
+        <v>-22127.465481420048</v>
       </c>
       <c r="E10">
-        <v>-19550180.481492933</v>
+        <v>-19575344.358450111</v>
       </c>
       <c r="F10">
-        <v>-15935.175840928887</v>
+        <v>-12809.479065078625</v>
       </c>
       <c r="G10">
-        <v>30632410444.567127</v>
+        <v>30672746660.546101</v>
       </c>
       <c r="H10">
-        <v>0.20816094010579747</v>
+        <v>0.20802455147557614</v>
       </c>
       <c r="I10">
-        <v>1.320322463924544E-4</v>
+        <v>1.3204139679686799E-4</v>
       </c>
       <c r="J10">
-        <v>-6.3804943118888648E-4</v>
+        <v>-6.3806154054529027E-4</v>
       </c>
       <c r="K10">
-        <v>-1.2569736090003222E-6</v>
+        <v>-1.0090019977620395E-6</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -742,28 +742,28 @@
         <v>1.5813E-6</v>
       </c>
       <c r="D11">
-        <v>37238.491016909014</v>
+        <v>33174.927488007117</v>
       </c>
       <c r="E11">
-        <v>-19683553.910390392</v>
+        <v>-19648127.402363796</v>
       </c>
       <c r="F11">
-        <v>37311.821682238471</v>
+        <v>30758.453720497328</v>
       </c>
       <c r="G11">
-        <v>28964567581.168037</v>
+        <v>28911336192.279854</v>
       </c>
       <c r="H11">
-        <v>0.18227937066241134</v>
+        <v>0.18247711078639436</v>
       </c>
       <c r="I11">
-        <v>1.252048631792662E-4</v>
+        <v>1.2516665976148342E-4</v>
       </c>
       <c r="J11">
-        <v>-6.7995913014005276E-4</v>
+        <v>-6.7982770670472754E-4</v>
       </c>
       <c r="K11">
-        <v>3.0467472840032162E-6</v>
+        <v>2.5161324744914335E-6</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -777,28 +777,28 @@
         <v>1.9032E-6</v>
       </c>
       <c r="D12">
-        <v>30271.592396956868</v>
+        <v>-4657.3210834716465</v>
       </c>
       <c r="E12">
-        <v>-19557563.242755894</v>
+        <v>-19551105.624372587</v>
       </c>
       <c r="F12">
-        <v>35043.009628027627</v>
+        <v>19299.594782257933</v>
       </c>
       <c r="G12">
-        <v>28879297943.221111</v>
+        <v>28860274017.048798</v>
       </c>
       <c r="H12">
-        <v>0.18236440839988444</v>
+        <v>0.18409263102808091</v>
       </c>
       <c r="I12">
-        <v>1.2458866440125268E-4</v>
+        <v>1.2473451776679259E-4</v>
       </c>
       <c r="J12">
-        <v>-6.7743587639711449E-4</v>
+        <v>-6.7733016661042649E-4</v>
       </c>
       <c r="K12">
-        <v>2.8696743608102107E-6</v>
+        <v>1.5809963358432629E-6</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -812,28 +812,28 @@
         <v>1.1694E-6</v>
       </c>
       <c r="D13">
-        <v>15978.404820718337</v>
+        <v>-8908.5630497752718</v>
       </c>
       <c r="E13">
-        <v>-19436580.771778539</v>
+        <v>-19462768.285742126</v>
       </c>
       <c r="F13">
-        <v>15123.341395588544</v>
+        <v>12613.944242025444</v>
       </c>
       <c r="G13">
-        <v>28831741610.175434</v>
+        <v>28863787952.639938</v>
       </c>
       <c r="H13">
-        <v>0.18344270580352753</v>
+        <v>0.18467932818554342</v>
       </c>
       <c r="I13">
-        <v>1.2424739674928492E-4</v>
+        <v>1.2437107764183197E-4</v>
       </c>
       <c r="J13">
-        <v>-6.7417165060788071E-4</v>
+        <v>-6.7396878207824878E-4</v>
       </c>
       <c r="K13">
-        <v>1.2414576118548464E-6</v>
+        <v>1.0321395132586427E-6</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -847,28 +847,28 @@
         <v>6.7472E-7</v>
       </c>
       <c r="D14">
-        <v>4973.0279171881266</v>
+        <v>-12027.556475960901</v>
       </c>
       <c r="E14">
-        <v>-19352299.119870096</v>
+        <v>-19404582.405758627</v>
       </c>
       <c r="F14">
-        <v>8006.7176727810029</v>
+        <v>6496.2334868500693</v>
       </c>
       <c r="G14">
-        <v>28872905917.122257</v>
+        <v>28946191482.081238</v>
       </c>
       <c r="H14">
-        <v>0.18523874360764903</v>
+        <v>0.18608538090352036</v>
       </c>
       <c r="I14">
-        <v>1.2435272640279809E-4</v>
+        <v>1.2443632942004247E-4</v>
       </c>
       <c r="J14">
-        <v>-6.7019102129844401E-4</v>
+        <v>-6.6993909368886497E-4</v>
       </c>
       <c r="K14">
-        <v>6.5729173180471964E-7</v>
+        <v>5.3061941991378177E-7</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -882,28 +882,28 @@
         <v>3.4219000000000002E-7</v>
       </c>
       <c r="D15">
-        <v>-2902.8463025172241</v>
+        <v>-14266.644718795684</v>
       </c>
       <c r="E15">
-        <v>-19355634.752403524</v>
+        <v>-19392152.783639088</v>
       </c>
       <c r="F15">
-        <v>1916.9677604145618</v>
+        <v>2462.784294918672</v>
       </c>
       <c r="G15">
-        <v>29075665224.83905</v>
+        <v>29127306114.216587</v>
       </c>
       <c r="H15">
-        <v>0.18777241513638648</v>
+        <v>0.18833741285478886</v>
       </c>
       <c r="I15">
-        <v>1.2492650499724343E-4</v>
+        <v>1.2497972501547962E-4</v>
       </c>
       <c r="J15">
-        <v>-6.6562065240490247E-4</v>
+        <v>-6.653709531994974E-4</v>
       </c>
       <c r="K15">
-        <v>1.5661390042297219E-7</v>
+        <v>2.0046552552754336E-7</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -917,28 +917,28 @@
         <v>-5.1307999999999999E-8</v>
       </c>
       <c r="D16">
-        <v>-7189.7051248415373</v>
+        <v>-15696.518307570568</v>
       </c>
       <c r="E16">
-        <v>-19402364.466673315</v>
+        <v>-19417962.40455813</v>
       </c>
       <c r="F16">
-        <v>-3124.06923358623</v>
+        <v>-1843.3876646934114</v>
       </c>
       <c r="G16">
-        <v>29370522861.789349</v>
+        <v>29391667103.784683</v>
       </c>
       <c r="H16">
-        <v>0.19089235975254443</v>
+        <v>0.19131418006402764</v>
       </c>
       <c r="I16">
-        <v>1.2588761068418062E-4</v>
+        <v>1.2591729120547501E-4</v>
       </c>
       <c r="J16">
-        <v>-6.6053086847458033E-4</v>
+        <v>-6.6036216554493914E-4</v>
       </c>
       <c r="K16">
-        <v>-2.5334402042453269E-7</v>
+        <v>-1.4844729368969079E-7</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -952,28 +952,28 @@
         <v>-6.4053999999999999E-7</v>
       </c>
       <c r="D17">
-        <v>-8984.1581835229881</v>
+        <v>-15677.365553935484</v>
       </c>
       <c r="E17">
-        <v>-19482585.674849831</v>
+        <v>-19467861.706474401</v>
       </c>
       <c r="F17">
-        <v>-11077.294040573363</v>
+        <v>-7616.7505365012357</v>
       </c>
       <c r="G17">
-        <v>29738565385.967209</v>
+        <v>29714087325.375237</v>
       </c>
       <c r="H17">
-        <v>0.19448391711547269</v>
+        <v>0.19481519829077315</v>
       </c>
       <c r="I17">
-        <v>1.2714042062669204E-4</v>
+        <v>1.2712987834029212E-4</v>
       </c>
       <c r="J17">
-        <v>-6.5508497208475883E-4</v>
+        <v>-6.5500205881417728E-4</v>
       </c>
       <c r="K17">
-        <v>-8.8991660568302168E-7</v>
+        <v>-6.0957310874419301E-7</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -987,28 +987,28 @@
         <v>-1.3919E-6</v>
       </c>
       <c r="D18">
-        <v>-6321.8810634822585</v>
+        <v>-13307.722770168246</v>
       </c>
       <c r="E18">
-        <v>-19558492.998047926</v>
+        <v>-19523258.774159584</v>
       </c>
       <c r="F18">
-        <v>-21266.340821899859</v>
+        <v>-14900.979331518703</v>
       </c>
       <c r="G18">
-        <v>30118657314.499115</v>
+        <v>30062234683.866032</v>
       </c>
       <c r="H18">
-        <v>0.19820342933926149</v>
+        <v>0.19854830605954035</v>
       </c>
       <c r="I18">
-        <v>1.2852845909858317E-4</v>
+        <v>1.2845758754115289E-4</v>
       </c>
       <c r="J18">
-        <v>-6.4937990124340006E-4</v>
+        <v>-6.4934500511234746E-4</v>
       </c>
       <c r="K18">
-        <v>-1.6922176284420111E-6</v>
+        <v>-1.1839128017385096E-6</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1022,28 +1022,28 @@
         <v>-2.0153999999999998E-6</v>
       </c>
       <c r="D19">
-        <v>2592.0772352721542</v>
+        <v>-8585.4158306831014</v>
       </c>
       <c r="E19">
-        <v>-19594370.525521912</v>
+        <v>-19567883.143185936</v>
       </c>
       <c r="F19">
-        <v>-33716.805124729326</v>
+        <v>-19588.917449873723</v>
       </c>
       <c r="G19">
-        <v>30456693233.291237</v>
+        <v>30411942514.892433</v>
       </c>
       <c r="H19">
-        <v>0.20157541154787978</v>
+        <v>0.20212506006581965</v>
       </c>
       <c r="I19">
-        <v>1.2979497428701622E-4</v>
+        <v>1.2964794916245747E-4</v>
       </c>
       <c r="J19">
-        <v>-6.4342217383073848E-4</v>
+        <v>-6.4334216089681809E-4</v>
       </c>
       <c r="K19">
-        <v>-2.6606584327019478E-6</v>
+        <v>-1.5460545429094213E-6</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1057,28 +1057,28 @@
         <v>-1.4313E-6</v>
       </c>
       <c r="D20">
-        <v>9294.6230011940934</v>
+        <v>8503.5487775113434</v>
       </c>
       <c r="E20">
-        <v>-19576554.537708156</v>
+        <v>-19597018.054959539</v>
       </c>
       <c r="F20">
-        <v>-28217.348918333031</v>
+        <v>-23596.352596402608</v>
       </c>
       <c r="G20">
-        <v>30735454281.670883</v>
+        <v>30767302393.616699</v>
       </c>
       <c r="H20">
-        <v>0.20456752166205233</v>
+        <v>0.20460727498196171</v>
       </c>
       <c r="I20">
-        <v>1.3061017235436992E-4</v>
+        <v>1.3060431578459193E-4</v>
       </c>
       <c r="J20">
-        <v>-6.3701717128366469E-4</v>
+        <v>-6.3701308910570553E-4</v>
       </c>
       <c r="K20">
-        <v>-2.2118426846807256E-6</v>
+        <v>-1.8477418057038023E-6</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1092,28 +1092,28 @@
         <v>6.5932E-7</v>
       </c>
       <c r="D21">
-        <v>-1941.8966078381054</v>
+        <v>-6064.2520098001696</v>
       </c>
       <c r="E21">
-        <v>-19717648.476236295</v>
+        <v>-19674121.641601287</v>
       </c>
       <c r="F21">
-        <v>14515.656357896365</v>
+        <v>15624.879600539611</v>
       </c>
       <c r="G21">
-        <v>29281967781.114414</v>
+        <v>29216220325.430004</v>
       </c>
       <c r="H21">
-        <v>0.18088972630679054</v>
+        <v>0.18109251899162057</v>
       </c>
       <c r="I21">
-        <v>1.2175691479906093E-4</v>
+        <v>1.2173751631178718E-4</v>
       </c>
       <c r="J21">
-        <v>-6.7350924264852267E-4</v>
+        <v>-6.733758657237977E-4</v>
       </c>
       <c r="K21">
-        <v>1.1710267859739443E-6</v>
+        <v>1.2633226166666083E-6</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1127,28 +1127,28 @@
         <v>8.9069000000000004E-7</v>
       </c>
       <c r="D22">
-        <v>33246.887300440576</v>
+        <v>22900.057494479202</v>
       </c>
       <c r="E22">
-        <v>-19542962.796934903</v>
+        <v>-19551922.094161425</v>
       </c>
       <c r="F22">
-        <v>22061.15697874633</v>
+        <v>15190.455902024119</v>
       </c>
       <c r="G22">
-        <v>29198475751.706978</v>
+        <v>29209072893.033623</v>
       </c>
       <c r="H22">
-        <v>0.17982666915469905</v>
+        <v>0.180340106289713</v>
       </c>
       <c r="I22">
-        <v>1.2149757127049362E-4</v>
+        <v>1.2203721167604686E-4</v>
       </c>
       <c r="J22">
-        <v>-6.6951854879784009E-4</v>
+        <v>-6.6979528585641313E-4</v>
       </c>
       <c r="K22">
-        <v>1.7828508254689752E-6</v>
+        <v>1.2354869385214325E-6</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1162,28 +1162,28 @@
         <v>7.1518000000000003E-7</v>
       </c>
       <c r="D23">
-        <v>56977.269174656831</v>
+        <v>30409.292559061734</v>
       </c>
       <c r="E23">
-        <v>-19428531.501888864</v>
+        <v>-19457711.013219301</v>
       </c>
       <c r="F23">
-        <v>13974.773695346206</v>
+        <v>11273.649018954398</v>
       </c>
       <c r="G23">
-        <v>29177311740.273926</v>
+        <v>29213981804.411964</v>
       </c>
       <c r="H23">
-        <v>0.18010349324496394</v>
+        <v>0.18142873241528046</v>
       </c>
       <c r="I23">
-        <v>1.2188434858381703E-4</v>
+        <v>1.2229050206032742E-4</v>
       </c>
       <c r="J23">
-        <v>-6.6617354425027944E-4</v>
+        <v>-6.6614727168883415E-4</v>
       </c>
       <c r="K23">
-        <v>1.1303713791186581E-6</v>
+        <v>9.1628301192445696E-7</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1197,28 +1197,28 @@
         <v>6.525E-7</v>
       </c>
       <c r="D24">
-        <v>65353.289393544197</v>
+        <v>34089.329819290324</v>
       </c>
       <c r="E24">
-        <v>-19351098.186510492</v>
+        <v>-19402065.522631124</v>
       </c>
       <c r="F24">
-        <v>9823.6009917357678</v>
+        <v>6954.565099808704</v>
       </c>
       <c r="G24">
-        <v>29216544239.458866</v>
+        <v>29284954503.467068</v>
       </c>
       <c r="H24">
-        <v>0.18166537245703185</v>
+        <v>0.18323181698488933</v>
       </c>
       <c r="I24">
-        <v>1.2256818833547675E-4</v>
+        <v>1.2287551059183541E-4</v>
       </c>
       <c r="J24">
-        <v>-6.6264125255950516E-4</v>
+        <v>-6.6248838793017413E-4</v>
       </c>
       <c r="K24">
-        <v>7.945410881971763E-7</v>
+        <v>5.6348599818358932E-7</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1232,28 +1232,28 @@
         <v>6.2223000000000003E-7</v>
       </c>
       <c r="D25">
-        <v>65195.068744348828</v>
+        <v>34102.172531661621</v>
       </c>
       <c r="E25">
-        <v>-19350472.855905831</v>
+        <v>-19389466.556397986</v>
       </c>
       <c r="F25">
-        <v>7741.2652099550769</v>
+        <v>4209.4789585501476</v>
       </c>
       <c r="G25">
-        <v>29388298533.175678</v>
+        <v>29438867677.335072</v>
       </c>
       <c r="H25">
-        <v>0.18417978333737783</v>
+        <v>0.18573518497666777</v>
       </c>
       <c r="I25">
-        <v>1.235103562367298E-4</v>
+        <v>1.2373885694862279E-4</v>
       </c>
       <c r="J25">
-        <v>-6.5879022815015938E-4</v>
+        <v>-6.5860425304128912E-4</v>
       </c>
       <c r="K25">
-        <v>6.2382569800269834E-7</v>
+        <v>3.3887839380430995E-7</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1267,28 +1267,28 @@
         <v>3.9292E-7</v>
       </c>
       <c r="D26">
-        <v>57412.610962906852</v>
+        <v>31161.334836705049</v>
       </c>
       <c r="E26">
-        <v>-19397842.0612523</v>
+        <v>-19413746.244458087</v>
       </c>
       <c r="F26">
-        <v>2777.7909017571874</v>
+        <v>731.29527794574392</v>
       </c>
       <c r="G26">
-        <v>29650019808.879314</v>
+        <v>29666857985.057251</v>
       </c>
       <c r="H26">
-        <v>0.18750938086978564</v>
+        <v>0.18881607029019462</v>
       </c>
       <c r="I26">
-        <v>1.2463431593735509E-4</v>
+        <v>1.2481502690858733E-4</v>
       </c>
       <c r="J26">
-        <v>-6.5456344689107529E-4</v>
+        <v>-6.5444593487090196E-4</v>
       </c>
       <c r="K26">
-        <v>2.2250528124368374E-7</v>
+        <v>5.7887955849446823E-8</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1302,28 +1302,28 @@
         <v>-1.6742E-7</v>
       </c>
       <c r="D27">
-        <v>47552.832364575472</v>
+        <v>26043.05976158577</v>
       </c>
       <c r="E27">
-        <v>-19472154.900890801</v>
+        <v>-19460941.465529647</v>
       </c>
       <c r="F27">
-        <v>-5216.666331783541</v>
+        <v>-5196.5419016687392</v>
       </c>
       <c r="G27">
-        <v>29968848517.921589</v>
+        <v>29945313191.825745</v>
       </c>
       <c r="H27">
-        <v>0.19123336343478484</v>
+        <v>0.19229664593316867</v>
       </c>
       <c r="I27">
-        <v>1.2586486261514904E-4</v>
+        <v>1.2601290307767479E-4</v>
       </c>
       <c r="J27">
-        <v>-6.5005844363854063E-4</v>
+        <v>-6.5002513834910912E-4</v>
       </c>
       <c r="K27">
-        <v>-4.1473295021561638E-7</v>
+        <v>-4.1403794765290055E-7</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1337,28 +1337,28 @@
         <v>-9.6919999999999997E-7</v>
       </c>
       <c r="D28">
-        <v>35650.200976342428</v>
+        <v>19482.474350580342</v>
       </c>
       <c r="E28">
-        <v>-19547159.988068908</v>
+        <v>-19515838.690527719</v>
       </c>
       <c r="F28">
-        <v>-17104.164160659919</v>
+        <v>-13136.090606921156</v>
       </c>
       <c r="G28">
-        <v>30301441971.825321</v>
+        <v>30248028815.919624</v>
       </c>
       <c r="H28">
-        <v>0.19517149319387755</v>
+        <v>0.19596573432756589</v>
       </c>
       <c r="I28">
-        <v>1.271044713803816E-4</v>
+        <v>1.272136306209006E-4</v>
       </c>
       <c r="J28">
-        <v>-6.4536651500028642E-4</v>
+        <v>-6.4539038806118694E-4</v>
       </c>
       <c r="K28">
-        <v>-1.3493947429254029E-6</v>
+        <v>-1.0389332304043913E-6</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1372,28 +1372,28 @@
         <v>-1.6011E-6</v>
       </c>
       <c r="D29">
-        <v>18529.35658733733</v>
+        <v>12269.07665681117</v>
       </c>
       <c r="E29">
-        <v>-19584659.998612054</v>
+        <v>-19568596.314826641</v>
       </c>
       <c r="F29">
-        <v>-28181.992870398666</v>
+        <v>-18098.154847539954</v>
       </c>
       <c r="G29">
-        <v>30580077837.558163</v>
+        <v>30553014593.467102</v>
       </c>
       <c r="H29">
-        <v>0.19922804526311969</v>
+        <v>0.19953566094173286</v>
       </c>
       <c r="I29">
-        <v>1.2821121524192252E-4</v>
+        <v>1.2827915092195402E-4</v>
       </c>
       <c r="J29">
-        <v>-6.405911618708141E-4</v>
+        <v>-6.4064856210351224E-4</v>
       </c>
       <c r="K29">
-        <v>-2.2104957227064761E-6</v>
+        <v>-1.4230301540047951E-6</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1407,28 +1407,28 @@
         <v>-1.1000000000000001E-6</v>
       </c>
       <c r="D30">
-        <v>971.12659987062216</v>
+        <v>-1213.2036048145965</v>
       </c>
       <c r="E30">
-        <v>-19607469.233699232</v>
+        <v>-19620191.803546209</v>
       </c>
       <c r="F30">
-        <v>-20391.420772648413</v>
+        <v>-18531.837482571271</v>
       </c>
       <c r="G30">
-        <v>30828715567.236919</v>
+        <v>30848014656.424847</v>
       </c>
       <c r="H30">
-        <v>0.20298017787182568</v>
+        <v>0.20308713145177679</v>
       </c>
       <c r="I30">
-        <v>1.2913335827741899E-4</v>
+        <v>1.2912981141097521E-4</v>
       </c>
       <c r="J30">
-        <v>-6.3604638118092236E-4</v>
+        <v>-6.360319743926446E-4</v>
       </c>
       <c r="K30">
-        <v>-1.5914679339405161E-6</v>
+        <v>-1.4455241683610431E-6</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1442,28 +1442,28 @@
         <v>-3.6991000000000001E-7</v>
       </c>
       <c r="D31">
-        <v>21154.74785068538</v>
+        <v>23411.555855162442</v>
       </c>
       <c r="E31">
-        <v>-19722539.060428768</v>
+        <v>-19682550.61462535</v>
       </c>
       <c r="F31">
-        <v>-1177.7248039361498</v>
+        <v>1902.3406392994389</v>
       </c>
       <c r="G31">
-        <v>29543657021.601696</v>
+        <v>29484364476.785431</v>
       </c>
       <c r="H31">
-        <v>0.1778293048731488</v>
+        <v>0.17771615209794386</v>
       </c>
       <c r="I31">
-        <v>1.1946806205292483E-4</v>
+        <v>1.1943939545334568E-4</v>
       </c>
       <c r="J31">
-        <v>-6.6784304836752027E-4</v>
+        <v>-6.6771711705537447E-4</v>
       </c>
       <c r="K31">
-        <v>-9.3927289610603454E-8</v>
+        <v>1.5197835155471035E-7</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1477,28 +1477,28 @@
         <v>-7.9564999999999995E-7</v>
       </c>
       <c r="D32">
-        <v>32957.998564688955</v>
+        <v>28062.424222745653</v>
       </c>
       <c r="E32">
-        <v>-19545159.714193176</v>
+        <v>-19552830.002914052</v>
       </c>
       <c r="F32">
-        <v>-5277.9280031790404</v>
+        <v>507.97350247226598</v>
       </c>
       <c r="G32">
-        <v>29490070980.568775</v>
+        <v>29500331610.061291</v>
       </c>
       <c r="H32">
-        <v>0.17831584955560659</v>
+        <v>0.17855896507849575</v>
       </c>
       <c r="I32">
-        <v>1.193095471715964E-4</v>
+        <v>1.1984927184320238E-4</v>
       </c>
       <c r="J32">
-        <v>-6.6296500624984261E-4</v>
+        <v>-6.633595001159779E-4</v>
       </c>
       <c r="K32">
-        <v>-4.2177586550998323E-7</v>
+        <v>4.823972166226263E-8</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1512,28 +1512,28 @@
         <v>-4.9912000000000004E-7</v>
       </c>
       <c r="D33">
-        <v>52435.477274132892</v>
+        <v>44137.009090475818</v>
       </c>
       <c r="E33">
-        <v>-19424942.213370148</v>
+        <v>-19456931.766595308</v>
       </c>
       <c r="F33">
-        <v>-3680.2663478076693</v>
+        <v>177.69284980643874</v>
       </c>
       <c r="G33">
-        <v>29473216022.637047</v>
+        <v>29519499677.414574</v>
       </c>
       <c r="H33">
-        <v>0.17932963433648244</v>
+        <v>0.17974672297840549</v>
       </c>
       <c r="I33">
-        <v>1.199623890843395E-4</v>
+        <v>1.2040515917408934E-4</v>
       </c>
       <c r="J33">
-        <v>-6.5933816191945244E-4</v>
+        <v>-6.594305423037076E-4</v>
       </c>
       <c r="K33">
-        <v>-2.9449894521117737E-7</v>
+        <v>2.0892791276033621E-8</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1547,28 +1547,28 @@
         <v>1.1864E-7</v>
       </c>
       <c r="D34">
-        <v>68189.958212159574</v>
+        <v>54752.987033438498</v>
       </c>
       <c r="E34">
-        <v>-19357436.821504183</v>
+        <v>-19402666.929990724</v>
       </c>
       <c r="F34">
-        <v>1531.8123484904038</v>
+        <v>1802.7440717828026</v>
       </c>
       <c r="G34">
-        <v>29523049448.036961</v>
+        <v>29588338528.739971</v>
       </c>
       <c r="H34">
-        <v>0.1809750617740144</v>
+        <v>0.1816527735144946</v>
       </c>
       <c r="I34">
-        <v>1.2095303765480075E-4</v>
+        <v>1.2134674683712156E-4</v>
       </c>
       <c r="J34">
-        <v>-6.5600023698685083E-4</v>
+        <v>-6.5597393483529328E-4</v>
       </c>
       <c r="K34">
-        <v>1.2253366481218032E-7</v>
+        <v>1.4744222317265215E-7</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1582,28 +1582,28 @@
         <v>6.9874999999999998E-7</v>
       </c>
       <c r="D35">
-        <v>74278.246955776587</v>
+        <v>58616.81920137089</v>
       </c>
       <c r="E35">
-        <v>-19351510.892674614</v>
+        <v>-19389982.80146876</v>
       </c>
       <c r="F35">
-        <v>8481.0215676835924</v>
+        <v>4376.854319129613</v>
       </c>
       <c r="G35">
-        <v>29669272034.946236</v>
+        <v>29723879714.569508</v>
       </c>
       <c r="H35">
-        <v>0.18340843040676869</v>
+        <v>0.18419635350003341</v>
       </c>
       <c r="I35">
-        <v>1.2211740970956362E-4</v>
+        <v>1.224485731062674E-4</v>
       </c>
       <c r="J35">
-        <v>-6.5263674693438029E-4</v>
+        <v>-6.5255644031371441E-4</v>
       </c>
       <c r="K35">
-        <v>6.7649315710371395E-7</v>
+        <v>3.4898728389714452E-7</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1617,28 +1617,28 @@
         <v>9.4620000000000004E-7</v>
       </c>
       <c r="D36">
-        <v>72694.390283033717</v>
+        <v>56174.832783749021</v>
       </c>
       <c r="E36">
-        <v>-19394040.813785322</v>
+        <v>-19411647.244306877</v>
       </c>
       <c r="F36">
-        <v>10631.627916071899</v>
+        <v>5396.3517225270771</v>
       </c>
       <c r="G36">
-        <v>29899227022.612877</v>
+        <v>29921671376.449345</v>
       </c>
       <c r="H36">
-        <v>0.18638607025039516</v>
+        <v>0.18721089182871628</v>
       </c>
       <c r="I36">
-        <v>1.233241761410133E-4</v>
+        <v>1.2362048849144579E-4</v>
       </c>
       <c r="J36">
-        <v>-6.4907135297588635E-4</v>
+        <v>-6.4901072123027417E-4</v>
       </c>
       <c r="K36">
-        <v>8.436773586864392E-7</v>
+        <v>4.2656320186800558E-7</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1652,28 +1652,28 @@
         <v>7.2341999999999995E-7</v>
       </c>
       <c r="D37">
-        <v>61841.882014318369</v>
+        <v>48262.439958050803</v>
       </c>
       <c r="E37">
-        <v>-19466193.517374862</v>
+        <v>-19455441.790785883</v>
       </c>
       <c r="F37">
-        <v>7658.5364268710437</v>
+        <v>3079.5314318932997</v>
       </c>
       <c r="G37">
-        <v>30184314129.828671</v>
+        <v>30163701174.188522</v>
       </c>
       <c r="H37">
-        <v>0.18993513817770391</v>
+        <v>0.19060628340097385</v>
       </c>
       <c r="I37">
-        <v>1.2454024085523693E-4</v>
+        <v>1.2479005244143528E-4</v>
       </c>
       <c r="J37">
-        <v>-6.4530508813455834E-4</v>
+        <v>-6.4529964464728705E-4</v>
       </c>
       <c r="K37">
-        <v>6.0383836617884136E-7</v>
+        <v>2.4074253855879914E-7</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1687,28 +1687,28 @@
         <v>1.3049E-7</v>
       </c>
       <c r="D38">
-        <v>44515.670457735192</v>
+        <v>35889.869075736162</v>
       </c>
       <c r="E38">
-        <v>-19533913.746838801</v>
+        <v>-19509421.168940678</v>
       </c>
       <c r="F38">
-        <v>-548.12449535759129</v>
+        <v>-2066.4106198786044</v>
       </c>
       <c r="G38">
-        <v>30466666929.936077</v>
+        <v>30425901658.5312</v>
       </c>
       <c r="H38">
-        <v>0.19375737477715554</v>
+        <v>0.19418011357311984</v>
       </c>
       <c r="I38">
-        <v>1.2569771717442003E-4</v>
+        <v>1.2589141089977229E-4</v>
       </c>
       <c r="J38">
-        <v>-6.4148186968406018E-4</v>
+        <v>-6.4148714030550077E-4</v>
       </c>
       <c r="K38">
-        <v>-4.2956451197658473E-8</v>
+        <v>-1.6490771242896903E-7</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1722,28 +1722,28 @@
         <v>-4.7189999999999998E-7</v>
       </c>
       <c r="D39">
-        <v>26193.554770272691</v>
+        <v>21094.001103391485</v>
       </c>
       <c r="E39">
-        <v>-19580128.336271994</v>
+        <v>-19568111.762129415</v>
       </c>
       <c r="F39">
-        <v>-8919.5780750893682</v>
+        <v>-6564.6713458402301</v>
       </c>
       <c r="G39">
-        <v>30711928433.971867</v>
+        <v>30691510639.527386</v>
       </c>
       <c r="H39">
-        <v>0.19748838232891078</v>
+        <v>0.19773811263762966</v>
       </c>
       <c r="I39">
-        <v>1.2676861551141308E-4</v>
+        <v>1.2692300917513461E-4</v>
       </c>
       <c r="J39">
-        <v>-6.3773341150682962E-4</v>
+        <v>-6.378045571068542E-4</v>
       </c>
       <c r="K39">
-        <v>-6.9559558967240837E-7</v>
+        <v>-5.1546266723143044E-7</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1757,28 +1757,28 @@
         <v>-4.6591999999999998E-7</v>
       </c>
       <c r="D40">
-        <v>11279.284283846617</v>
+        <v>11791.30506222602</v>
       </c>
       <c r="E40">
-        <v>-19624134.883557599</v>
+        <v>-19634334.395025752</v>
       </c>
       <c r="F40">
-        <v>-8699.3765337892437</v>
+        <v>-8674.6272997726992</v>
       </c>
       <c r="G40">
-        <v>30929153458.664318</v>
+        <v>30945388437.72718</v>
       </c>
       <c r="H40">
-        <v>0.20092659277927258</v>
+        <v>0.20090185541236655</v>
       </c>
       <c r="I40">
-        <v>1.2786088976296945E-4</v>
+        <v>1.278556690591474E-4</v>
       </c>
       <c r="J40">
-        <v>-6.3458799846335327E-4</v>
+        <v>-6.3457263301451941E-4</v>
       </c>
       <c r="K40">
-        <v>-6.755986820296267E-7</v>
+        <v>-6.7329115819084445E-7</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1792,28 +1792,28 @@
         <v>-1.2176E-6</v>
       </c>
       <c r="D41">
-        <v>4762.9841436487623</v>
+        <v>1405.2473540860228</v>
       </c>
       <c r="E41">
-        <v>-19703353.286422022</v>
+        <v>-19670911.881545197</v>
       </c>
       <c r="F41">
-        <v>-15807.972101692856</v>
+        <v>-11475.517510469954</v>
       </c>
       <c r="G41">
-        <v>29729627480.963093</v>
+        <v>29679767373.195541</v>
       </c>
       <c r="H41">
-        <v>0.1781207188498394</v>
+        <v>0.17828590116613399</v>
       </c>
       <c r="I41">
-        <v>1.1822393770036634E-4</v>
+        <v>1.182061701561943E-4</v>
       </c>
       <c r="J41">
-        <v>-6.6290214820008777E-4</v>
+        <v>-6.6279329235508443E-4</v>
       </c>
       <c r="K41">
-        <v>-1.2530897630496371E-6</v>
+        <v>-9.1116597490691932E-7</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1827,28 +1827,28 @@
         <v>-2.4233000000000002E-6</v>
       </c>
       <c r="D42">
-        <v>26072.33188107796</v>
+        <v>25598.840047513899</v>
       </c>
       <c r="E42">
-        <v>-19547434.395631455</v>
+        <v>-19550688.843992356</v>
       </c>
       <c r="F42">
-        <v>-27783.007745806655</v>
+        <v>-16824.377999285462</v>
       </c>
       <c r="G42">
-        <v>29727954116.037762</v>
+        <v>29732730128.634098</v>
       </c>
       <c r="H42">
-        <v>0.17838094330470736</v>
+        <v>0.17840584176252719</v>
       </c>
       <c r="I42">
-        <v>1.1816681347671064E-4</v>
+        <v>1.1864736710900904E-4</v>
       </c>
       <c r="J42">
-        <v>-6.5769548053586872E-4</v>
+        <v>-6.5811665368229041E-4</v>
       </c>
       <c r="K42">
-        <v>-2.2025473947324915E-6</v>
+        <v>-1.3301801760020512E-6</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1862,28 +1862,28 @@
         <v>-1.9112E-6</v>
       </c>
       <c r="D43">
-        <v>47091.722271656618</v>
+        <v>41865.935401190858</v>
       </c>
       <c r="E43">
-        <v>-19431626.161513627</v>
+        <v>-19461170.127051845</v>
       </c>
       <c r="F43">
-        <v>-22615.285974861396</v>
+        <v>-15782.250481908384</v>
       </c>
       <c r="G43">
-        <v>29730339903.640064</v>
+        <v>29774080456.898529</v>
       </c>
       <c r="H43">
-        <v>0.17949346209465467</v>
+        <v>0.17975755435768587</v>
       </c>
       <c r="I43">
-        <v>1.1889398287143974E-4</v>
+        <v>1.1928292533620606E-4</v>
       </c>
       <c r="J43">
-        <v>-6.5383014998345273E-4</v>
+        <v>-6.5400184395333623E-4</v>
       </c>
       <c r="K43">
-        <v>-1.7943046712265648E-6</v>
+        <v>-1.2466521529014486E-6</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1897,28 +1897,28 @@
         <v>-6.7843000000000002E-7</v>
       </c>
       <c r="D44">
-        <v>60042.777836396825</v>
+        <v>54941.777796313865</v>
       </c>
       <c r="E44">
-        <v>-19370729.325672884</v>
+        <v>-19409874.826539021</v>
       </c>
       <c r="F44">
-        <v>-9601.1013259297688</v>
+        <v>-7618.1129284964163</v>
       </c>
       <c r="G44">
-        <v>29790383254.213459</v>
+        <v>29849147926.198807</v>
       </c>
       <c r="H44">
-        <v>0.18141837561328142</v>
+        <v>0.18167865356535129</v>
       </c>
       <c r="I44">
-        <v>1.1996661631334535E-4</v>
+        <v>1.2032310358956711E-4</v>
       </c>
       <c r="J44">
-        <v>-6.5052596603180956E-4</v>
+        <v>-6.5056915537359803E-4</v>
       </c>
       <c r="K44">
-        <v>-7.6142906875399825E-7</v>
+        <v>-6.0075965966678425E-7</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1932,28 +1932,28 @@
         <v>5.8530000000000003E-7</v>
       </c>
       <c r="D45">
-        <v>66856.814896214288</v>
+        <v>61140.720555015578</v>
       </c>
       <c r="E45">
-        <v>-19361569.31053241</v>
+        <v>-19396605.217961289</v>
       </c>
       <c r="F45">
-        <v>5721.9693313299504</v>
+        <v>2395.1276734832763</v>
       </c>
       <c r="G45">
-        <v>29923327384.438328</v>
+        <v>29975843010.717293</v>
       </c>
       <c r="H45">
-        <v>0.1838308289812581</v>
+        <v>0.18412164841623779</v>
       </c>
       <c r="I45">
-        <v>1.2116650721073416E-4</v>
+        <v>1.2148971108073179E-4</v>
       </c>
       <c r="J45">
-        <v>-6.4739114665741406E-4</v>
+        <v>-6.4737518131821907E-4</v>
       </c>
       <c r="K45">
-        <v>4.5270402207584111E-7</v>
+        <v>1.8902582066642781E-7</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1967,28 +1967,28 @@
         <v>1.4465E-6</v>
       </c>
       <c r="D46">
-        <v>64330.072103064042</v>
+        <v>59843.548951332181</v>
       </c>
       <c r="E46">
-        <v>-19398932.411509626</v>
+        <v>-19414877.041213058</v>
       </c>
       <c r="F46">
-        <v>17089.756745486684</v>
+        <v>10323.110067991154</v>
       </c>
       <c r="G46">
-        <v>30129520955.562828</v>
+        <v>30152972929.94875</v>
       </c>
       <c r="H46">
-        <v>0.1867589089726174</v>
+        <v>0.18698502954057486</v>
       </c>
       <c r="I46">
-        <v>1.2236959067886839E-4</v>
+        <v>1.2266147783957315E-4</v>
       </c>
       <c r="J46">
-        <v>-6.4422457969483715E-4</v>
+        <v>-6.4419834117692104E-4</v>
       </c>
       <c r="K46">
-        <v>1.3462191043485394E-6</v>
+        <v>8.1063269521134704E-7</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2002,28 +2002,28 @@
         <v>1.7081E-6</v>
       </c>
       <c r="D47">
-        <v>54825.809241429437</v>
+        <v>51662.031530380416</v>
       </c>
       <c r="E47">
-        <v>-19462532.660233412</v>
+        <v>-19454399.150431089</v>
       </c>
       <c r="F47">
-        <v>20915.379091400031</v>
+        <v>14021.301559387914</v>
       </c>
       <c r="G47">
-        <v>30380435570.0303</v>
+        <v>30366798033.816719</v>
       </c>
       <c r="H47">
-        <v>0.19000978827372478</v>
+        <v>0.19016601223176466</v>
       </c>
       <c r="I47">
-        <v>1.2352436501939849E-4</v>
+        <v>1.2377845133893479E-4</v>
       </c>
       <c r="J47">
-        <v>-6.4097549911556789E-4</v>
+        <v>-6.4096835588762862E-4</v>
       </c>
       <c r="K47">
-        <v>1.638521370472823E-6</v>
+        <v>1.0961748587994217E-6</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2037,28 +2037,28 @@
         <v>1.4191999999999999E-6</v>
       </c>
       <c r="D48">
-        <v>41048.503565996885</v>
+        <v>38016.357854578462</v>
       </c>
       <c r="E48">
-        <v>-19526643.519797105</v>
+        <v>-19505493.508383993</v>
       </c>
       <c r="F48">
-        <v>17333.988376171867</v>
+        <v>13244.41692962725</v>
       </c>
       <c r="G48">
-        <v>30632387065.486702</v>
+        <v>30598298939.018623</v>
       </c>
       <c r="H48">
-        <v>0.19337963299509794</v>
+        <v>0.19352738599806202</v>
       </c>
       <c r="I48">
-        <v>1.246117226262433E-4</v>
+        <v>1.2482153751894418E-4</v>
       </c>
       <c r="J48">
-        <v>-6.3774471318422195E-4</v>
+        <v>-6.3774899978687161E-4</v>
       </c>
       <c r="K48">
-        <v>1.35066287644558E-6</v>
+        <v>1.0303647771968728E-6</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2072,28 +2072,28 @@
         <v>8.1691000000000003E-7</v>
       </c>
       <c r="D49">
-        <v>21592.677397949621</v>
+        <v>22194.26915179193</v>
       </c>
       <c r="E49">
-        <v>-19574198.09487465</v>
+        <v>-19564286.341844477</v>
       </c>
       <c r="F49">
-        <v>11125.804634555534</v>
+        <v>8840.5323832794711</v>
       </c>
       <c r="G49">
-        <v>30846294527.236816</v>
+        <v>30830859579.733665</v>
       </c>
       <c r="H49">
-        <v>0.19695155873371631</v>
+        <v>0.19692157863682636</v>
       </c>
       <c r="I49">
-        <v>1.2567813309554535E-4</v>
+        <v>1.2586269956404815E-4</v>
       </c>
       <c r="J49">
-        <v>-6.3472950662491964E-4</v>
+        <v>-6.3479135040828117E-4</v>
       </c>
       <c r="K49">
-        <v>8.6346572490702579E-7</v>
+        <v>6.8448366382661352E-7</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2107,28 +2107,28 @@
         <v>2.0029E-7</v>
       </c>
       <c r="D50">
-        <v>4654.6084058438428</v>
+        <v>3298.2713280953467</v>
       </c>
       <c r="E50">
-        <v>-19622980.833812445</v>
+        <v>-19633308.164641801</v>
       </c>
       <c r="F50">
-        <v>3620.468969299644</v>
+        <v>2863.7415483506561</v>
       </c>
       <c r="G50">
-        <v>31031347701.16275</v>
+        <v>31047248411.34193</v>
       </c>
       <c r="H50">
-        <v>0.20039218893319877</v>
+        <v>0.20045862930270125</v>
       </c>
       <c r="I50">
-        <v>1.2686920456555625E-4</v>
+        <v>1.268687270918677E-4</v>
       </c>
       <c r="J50">
-        <v>-6.3241189412075426E-4</v>
+        <v>-6.3240025899351303E-4</v>
       </c>
       <c r="K50">
-        <v>2.8011052730851464E-7</v>
+        <v>2.2145885022616281E-7</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2142,28 +2142,28 @@
         <v>-1.8450999999999999E-6</v>
       </c>
       <c r="D51">
-        <v>6801.9679042501375</v>
+        <v>9969.003900251817</v>
       </c>
       <c r="E51">
-        <v>-19665430.156397562</v>
+        <v>-19642072.719928533</v>
       </c>
       <c r="F51">
-        <v>-23817.704360538733</v>
+        <v>-19594.067917313569</v>
       </c>
       <c r="G51">
-        <v>29861746693.091282</v>
+        <v>29827121828.975693</v>
       </c>
       <c r="H51">
-        <v>0.17882061212520403</v>
+        <v>0.17866458460181903</v>
       </c>
       <c r="I51">
-        <v>1.180141721482433E-4</v>
+        <v>1.1799894072462148E-4</v>
       </c>
       <c r="J51">
-        <v>-6.5869522768018346E-4</v>
+        <v>-6.5860376115113627E-4</v>
       </c>
       <c r="K51">
-        <v>-1.8807662234029791E-6</v>
+        <v>-1.548623425409474E-6</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2177,28 +2177,28 @@
         <v>-3.7050999999999999E-6</v>
       </c>
       <c r="D52">
-        <v>17045.887952831108</v>
+        <v>18632.686334722759</v>
       </c>
       <c r="E52">
-        <v>-19547243.487801734</v>
+        <v>-19544163.661068216</v>
       </c>
       <c r="F52">
-        <v>-47222.749162333188</v>
+        <v>-31507.715250490284</v>
       </c>
       <c r="G52">
-        <v>29913565285.046421</v>
+        <v>29909173152.523232</v>
       </c>
       <c r="H52">
-        <v>0.17979763756889544</v>
+        <v>0.17972206523337317</v>
       </c>
       <c r="I52">
-        <v>1.1806288298416565E-4</v>
+        <v>1.1844489220081626E-4</v>
       </c>
       <c r="J52">
-        <v>-6.5356194832491858E-4</v>
+        <v>-6.539601787107428E-4</v>
       </c>
       <c r="K52">
-        <v>-3.7249751479850185E-6</v>
+        <v>-2.4854032326503352E-6</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2212,28 +2212,28 @@
         <v>-3.1369E-6</v>
       </c>
       <c r="D53">
-        <v>31810.553307261318</v>
+        <v>31367.143915022145</v>
       </c>
       <c r="E53">
-        <v>-19444286.705933001</v>
+        <v>-19468940.190132491</v>
       </c>
       <c r="F53">
-        <v>-39953.070169072489</v>
+        <v>-30604.533808798555</v>
       </c>
       <c r="G53">
-        <v>29940199349.290527</v>
+        <v>29977965079.190166</v>
       </c>
       <c r="H53">
-        <v>0.18119912639815947</v>
+        <v>0.18122484514658524</v>
       </c>
       <c r="I53">
-        <v>1.1873031507171909E-4</v>
+        <v>1.1905743409760353E-4</v>
       </c>
       <c r="J53">
-        <v>-6.4958238058160822E-4</v>
+        <v>-6.4980851692704336E-4</v>
       </c>
       <c r="K53">
-        <v>-3.152217883556005E-6</v>
+        <v>-2.4114704595868475E-6</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2247,28 +2247,28 @@
         <v>-1.4591999999999999E-6</v>
       </c>
       <c r="D54">
-        <v>46030.933141239453</v>
+        <v>42081.588094967847</v>
       </c>
       <c r="E54">
-        <v>-19391244.773958568</v>
+        <v>-19423778.050242111</v>
       </c>
       <c r="F54">
-        <v>-20434.957183548137</v>
+        <v>-17515.865198239437</v>
       </c>
       <c r="G54">
-        <v>30017905194.086548</v>
+        <v>30067129680.332321</v>
       </c>
       <c r="H54">
-        <v>0.18296960008033947</v>
+        <v>0.18317024039657603</v>
       </c>
       <c r="I54">
-        <v>1.1971974651671846E-4</v>
+        <v>1.200123254282278E-4</v>
       </c>
       <c r="J54">
-        <v>-6.4620925179187621E-4</v>
+        <v>-6.4631848207615016E-4</v>
       </c>
       <c r="K54">
-        <v>-1.6104855970486623E-6</v>
+        <v>-1.37864019545766E-6</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2282,28 +2282,28 @@
         <v>3.9359999999999998E-7</v>
       </c>
       <c r="D55">
-        <v>52040.345561175607</v>
+        <v>47745.935729349054</v>
       </c>
       <c r="E55">
-        <v>-19380515.652785897</v>
+        <v>-19410388.59556647</v>
       </c>
       <c r="F55">
-        <v>2830.6558973881934</v>
+        <v>-576.16067232525188</v>
       </c>
       <c r="G55">
-        <v>30148262521.020409</v>
+        <v>30193487979.722172</v>
       </c>
       <c r="H55">
-        <v>0.18527759110319236</v>
+        <v>0.18549524186793281</v>
       </c>
       <c r="I55">
-        <v>1.2082162360744852E-4</v>
+        <v>1.2107895791520527E-4</v>
       </c>
       <c r="J55">
-        <v>-6.4310903667254738E-4</v>
+        <v>-6.4314583006089331E-4</v>
       </c>
       <c r="K55">
-        <v>2.2255691211193855E-7</v>
+        <v>-4.6719166435747712E-8</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2317,28 +2317,28 @@
         <v>1.8341999999999999E-6</v>
       </c>
       <c r="D56">
-        <v>51003.65371711133</v>
+        <v>47173.927144122979</v>
       </c>
       <c r="E56">
-        <v>-19411480.209311519</v>
+        <v>-19424749.041576568</v>
       </c>
       <c r="F56">
-        <v>22321.45679700531</v>
+        <v>14406.83675591539</v>
       </c>
       <c r="G56">
-        <v>30340668339.405308</v>
+        <v>30360259755.271656</v>
       </c>
       <c r="H56">
-        <v>0.18792128480673503</v>
+        <v>0.18811394564706277</v>
       </c>
       <c r="I56">
-        <v>1.2190532140370097E-4</v>
+        <v>1.2214114811391418E-4</v>
       </c>
       <c r="J56">
-        <v>-6.400789498975355E-4</v>
+        <v>-6.4009028965838371E-4</v>
       </c>
       <c r="K56">
-        <v>1.7478343577880147E-6</v>
+        <v>1.1250896366372376E-6</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2352,28 +2352,28 @@
         <v>2.5646E-6</v>
       </c>
       <c r="D57">
-        <v>43582.836809405591</v>
+        <v>40646.57446290474</v>
       </c>
       <c r="E57">
-        <v>-19464609.265058983</v>
+        <v>-19458842.915176693</v>
       </c>
       <c r="F57">
-        <v>32406.675907642999</v>
+        <v>24253.179957880915</v>
       </c>
       <c r="G57">
-        <v>30567340094.933075</v>
+        <v>30557374010.877514</v>
       </c>
       <c r="H57">
-        <v>0.19082674264078844</v>
+        <v>0.19097266928990381</v>
       </c>
       <c r="I57">
-        <v>1.2293726315407811E-4</v>
+        <v>1.2316022121947249E-4</v>
       </c>
       <c r="J57">
-        <v>-6.370551158510528E-4</v>
+        <v>-6.370822374820172E-4</v>
       </c>
       <c r="K57">
-        <v>2.5249727488934302E-6</v>
+        <v>1.8880373530926146E-6</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2387,28 +2387,28 @@
         <v>2.5523000000000001E-6</v>
       </c>
       <c r="D58">
-        <v>30310.977741361596</v>
+        <v>29677.179027628543</v>
       </c>
       <c r="E58">
-        <v>-19522219.565580044</v>
+        <v>-19504228.403556939</v>
       </c>
       <c r="F58">
-        <v>32999.587453838845</v>
+        <v>27550.969980245332</v>
       </c>
       <c r="G58">
-        <v>30796076418.070671</v>
+        <v>30767480050.79295</v>
       </c>
       <c r="H58">
-        <v>0.1939928143065037</v>
+        <v>0.19402353528219049</v>
       </c>
       <c r="I58">
-        <v>1.2396015907266717E-4</v>
+        <v>1.2415220990554519E-4</v>
       </c>
       <c r="J58">
-        <v>-6.3413620271565588E-4</v>
+        <v>-6.3417726390941004E-4</v>
       </c>
       <c r="K58">
-        <v>2.5589390727550482E-6</v>
+        <v>2.1366781600287862E-6</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2422,28 +2422,28 @@
         <v>1.9263000000000001E-6</v>
       </c>
       <c r="D59">
-        <v>17056.446690602228</v>
+        <v>17082.532256465965</v>
       </c>
       <c r="E59">
-        <v>-19567947.870363038</v>
+        <v>-19556512.638533738</v>
       </c>
       <c r="F59">
-        <v>28092.596099565628</v>
+        <v>22870.97007978852</v>
       </c>
       <c r="G59">
-        <v>30992779874.723587</v>
+        <v>30974653673.504551</v>
       </c>
       <c r="H59">
-        <v>0.19714129881838088</v>
+        <v>0.19714019220840309</v>
       </c>
       <c r="I59">
-        <v>1.2502302219805024E-4</v>
+        <v>1.2520057687538577E-4</v>
       </c>
       <c r="J59">
-        <v>-6.3149961505167581E-4</v>
+        <v>-6.315756591015716E-4</v>
       </c>
       <c r="K59">
-        <v>2.1703017823620271E-6</v>
+        <v>1.767778235381154E-6</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2457,28 +2457,28 @@
         <v>7.6183000000000004E-7</v>
       </c>
       <c r="D60">
-        <v>6568.048539057374</v>
+        <v>8219.4804783086292</v>
       </c>
       <c r="E60">
-        <v>-19605022.312809385</v>
+        <v>-19616664.571364935</v>
       </c>
       <c r="F60">
-        <v>12777.508719941277</v>
+        <v>12336.724938542309</v>
       </c>
       <c r="G60">
-        <v>31147380392.545612</v>
+        <v>31166398927.361698</v>
       </c>
       <c r="H60">
-        <v>0.20024382791698866</v>
+        <v>0.20016323601731326</v>
       </c>
       <c r="I60">
-        <v>1.2625694378787095E-4</v>
+        <v>1.2625546640485192E-4</v>
       </c>
       <c r="J60">
-        <v>-6.2949090701201142E-4</v>
+        <v>-6.2948015830511616E-4</v>
       </c>
       <c r="K60">
-        <v>9.847824246527262E-7</v>
+        <v>9.5015109426123054E-7</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2492,28 +2492,28 @@
         <v>-2.2411E-6</v>
       </c>
       <c r="D61">
-        <v>7633.0477393367328</v>
+        <v>5198.2643764461391</v>
       </c>
       <c r="E61">
-        <v>-19616323.009216748</v>
+        <v>-19601470.412494369</v>
       </c>
       <c r="F61">
-        <v>-30101.568924252344</v>
+        <v>-26341.011608245673</v>
       </c>
       <c r="G61">
-        <v>29947498748.003807</v>
+        <v>29924135502.764992</v>
       </c>
       <c r="H61">
-        <v>0.18067271781520283</v>
+        <v>0.18079311963882147</v>
       </c>
       <c r="I61">
-        <v>1.1861092879982005E-4</v>
+        <v>1.185967771431221E-4</v>
       </c>
       <c r="J61">
-        <v>-6.5515442424753795E-4</v>
+        <v>-6.5507902158569876E-4</v>
       </c>
       <c r="K61">
-        <v>-2.3737875317650196E-6</v>
+        <v>-2.0788236422208083E-6</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2527,28 +2527,28 @@
         <v>-4.5117000000000004E-6</v>
       </c>
       <c r="D62">
-        <v>10550.363233648241</v>
+        <v>9423.120409168303</v>
       </c>
       <c r="E62">
-        <v>-19541015.725587312</v>
+        <v>-19533845.301595893</v>
       </c>
       <c r="F62">
-        <v>-57849.903857647631</v>
+        <v>-40597.781895594206</v>
       </c>
       <c r="G62">
-        <v>30047109787.924103</v>
+        <v>30035612864.304424</v>
       </c>
       <c r="H62">
-        <v>0.18211654412257203</v>
+        <v>0.1821764371440675</v>
       </c>
       <c r="I62">
-        <v>1.1878863709229904E-4</v>
+        <v>1.190738260262927E-4</v>
       </c>
       <c r="J62">
-        <v>-6.5041363958130141E-4</v>
+        <v>-6.5077075947231702E-4</v>
       </c>
       <c r="K62">
-        <v>-4.5518888410779872E-6</v>
+        <v>-3.1970571833135208E-6</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2562,28 +2562,28 @@
         <v>-3.9497999999999999E-6</v>
       </c>
       <c r="D63">
-        <v>18853.023670815397</v>
+        <v>15026.025760262992</v>
       </c>
       <c r="E63">
-        <v>-19462368.984319557</v>
+        <v>-19478460.755290546</v>
       </c>
       <c r="F63">
-        <v>-51944.115513212142</v>
+        <v>-40239.338302704185</v>
       </c>
       <c r="G63">
-        <v>30110044589.833221</v>
+        <v>30133751010.342495</v>
       </c>
       <c r="H63">
-        <v>0.18369147654356566</v>
+        <v>0.18388483888808527</v>
       </c>
       <c r="I63">
-        <v>1.1935788424802496E-4</v>
+        <v>1.1960017847252861E-4</v>
       </c>
       <c r="J63">
-        <v>-6.4645007285464009E-4</v>
+        <v>-6.4672761788692277E-4</v>
       </c>
       <c r="K63">
-        <v>-4.0838523341463987E-6</v>
+        <v>-3.1641212688504384E-6</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2597,28 +2597,28 @@
         <v>-2.0140000000000001E-6</v>
       </c>
       <c r="D64">
-        <v>24870.985406497028</v>
+        <v>20289.956282750714</v>
       </c>
       <c r="E64">
-        <v>-19415407.332451712</v>
+        <v>-19442467.152467083</v>
       </c>
       <c r="F64">
-        <v>-29042.272471369019</v>
+        <v>-24490.096964022829</v>
       </c>
       <c r="G64">
-        <v>30200354131.06834</v>
+        <v>30241096705.958477</v>
       </c>
       <c r="H64">
-        <v>0.18564092906496868</v>
+        <v>0.18587076644780295</v>
       </c>
       <c r="I64">
-        <v>1.2016939289825017E-4</v>
+        <v>1.2036091451154492E-4</v>
       </c>
       <c r="J64">
-        <v>-6.4299058983243937E-4</v>
+        <v>-6.4316176046052133E-4</v>
       </c>
       <c r="K64">
-        <v>-2.2802039966011989E-6</v>
+        <v>-1.9230486354187553E-6</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2632,28 +2632,28 @@
         <v>2.4084999999999999E-7</v>
       </c>
       <c r="D65">
-        <v>29906.129008769989</v>
+        <v>23497.45573695553</v>
       </c>
       <c r="E65">
-        <v>-19407987.607301179</v>
+        <v>-19430128.664528668</v>
       </c>
       <c r="F65">
-        <v>-393.7344257567064</v>
+        <v>-3003.073643391795</v>
       </c>
       <c r="G65">
-        <v>30342759157.448322</v>
+        <v>30375497216.847595</v>
       </c>
       <c r="H65">
-        <v>0.18771062253243481</v>
+        <v>0.18803048469982495</v>
       </c>
       <c r="I65">
-        <v>1.2105574269600421E-4</v>
+        <v>1.2122046219740719E-4</v>
       </c>
       <c r="J65">
-        <v>-6.3977316601152197E-4</v>
+        <v>-6.3987099408635909E-4</v>
       </c>
       <c r="K65">
-        <v>-3.0822735995255854E-8</v>
+        <v>-2.377869925846902E-7</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2667,28 +2667,28 @@
         <v>2.1055E-6</v>
       </c>
       <c r="D66">
-        <v>31110.311883753631</v>
+        <v>23329.428135198115</v>
       </c>
       <c r="E66">
-        <v>-19429786.012396716</v>
+        <v>-19440421.672357552</v>
       </c>
       <c r="F66">
-        <v>25349.281221541514</v>
+        <v>17149.621791459067</v>
       </c>
       <c r="G66">
-        <v>30527581935.587009</v>
+        <v>30541946500.046143</v>
       </c>
       <c r="H66">
-        <v>0.18995668734703702</v>
+        <v>0.19034419038145836</v>
       </c>
       <c r="I66">
-        <v>1.2193210197233736E-4</v>
+        <v>1.2209033442416283E-4</v>
       </c>
       <c r="J66">
-        <v>-6.3664404369960081E-4</v>
+        <v>-6.3671676743794572E-4</v>
       </c>
       <c r="K66">
-        <v>1.9762049726969062E-6</v>
+        <v>1.3338450301558036E-6</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2702,28 +2702,28 @@
         <v>3.1677000000000002E-6</v>
       </c>
       <c r="D67">
-        <v>26668.455635876395</v>
+        <v>19670.846644563491</v>
       </c>
       <c r="E67">
-        <v>-19472329.564865749</v>
+        <v>-19467795.320296455</v>
       </c>
       <c r="F67">
-        <v>40976.00296890091</v>
+        <v>31366.451484607365</v>
       </c>
       <c r="G67">
-        <v>30742402015.808266</v>
+        <v>30733063199.208572</v>
       </c>
       <c r="H67">
-        <v>0.19248803044390622</v>
+        <v>0.19283558462621886</v>
       </c>
       <c r="I67">
-        <v>1.2280666888226231E-4</v>
+        <v>1.2296003648587864E-4</v>
       </c>
       <c r="J67">
-        <v>-6.3357853566775395E-4</v>
+        <v>-6.3366640908861722E-4</v>
       </c>
       <c r="K67">
-        <v>3.1789984649146456E-6</v>
+        <v>2.4329973475837421E-6</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2737,28 +2737,28 @@
         <v>3.3098000000000001E-6</v>
       </c>
       <c r="D68">
-        <v>19596.803385453299</v>
+        <v>13839.912472524513</v>
       </c>
       <c r="E68">
-        <v>-19518982.952234607</v>
+        <v>-19504808.766913366</v>
       </c>
       <c r="F68">
-        <v>44257.077610348948</v>
+        <v>37056.730742137835</v>
       </c>
       <c r="G68">
-        <v>30956166348.940155</v>
+        <v>30931859009.022072</v>
       </c>
       <c r="H68">
-        <v>0.19520959023328499</v>
+        <v>0.19549424540479099</v>
       </c>
       <c r="I68">
-        <v>1.2373458952974955E-4</v>
+        <v>1.2388070487286812E-4</v>
       </c>
       <c r="J68">
-        <v>-6.3067794072723163E-4</v>
+        <v>-6.3079192292776135E-4</v>
       </c>
       <c r="K68">
-        <v>3.4176582248460728E-6</v>
+        <v>2.8643479159819523E-6</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2772,28 +2772,28 @@
         <v>2.6205000000000002E-6</v>
       </c>
       <c r="D69">
-        <v>10322.077247548383</v>
+        <v>8009.1151817237378</v>
       </c>
       <c r="E69">
-        <v>-19561288.641388245</v>
+        <v>-19545476.052016728</v>
       </c>
       <c r="F69">
-        <v>39228.355956927575</v>
+        <v>31741.269024009751</v>
       </c>
       <c r="G69">
-        <v>31147874618.31601</v>
+        <v>31121918720.830215</v>
       </c>
       <c r="H69">
-        <v>0.19814518004963538</v>
+        <v>0.19825978659244939</v>
       </c>
       <c r="I69">
-        <v>1.2477673382904375E-4</v>
+        <v>1.2492456714135561E-4</v>
       </c>
       <c r="J69">
-        <v>-6.2810031834829752E-4</v>
+        <v>-6.2822411126956196E-4</v>
       </c>
       <c r="K69">
-        <v>3.0180580861945226E-6</v>
+        <v>2.4459909001948514E-6</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2807,28 +2807,28 @@
         <v>1.1069999999999999E-6</v>
       </c>
       <c r="D70">
-        <v>3339.0279052886181</v>
+        <v>1180.7974801282398</v>
       </c>
       <c r="E70">
-        <v>-19574510.170238052</v>
+        <v>-19588216.97781229</v>
       </c>
       <c r="F70">
-        <v>19520.877434410988</v>
+        <v>18562.12699563587</v>
       </c>
       <c r="G70">
-        <v>31270774757.950253</v>
+        <v>31291974219.482952</v>
       </c>
       <c r="H70">
-        <v>0.20110108560874393</v>
+        <v>0.20120701438985417</v>
       </c>
       <c r="I70">
-        <v>1.2599157024467954E-4</v>
+        <v>1.2598827566458992E-4</v>
       </c>
       <c r="J70">
-        <v>-6.2600735364648648E-4</v>
+        <v>-6.2599667666936049E-4</v>
       </c>
       <c r="K70">
-        <v>1.4996211969474718E-6</v>
+        <v>1.4251015109443925E-6</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2842,28 +2842,28 @@
         <v>-2.3705E-6</v>
       </c>
       <c r="D71">
-        <v>-3000.9439296289347</v>
+        <v>-2780.4943741993047</v>
       </c>
       <c r="E71">
-        <v>-19560673.556180269</v>
+        <v>-19555862.844660237</v>
       </c>
       <c r="F71">
-        <v>-32907.205658703089</v>
+        <v>-27251.531490675177</v>
       </c>
       <c r="G71">
-        <v>29990543770.253361</v>
+        <v>29983198425.117023</v>
       </c>
       <c r="H71">
-        <v>0.18393826933856439</v>
+        <v>0.18392827288936234</v>
       </c>
       <c r="I71">
-        <v>1.1989253080089751E-4</v>
+        <v>1.1987616685895112E-4</v>
       </c>
       <c r="J71">
-        <v>-6.5227052288303585E-4</v>
+        <v>-6.5221767795476011E-4</v>
       </c>
       <c r="K71">
-        <v>-2.5984409201852687E-6</v>
+        <v>-2.1521660215776187E-6</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2877,28 +2877,28 @@
         <v>-4.6960999999999998E-6</v>
       </c>
       <c r="D72">
-        <v>3896.3421981781721</v>
+        <v>-3754.947904313512</v>
       </c>
       <c r="E72">
-        <v>-19534785.349273104</v>
+        <v>-19521622.680323239</v>
       </c>
       <c r="F72">
-        <v>-61620.675625047297</v>
+        <v>-41516.419807289567</v>
       </c>
       <c r="G72">
-        <v>30139966637.190613</v>
+        <v>30117277513.712673</v>
       </c>
       <c r="H72">
-        <v>0.18514684212937085</v>
+        <v>0.18553042361776326</v>
       </c>
       <c r="I72">
-        <v>1.2015929723385157E-4</v>
+        <v>1.2026557265881051E-4</v>
       </c>
       <c r="J72">
-        <v>-6.4817824701112131E-4</v>
+        <v>-6.484690796341769E-4</v>
       </c>
       <c r="K72">
-        <v>-4.846332964739521E-6</v>
+        <v>-3.2689261367853373E-6</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2912,28 +2912,28 @@
         <v>-4.1685E-6</v>
       </c>
       <c r="D73">
-        <v>546.074103503488</v>
+        <v>-7801.0773706102791</v>
       </c>
       <c r="E73">
-        <v>-19478988.693605278</v>
+        <v>-19487886.708147347</v>
       </c>
       <c r="F73">
-        <v>-54998.261248712784</v>
+        <v>-41847.872259328557</v>
       </c>
       <c r="G73">
-        <v>30229217911.341671</v>
+        <v>30240478817.343872</v>
       </c>
       <c r="H73">
-        <v>0.18698939660815503</v>
+        <v>0.18740596318894914</v>
       </c>
       <c r="I73">
-        <v>1.2053162655035869E-4</v>
+        <v>1.2061120457973201E-4</v>
       </c>
       <c r="J73">
-        <v>-6.4434786291176415E-4</v>
+        <v>-6.446459458343014E-4</v>
       </c>
       <c r="K73">
-        <v>-4.319101301634206E-6</v>
+        <v>-3.2888040027746723E-6</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2947,28 +2947,28 @@
         <v>-2.1983000000000002E-6</v>
       </c>
       <c r="D74">
-        <v>-1242.9950752216391</v>
+        <v>-9818.4817827858024</v>
       </c>
       <c r="E74">
-        <v>-19444307.578595497</v>
+        <v>-19462791.227210332</v>
       </c>
       <c r="F74">
-        <v>-31383.489691726416</v>
+        <v>-26597.561082893662</v>
       </c>
       <c r="G74">
-        <v>30341559271.789429</v>
+        <v>30367840741.02639</v>
       </c>
       <c r="H74">
-        <v>0.18893823809592614</v>
+        <v>0.18936373433832177</v>
       </c>
       <c r="I74">
-        <v>1.2106026443062316E-4</v>
+        <v>1.2110168452761681E-4</v>
       </c>
       <c r="J74">
-        <v>-6.408090072709898E-4</v>
+        <v>-6.4102261526359223E-4</v>
       </c>
       <c r="K74">
-        <v>-2.459500798568208E-6</v>
+        <v>-2.0866043751981925E-6</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2982,28 +2982,28 @@
         <v>1.9805999999999999E-7</v>
       </c>
       <c r="D75">
-        <v>-4334.3751577581279</v>
+        <v>-9803.7427134566224</v>
       </c>
       <c r="E75">
-        <v>-19438090.816047531</v>
+        <v>-19452947.739654705</v>
       </c>
       <c r="F75">
-        <v>-133.24303680589188</v>
+        <v>-4216.8668046122011</v>
       </c>
       <c r="G75">
-        <v>30494128228.74567</v>
+        <v>30515794584.183479</v>
       </c>
       <c r="H75">
-        <v>0.19106534187040544</v>
+        <v>0.19133601284501306</v>
       </c>
       <c r="I75">
-        <v>1.2166735367922875E-4</v>
+        <v>1.2171040613249246E-4</v>
       </c>
       <c r="J75">
-        <v>-6.3738531691029431E-4</v>
+        <v>-6.3754183409895065E-4</v>
       </c>
       <c r="K75">
-        <v>-1.0408536633933416E-8</v>
+        <v>-3.3308380513468025E-7</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3017,28 +3017,28 @@
         <v>2.2446999999999999E-6</v>
       </c>
       <c r="D76">
-        <v>-8991.0594336492941</v>
+        <v>-8932.5655278860231</v>
       </c>
       <c r="E76">
-        <v>-19453368.883470703</v>
+        <v>-19459446.892170683</v>
       </c>
       <c r="F76">
-        <v>28148.658034923854</v>
+        <v>17880.65376700359</v>
       </c>
       <c r="G76">
-        <v>30681769294.090961</v>
+        <v>30691328437.782673</v>
       </c>
       <c r="H76">
-        <v>0.1933375717975459</v>
+        <v>0.19333574309808024</v>
       </c>
       <c r="I76">
-        <v>1.2230690890805015E-4</v>
+        <v>1.2237279502144656E-4</v>
       </c>
       <c r="J76">
-        <v>-6.3396830567369984E-4</v>
+        <v>-6.341232188561899E-4</v>
       </c>
       <c r="K76">
-        <v>2.1896439771124012E-6</v>
+        <v>1.3871029963266423E-6</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3052,28 +3052,28 @@
         <v>3.4273000000000002E-6</v>
       </c>
       <c r="D77">
-        <v>-11611.600203420501</v>
+        <v>-7971.8322205922959</v>
       </c>
       <c r="E77">
-        <v>-19481650.374316145</v>
+        <v>-19478913.767279945</v>
       </c>
       <c r="F77">
-        <v>45169.41867793991</v>
+        <v>33655.775581890615</v>
       </c>
       <c r="G77">
-        <v>30890238075.404293</v>
+        <v>30886941201.601189</v>
       </c>
       <c r="H77">
-        <v>0.19559370451526514</v>
+        <v>0.1954163730935714</v>
       </c>
       <c r="I77">
-        <v>1.2300007587359138E-4</v>
+        <v>1.230908804375078E-4</v>
       </c>
       <c r="J77">
-        <v>-6.3061069529248351E-4</v>
+        <v>-6.3079312999187777E-4</v>
       </c>
       <c r="K77">
-        <v>3.4966710480582343E-6</v>
+        <v>2.6039384238090853E-6</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3087,28 +3087,28 @@
         <v>3.5425E-6</v>
       </c>
       <c r="D78">
-        <v>-11879.924630754162</v>
+        <v>-6648.9533646196087</v>
       </c>
       <c r="E78">
-        <v>-19515695.568533812</v>
+        <v>-19505724.546872132</v>
       </c>
       <c r="F78">
-        <v>47748.261931297253</v>
+        <v>39396.603489754132</v>
       </c>
       <c r="G78">
-        <v>31099953378.459255</v>
+        <v>31085643195.941242</v>
       </c>
       <c r="H78">
-        <v>0.19789425343612357</v>
+        <v>0.19763870146223403</v>
       </c>
       <c r="I78">
-        <v>1.238196023301464E-4</v>
+        <v>1.239342028326355E-4</v>
       </c>
       <c r="J78">
-        <v>-6.2744727009298503E-4</v>
+        <v>-6.2768993440574512E-4</v>
       </c>
       <c r="K78">
-        <v>3.6784276533068788E-6</v>
+        <v>3.0373099107593543E-6</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3122,28 +3122,28 @@
         <v>2.7062999999999998E-6</v>
       </c>
       <c r="D79">
-        <v>-6209.3273286907934</v>
+        <v>-4272.9843931051355</v>
       </c>
       <c r="E79">
-        <v>-19553289.164917685</v>
+        <v>-19532700.618643597</v>
       </c>
       <c r="F79">
-        <v>39974.45188703094</v>
+        <v>32930.339597275335</v>
       </c>
       <c r="G79">
-        <v>31298832925.839443</v>
+        <v>31266445732.859516</v>
       </c>
       <c r="H79">
-        <v>0.20016309948574509</v>
+        <v>0.20006954236333957</v>
       </c>
       <c r="I79">
-        <v>1.2487175337248406E-4</v>
+        <v>1.2497291856717422E-4</v>
       </c>
       <c r="J79">
-        <v>-6.2471817377680958E-4</v>
+        <v>-6.2492795302629813E-4</v>
       </c>
       <c r="K79">
-        <v>3.0658744658330905E-6</v>
+        <v>2.5311431592907972E-6</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3157,28 +3157,28 @@
         <v>1.1195E-6</v>
       </c>
       <c r="D80">
-        <v>-351.78670966345817</v>
+        <v>1726.6648298762739</v>
       </c>
       <c r="E80">
-        <v>-19539150.015059311</v>
+        <v>-19555027.704012331</v>
       </c>
       <c r="F80">
-        <v>20002.084729680195</v>
+        <v>18985.677103241407</v>
       </c>
       <c r="G80">
-        <v>31397175430.26099</v>
+        <v>31423361631.263355</v>
       </c>
       <c r="H80">
-        <v>0.20262960019032386</v>
+        <v>0.20252776188353608</v>
       </c>
       <c r="I80">
-        <v>1.2609954976188945E-4</v>
+        <v>1.2609347107397638E-4</v>
       </c>
       <c r="J80">
-        <v>-6.2233035271055644E-4</v>
+        <v>-6.2232524350408188E-4</v>
       </c>
       <c r="K80">
-        <v>1.5323520053305353E-6</v>
+        <v>1.453128242551345E-6</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3192,28 +3192,28 @@
         <v>-2.0524999999999998E-6</v>
       </c>
       <c r="D81">
-        <v>-455.4016686193645</v>
+        <v>3802.521834757179</v>
       </c>
       <c r="E81">
-        <v>-19512550.865275774</v>
+        <v>-19515218.558495235</v>
       </c>
       <c r="F81">
-        <v>-24698.013733591193</v>
+        <v>-22869.489104492277</v>
       </c>
       <c r="G81">
-        <v>30012707743.184231</v>
+        <v>30018026994.850082</v>
       </c>
       <c r="H81">
-        <v>0.18710546430659317</v>
+        <v>0.18689512758892507</v>
       </c>
       <c r="I81">
-        <v>1.2162397153411874E-4</v>
+        <v>1.2162753850453038E-4</v>
       </c>
       <c r="J81">
-        <v>-6.5016293024506081E-4</v>
+        <v>-6.5014268938670943E-4</v>
       </c>
       <c r="K81">
-        <v>-1.953824337842195E-6</v>
+        <v>-1.808491393630058E-6</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3227,28 +3227,28 @@
         <v>-3.9267E-6</v>
       </c>
       <c r="D82">
-        <v>-37661.033214484807</v>
+        <v>-20782.244201734051</v>
       </c>
       <c r="E82">
-        <v>-19525110.376377668</v>
+        <v>-19510249.348906938</v>
       </c>
       <c r="F82">
-        <v>-45968.901367059807</v>
+        <v>-32038.185375844419</v>
       </c>
       <c r="G82">
-        <v>30175207886.714306</v>
+        <v>30157117680.142502</v>
       </c>
       <c r="H82">
-        <v>0.19012022534031878</v>
+        <v>0.18929040883095527</v>
       </c>
       <c r="I82">
-        <v>1.2175753834909979E-4</v>
+        <v>1.2169633208191239E-4</v>
       </c>
       <c r="J82">
-        <v>-6.4683939397724771E-4</v>
+        <v>-6.4703848831393666E-4</v>
       </c>
       <c r="K82">
-        <v>-3.6260832242296544E-6</v>
+        <v>-2.524745011087748E-6</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3262,28 +3262,28 @@
         <v>-3.5599E-6</v>
       </c>
       <c r="D83">
-        <v>-59121.501922517084</v>
+        <v>-36209.227320820086</v>
       </c>
       <c r="E83">
-        <v>-19493602.952467706</v>
+        <v>-19495201.508834537</v>
       </c>
       <c r="F83">
-        <v>-46597.924873810007</v>
+        <v>-33472.493871562867</v>
       </c>
       <c r="G83">
-        <v>30289561624.809975</v>
+        <v>30298857530.068214</v>
       </c>
       <c r="H83">
-        <v>0.19222566397417806</v>
+        <v>0.19109599998158056</v>
       </c>
       <c r="I83">
-        <v>1.2175260477050747E-4</v>
+        <v>1.2168384891597279E-4</v>
       </c>
       <c r="J83">
-        <v>-6.4317130948457349E-4</v>
+        <v>-6.4345313646341109E-4</v>
       </c>
       <c r="K83">
-        <v>-3.668105802703478E-6</v>
+        <v>-2.6321008977215915E-6</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3297,28 +3297,28 @@
         <v>-1.8969E-6</v>
       </c>
       <c r="D84">
-        <v>-68276.990344908088</v>
+        <v>-47932.382607830717</v>
       </c>
       <c r="E84">
-        <v>-19469688.182040755</v>
+        <v>-19480387.889330048</v>
       </c>
       <c r="F84">
-        <v>-28571.747695968133</v>
+        <v>-22310.862698978246</v>
       </c>
       <c r="G84">
-        <v>30418299004.987659</v>
+        <v>30441242170.613438</v>
       </c>
       <c r="H84">
-        <v>0.19400238172503234</v>
+        <v>0.19299607686315859</v>
       </c>
       <c r="I84">
-        <v>1.2193750812132461E-4</v>
+        <v>1.217994286265484E-4</v>
       </c>
       <c r="J84">
-        <v>-6.3961312641438702E-4</v>
+        <v>-6.3981020265882092E-4</v>
       </c>
       <c r="K84">
-        <v>-2.2430154562129954E-6</v>
+        <v>-1.7508217949361015E-6</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3332,28 +3332,28 @@
         <v>2.3398999999999999E-7</v>
       </c>
       <c r="D85">
-        <v>-68347.748708378524</v>
+        <v>-52736.669122655228</v>
       </c>
       <c r="E85">
-        <v>-19471144.295924392</v>
+        <v>-19474807.041166447</v>
       </c>
       <c r="F85">
-        <v>299.32770591577975</v>
+        <v>-3960.3227691564562</v>
       </c>
       <c r="G85">
-        <v>30595909223.369419</v>
+        <v>30606535747.839298</v>
       </c>
       <c r="H85">
-        <v>0.19560731204092552</v>
+        <v>0.19483557623593453</v>
       </c>
       <c r="I85">
-        <v>1.222624432902644E-4</v>
+        <v>1.2213467945954332E-4</v>
       </c>
       <c r="J85">
-        <v>-6.3594754236991589E-4</v>
+        <v>-6.36124032409431E-4</v>
       </c>
       <c r="K85">
-        <v>2.33938705750808E-8</v>
+        <v>-3.1282425430758846E-7</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3367,28 +3367,28 @@
         <v>2.0866999999999999E-6</v>
       </c>
       <c r="D86">
-        <v>-61094.622217683122</v>
+        <v>-49976.626785268745</v>
       </c>
       <c r="E86">
-        <v>-19473984.999170534</v>
+        <v>-19477875.764100328</v>
       </c>
       <c r="F86">
-        <v>26272.57654924475</v>
+        <v>15031.882564351768</v>
       </c>
       <c r="G86">
-        <v>30786900934.936863</v>
+        <v>30796520826.023079</v>
       </c>
       <c r="H86">
-        <v>0.19713258833496994</v>
+        <v>0.19658448581207774</v>
       </c>
       <c r="I86">
-        <v>1.2271697051785519E-4</v>
+        <v>1.2267443419669986E-4</v>
       </c>
       <c r="J86">
-        <v>-6.3213909626025225E-4</v>
+        <v>-6.323631987151904E-4</v>
       </c>
       <c r="K86">
-        <v>2.0431799091220719E-6</v>
+        <v>1.1646751907384294E-6</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3402,28 +3402,28 @@
         <v>3.1294000000000001E-6</v>
       </c>
       <c r="D87">
-        <v>-51903.371008773334</v>
+        <v>-41011.392080423248</v>
       </c>
       <c r="E87">
-        <v>-19493313.482409127</v>
+        <v>-19489445.391040523</v>
       </c>
       <c r="F87">
-        <v>42053.962915331853</v>
+        <v>28561.223183303708</v>
       </c>
       <c r="G87">
-        <v>31008579705.876579</v>
+        <v>31005811733.548046</v>
       </c>
       <c r="H87">
-        <v>0.19884682286677768</v>
+        <v>0.19831292308847545</v>
       </c>
       <c r="I87">
-        <v>1.2332939330277629E-4</v>
+        <v>1.233940077879158E-4</v>
       </c>
       <c r="J87">
-        <v>-6.2831954477829844E-4</v>
+        <v>-6.2861753842885634E-4</v>
       </c>
       <c r="K87">
-        <v>3.2518028667966048E-6</v>
+        <v>2.2068355686564341E-6</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3437,28 +3437,28 @@
         <v>3.0937000000000001E-6</v>
       </c>
       <c r="D88">
-        <v>-42472.391093106475</v>
+        <v>-28442.987384922526</v>
       </c>
       <c r="E88">
-        <v>-19507278.589631751</v>
+        <v>-19505235.740250863</v>
       </c>
       <c r="F88">
-        <v>42454.883135079988</v>
+        <v>32473.888015711651</v>
       </c>
       <c r="G88">
-        <v>31213500675.871017</v>
+        <v>31214697372.299747</v>
       </c>
       <c r="H88">
-        <v>0.20079647491577993</v>
+        <v>0.200108226691948</v>
       </c>
       <c r="I88">
-        <v>1.241125770982339E-4</v>
+        <v>1.2429064227687233E-4</v>
       </c>
       <c r="J88">
-        <v>-6.2467998266435305E-4</v>
+        <v>-6.2510435161979103E-4</v>
       </c>
       <c r="K88">
-        <v>3.2663978559955772E-6</v>
+        <v>2.4997327144602043E-6</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3472,28 +3472,28 @@
         <v>2.0702000000000001E-6</v>
       </c>
       <c r="D89">
-        <v>-30743.708767697681</v>
+        <v>-15523.144809947918</v>
       </c>
       <c r="E89">
-        <v>-19540531.768169846</v>
+        <v>-19520259.260644995</v>
       </c>
       <c r="F89">
-        <v>27236.496154561773</v>
+        <v>25165.267528453631</v>
       </c>
       <c r="G89">
-        <v>31426332719.695374</v>
+        <v>31398695270.294731</v>
       </c>
       <c r="H89">
-        <v>0.2029118602699353</v>
+        <v>0.20216595329081058</v>
       </c>
       <c r="I89">
-        <v>1.2517353272603992E-4</v>
+        <v>1.2536736707308236E-4</v>
       </c>
       <c r="J89">
-        <v>-6.2161315476648741E-4</v>
+        <v>-6.2201494714629005E-4</v>
       </c>
       <c r="K89">
-        <v>2.0850921271147252E-6</v>
+        <v>1.931207317482384E-6</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3507,28 +3507,28 @@
         <v>6.4796000000000004E-7</v>
       </c>
       <c r="D90">
-        <v>-10487.969428312033</v>
+        <v>-7210.1422150251456</v>
       </c>
       <c r="E90">
-        <v>-19512794.488532148</v>
+        <v>-19526293.87937431</v>
       </c>
       <c r="F90">
-        <v>7519.3412102170487</v>
+        <v>11548.377138742995</v>
       </c>
       <c r="G90">
-        <v>31517074782.572021</v>
+        <v>31539975571.239548</v>
       </c>
       <c r="H90">
-        <v>0.20484424746035096</v>
+        <v>0.20468286948417547</v>
       </c>
       <c r="I90">
-        <v>1.2647848014292842E-4</v>
+        <v>1.2648825672074613E-4</v>
       </c>
       <c r="J90">
-        <v>-6.1904502144937562E-4</v>
+        <v>-6.1905159873867563E-4</v>
       </c>
       <c r="K90">
-        <v>5.7489052212537223E-7</v>
+        <v>8.8219053094367936E-7</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3542,28 +3542,28 @@
         <v>-7.7293999999999998E-7</v>
       </c>
       <c r="D91">
-        <v>-19618.503207665402</v>
+        <v>-21069.068776024971</v>
       </c>
       <c r="E91">
-        <v>-19484106.788605209</v>
+        <v>-19485406.779113032</v>
       </c>
       <c r="F91">
-        <v>-4395.8127762935401</v>
+        <v>-6315.9281771626611</v>
       </c>
       <c r="G91">
-        <v>29993297289.169518</v>
+        <v>29994870927.994438</v>
       </c>
       <c r="H91">
-        <v>0.19142750701619446</v>
+        <v>0.19149910479924559</v>
       </c>
       <c r="I91">
-        <v>1.2369689641746951E-4</v>
+        <v>1.2370032482371862E-4</v>
       </c>
       <c r="J91">
-        <v>-6.4949138652944461E-4</v>
+        <v>-6.4948957499504382E-4</v>
       </c>
       <c r="K91">
-        <v>-3.4922992917397339E-7</v>
+        <v>-5.0178043016274251E-7</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3577,28 +3577,28 @@
         <v>-1.6673999999999999E-6</v>
       </c>
       <c r="D92">
-        <v>-34282.066870448645</v>
+        <v>-37580.641101438552</v>
       </c>
       <c r="E92">
-        <v>-19521672.017066762</v>
+        <v>-19518956.537335049</v>
       </c>
       <c r="F92">
-        <v>-15957.462117574716</v>
+        <v>-15310.075150777146</v>
       </c>
       <c r="G92">
-        <v>30194595521.891518</v>
+        <v>30189401359.863308</v>
       </c>
       <c r="H92">
-        <v>0.19226642517550252</v>
+        <v>0.19242945295995723</v>
       </c>
       <c r="I92">
-        <v>1.2314804518610346E-4</v>
+        <v>1.2316824464868423E-4</v>
       </c>
       <c r="J92">
-        <v>-6.4632221975776836E-4</v>
+        <v>-6.463139311996078E-4</v>
       </c>
       <c r="K92">
-        <v>-1.2601782624376869E-6</v>
+        <v>-1.209445369995503E-6</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3612,28 +3612,28 @@
         <v>-1.6525000000000001E-6</v>
       </c>
       <c r="D93">
-        <v>-68279.116249450017</v>
+        <v>-67890.925589887425</v>
       </c>
       <c r="E93">
-        <v>-19488184.907574106</v>
+        <v>-19486735.172507439</v>
       </c>
       <c r="F93">
-        <v>-24268.278496856801</v>
+        <v>-20037.326985972075</v>
       </c>
       <c r="G93">
-        <v>30291870440.472782</v>
+        <v>30289716658.491463</v>
       </c>
       <c r="H93">
-        <v>0.19402240375385055</v>
+        <v>0.1940039616705844</v>
       </c>
       <c r="I93">
-        <v>1.2250346053612826E-4</v>
+        <v>1.2256256502537056E-4</v>
       </c>
       <c r="J93">
-        <v>-6.4287919659757314E-4</v>
+        <v>-6.4290334198621431E-4</v>
       </c>
       <c r="K93">
-        <v>-1.9129361058262823E-6</v>
+        <v>-1.5796914049443986E-6</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3647,28 +3647,28 @@
         <v>-8.8332E-7</v>
       </c>
       <c r="D94">
-        <v>-100102.60081182048</v>
+        <v>-95003.830527144019</v>
       </c>
       <c r="E94">
-        <v>-19498518.871966507</v>
+        <v>-19503083.617529329</v>
       </c>
       <c r="F94">
-        <v>-14960.527640280061</v>
+        <v>-13872.508936390454</v>
       </c>
       <c r="G94">
-        <v>30469122533.261196</v>
+        <v>30477860024.907196</v>
       </c>
       <c r="H94">
-        <v>0.19594725042957675</v>
+        <v>0.19569476011063805</v>
       </c>
       <c r="I94">
-        <v>1.2202456506321988E-4</v>
+        <v>1.2210168023586644E-4</v>
       </c>
       <c r="J94">
-        <v>-6.3928761482148159E-4</v>
+        <v>-6.3930344952376709E-4</v>
       </c>
       <c r="K94">
-        <v>-1.1742847200349286E-6</v>
+        <v>-1.0884744480366311E-6</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3682,28 +3682,28 @@
         <v>1.4308000000000001E-7</v>
       </c>
       <c r="D95">
-        <v>-113194.57228704775</v>
+        <v>-108413.37063468061</v>
       </c>
       <c r="E95">
-        <v>-19486219.037065025</v>
+        <v>-19485175.579357456</v>
       </c>
       <c r="F95">
-        <v>-711.53904409959659</v>
+        <v>-2893.3319678761518</v>
       </c>
       <c r="G95">
-        <v>30631922021.745312</v>
+        <v>30631809115.155613</v>
       </c>
       <c r="H95">
-        <v>0.19779472750046181</v>
+        <v>0.19755921068082896</v>
       </c>
       <c r="I95">
-        <v>1.2203988945467934E-4</v>
+        <v>1.2211817643483018E-4</v>
       </c>
       <c r="J95">
-        <v>-6.3537892444688431E-4</v>
+        <v>-6.354015850620052E-4</v>
       </c>
       <c r="K95">
-        <v>-5.5637472590446685E-8</v>
+        <v>-2.2622521953126473E-7</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3717,28 +3717,28 @@
         <v>1.0394E-6</v>
       </c>
       <c r="D96">
-        <v>-103146.84279758669</v>
+        <v>-103119.88347817352</v>
       </c>
       <c r="E96">
-        <v>-19497011.456440561</v>
+        <v>-19499069.555339947</v>
       </c>
       <c r="F96">
-        <v>13406.371235180402</v>
+        <v>9710.2220902875852</v>
       </c>
       <c r="G96">
-        <v>30853277003.881588</v>
+        <v>30856537719.475006</v>
       </c>
       <c r="H96">
-        <v>0.19944263478351754</v>
+        <v>0.19944098913169289</v>
       </c>
       <c r="I96">
-        <v>1.2262083812218996E-4</v>
+        <v>1.2268105637633164E-4</v>
       </c>
       <c r="J96">
-        <v>-6.3125021658555231E-4</v>
+        <v>-6.3126292251358988E-4</v>
       </c>
       <c r="K96">
-        <v>1.042254901146341E-6</v>
+        <v>7.5489611001382934E-7</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3752,28 +3752,28 @@
         <v>1.5324999999999999E-6</v>
       </c>
       <c r="D97">
-        <v>-73681.908172719181</v>
+        <v>-80673.555452622473</v>
       </c>
       <c r="E97">
-        <v>-19494685.204471983</v>
+        <v>-19493199.065599386</v>
       </c>
       <c r="F97">
-        <v>21922.277914114697</v>
+        <v>18207.546016016393</v>
       </c>
       <c r="G97">
-        <v>31068403397.023418</v>
+        <v>31063734045.13335</v>
       </c>
       <c r="H97">
-        <v>0.20088637402528756</v>
+        <v>0.20123120640006462</v>
       </c>
       <c r="I97">
-        <v>1.2363576013390816E-4</v>
+        <v>1.2367110943985258E-4</v>
       </c>
       <c r="J97">
-        <v>-6.2698818170075967E-4</v>
+        <v>-6.2699412838972644E-4</v>
       </c>
       <c r="K97">
-        <v>1.6945969691507627E-6</v>
+        <v>1.4081394873904397E-6</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3787,28 +3787,28 @@
         <v>1.4609000000000001E-6</v>
       </c>
       <c r="D98">
-        <v>-36202.641727597453</v>
+        <v>-48940.548625155352</v>
       </c>
       <c r="E98">
-        <v>-19506624.433555204</v>
+        <v>-19506084.593988061</v>
       </c>
       <c r="F98">
-        <v>22533.442058970053</v>
+        <v>20364.56924526257</v>
       </c>
       <c r="G98">
-        <v>31304077500.302967</v>
+        <v>31299015670.628296</v>
       </c>
       <c r="H98">
-        <v>0.20229399077741747</v>
+        <v>0.2029204927992258</v>
       </c>
       <c r="I98">
-        <v>1.2488303494343606E-4</v>
+        <v>1.2489520234857876E-4</v>
       </c>
       <c r="J98">
-        <v>-6.228975715552457E-4</v>
+        <v>-6.2290144241397474E-4</v>
       </c>
       <c r="K98">
-        <v>1.7308377958645017E-6</v>
+        <v>1.5653434561760729E-6</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3822,28 +3822,28 @@
         <v>7.8472E-7</v>
       </c>
       <c r="D99">
-        <v>-7104.0011142236181</v>
+        <v>-19294.002870555501</v>
       </c>
       <c r="E99">
-        <v>-19512373.837993585</v>
+        <v>-19507586.13391459</v>
       </c>
       <c r="F99">
-        <v>9309.067264653755</v>
+        <v>12767.639373146123</v>
       </c>
       <c r="G99">
-        <v>31503275759.845673</v>
+        <v>31491519907.555603</v>
       </c>
       <c r="H99">
-        <v>0.20395612879064043</v>
+        <v>0.20455483645116015</v>
       </c>
       <c r="I99">
-        <v>1.2610273987307172E-4</v>
+        <v>1.2609741690950159E-4</v>
       </c>
       <c r="J99">
-        <v>-6.1933887026701133E-4</v>
+        <v>-6.1932847334504387E-4</v>
       </c>
       <c r="K99">
-        <v>7.1153756381727232E-7</v>
+        <v>9.7672272995289605E-7</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3857,28 +3857,28 @@
         <v>-5.1198E-8</v>
       </c>
       <c r="D100">
-        <v>-376.20281229075044</v>
+        <v>-4169.2566549228504</v>
       </c>
       <c r="E100">
-        <v>-19510603.445260979</v>
+        <v>-19514702.965315565</v>
       </c>
       <c r="F100">
-        <v>-6877.5383978366071</v>
+        <v>-2620.8055065152862</v>
       </c>
       <c r="G100">
-        <v>31641089708.048248</v>
+        <v>31646463816.056595</v>
       </c>
       <c r="H100">
-        <v>0.20628800730980618</v>
+        <v>0.20647419536573269</v>
       </c>
       <c r="I100">
-        <v>1.2719268059476385E-4</v>
+        <v>1.2719028143833255E-4</v>
       </c>
       <c r="J100">
-        <v>-6.1661827615052756E-4</v>
+        <v>-6.1662088163828453E-4</v>
       </c>
       <c r="K100">
-        <v>-5.2440070043031223E-7</v>
+        <v>-1.9982891509865916E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- updated figure numbers
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\theia\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16B9895-0E74-4C2F-916C-5695FEB8AC9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6D014F-D76B-41BD-9630-FB0AC21B0FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1830" windowWidth="16578" windowHeight="9444" xr2:uid="{BEE921D4-70B4-4CBA-B92B-ED4A2FE488D6}"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="16578" windowHeight="9444" xr2:uid="{DE6E1BFC-DC39-49DA-B0F3-FA276F7A90C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -372,7 +372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F74DC7-A33A-402C-A12F-66C545FCB857}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96221B8-F293-4A2B-AFF3-0F2A1090D2CF}">
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3887,7 +3887,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F2C804-5DF3-4BF3-A84B-A179DAC3644F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29192216-70FA-4B49-9B3F-905D6E36BE14}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3899,7 +3899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C755E4A-7383-48D8-AD18-6E6733A31ABA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22729120-105F-4941-BD2A-8422719389D7}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
- added proper scaling and sizing to subplots
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\theia\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6D014F-D76B-41BD-9630-FB0AC21B0FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C37FC9-1AE5-4ECA-B7AD-0ADC5F53DE77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1830" windowWidth="16578" windowHeight="9444" xr2:uid="{DE6E1BFC-DC39-49DA-B0F3-FA276F7A90C6}"/>
+    <workbookView xWindow="2562" yWindow="2562" windowWidth="16578" windowHeight="9444" xr2:uid="{CDA2BFD1-6A2D-4015-B92F-23896491A066}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -372,7 +372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96221B8-F293-4A2B-AFF3-0F2A1090D2CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229B3BA6-2BB0-4A72-B166-85711DF8637D}">
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3887,7 +3887,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29192216-70FA-4B49-9B3F-905D6E36BE14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7FD3616-46EB-4AE0-8426-FBB938E14EEF}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3899,7 +3899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22729120-105F-4941-BD2A-8422719389D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C5C16C-B754-4C94-B404-C2379BC0B151}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>